<commit_message>
Repo Update: 2024-05-31 11:34:04
</commit_message>
<xml_diff>
--- a/Database/Run_shortcut_creator_aliases.xlsx
+++ b/Database/Run_shortcut_creator_aliases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\player-1\Documents\Windows-Git-Repos\win-t\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EA428E5-5C3E-46DD-A500-7BCC6FF233D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D93ECB03-A736-426C-934E-552F6AECA324}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D65865D6-BB34-410C-8183-31ED199784FF}"/>
   </bookViews>
@@ -35,8 +35,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="321">
   <si>
     <t>Number</t>
   </si>
@@ -993,6 +1015,12 @@
   </si>
   <si>
     <t>dot</t>
+  </si>
+  <si>
+    <t>C:\Users\player-1\Documents\Windows-Git-Repos\win-t\Configs &amp; Backups</t>
+  </si>
+  <si>
+    <t>cb</t>
   </si>
 </sst>
 </file>
@@ -1424,16 +1452,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58A033C2-67FB-408D-B72B-8C45836FCF74}">
-  <dimension ref="B2:G160"/>
+  <dimension ref="B2:G161"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A54" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A138" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21"/>
   <cols>
     <col min="2" max="2" width="13.625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="79.125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="90.125" style="4" customWidth="1"/>
     <col min="4" max="4" width="19.375" style="4" customWidth="1"/>
     <col min="5" max="5" width="25.75" style="5" customWidth="1"/>
     <col min="6" max="6" width="28.25" style="5" customWidth="1"/>
@@ -1462,7 +1490,8 @@
       </c>
     </row>
     <row r="3" spans="2:7" ht="24.95" customHeight="1">
-      <c r="B3" s="6">
+      <c r="B3" s="6" cm="1">
+        <f t="array" ref="B3:B157">_xlfn.SEQUENCE(COUNTA(C:C)-1)</f>
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -1860,17 +1889,15 @@
         <v>24</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>117</v>
+        <v>319</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>56</v>
+        <v>320</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="F26" s="1"/>
       <c r="G26" s="1"/>
     </row>
     <row r="27" spans="2:7" ht="24.95" customHeight="1">
@@ -1878,15 +1905,17 @@
         <v>25</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>57</v>
+        <v>117</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F27" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="G27" s="1"/>
     </row>
     <row r="28" spans="2:7" ht="24.95" customHeight="1">
@@ -1894,13 +1923,13 @@
         <v>26</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
@@ -1910,13 +1939,13 @@
         <v>27</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
@@ -1926,17 +1955,15 @@
         <v>28</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F30" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="F30" s="1"/>
       <c r="G30" s="1"/>
     </row>
     <row r="31" spans="2:7" ht="24.95" customHeight="1">
@@ -1944,10 +1971,10 @@
         <v>29</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>5</v>
@@ -1962,10 +1989,10 @@
         <v>30</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>5</v>
@@ -1980,15 +2007,17 @@
         <v>31</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F33" s="1"/>
+        <v>5</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="G33" s="1"/>
     </row>
     <row r="34" spans="2:7" ht="24.95" customHeight="1">
@@ -1996,33 +2025,31 @@
         <v>32</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
     </row>
-    <row r="35" spans="2:7">
+    <row r="35" spans="2:7" ht="24.95" customHeight="1">
       <c r="B35" s="6">
         <v>33</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>34</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F35" s="1"/>
       <c r="G35" s="1"/>
     </row>
     <row r="36" spans="2:7">
@@ -2030,15 +2057,17 @@
         <v>34</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F36" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="G36" s="1"/>
     </row>
     <row r="37" spans="2:7">
@@ -2046,17 +2075,15 @@
         <v>35</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>34</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F37" s="1"/>
       <c r="G37" s="1"/>
     </row>
     <row r="38" spans="2:7">
@@ -2064,15 +2091,17 @@
         <v>36</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F38" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="G38" s="1"/>
     </row>
     <row r="39" spans="2:7">
@@ -2080,17 +2109,15 @@
         <v>37</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F39" s="1"/>
       <c r="G39" s="1"/>
     </row>
     <row r="40" spans="2:7">
@@ -2098,16 +2125,16 @@
         <v>38</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="G40" s="1"/>
     </row>
@@ -2116,15 +2143,17 @@
         <v>39</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>317</v>
+        <v>83</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>318</v>
+        <v>84</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F41" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="G41" s="1"/>
     </row>
     <row r="42" spans="2:7">
@@ -2132,17 +2161,15 @@
         <v>40</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>85</v>
+        <v>317</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>86</v>
+        <v>318</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>34</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="F42" s="1"/>
       <c r="G42" s="1"/>
     </row>
     <row r="43" spans="2:7">
@@ -2150,16 +2177,16 @@
         <v>41</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="G43" s="1"/>
     </row>
@@ -2168,16 +2195,16 @@
         <v>42</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="G44" s="1"/>
     </row>
@@ -2186,15 +2213,17 @@
         <v>43</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F45" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="G45" s="1"/>
     </row>
     <row r="46" spans="2:7">
@@ -2202,10 +2231,10 @@
         <v>44</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>5</v>
@@ -2218,17 +2247,15 @@
         <v>45</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F47" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F47" s="1"/>
       <c r="G47" s="1"/>
     </row>
     <row r="48" spans="2:7">
@@ -2236,10 +2263,10 @@
         <v>46</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>7</v>
@@ -2254,15 +2281,17 @@
         <v>47</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F49" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="G49" s="1"/>
     </row>
     <row r="50" spans="2:7">
@@ -2270,10 +2299,10 @@
         <v>48</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>5</v>
@@ -2286,10 +2315,10 @@
         <v>49</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>5</v>
@@ -2302,10 +2331,10 @@
         <v>50</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>5</v>
@@ -2318,10 +2347,10 @@
         <v>51</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>5</v>
@@ -2334,10 +2363,10 @@
         <v>52</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>5</v>
@@ -2350,13 +2379,13 @@
         <v>53</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
@@ -2366,13 +2395,13 @@
         <v>54</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F56" s="1"/>
       <c r="G56" s="1"/>
@@ -2382,10 +2411,10 @@
         <v>55</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>5</v>
@@ -2398,17 +2427,15 @@
         <v>56</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F58" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F58" s="1"/>
       <c r="G58" s="1"/>
     </row>
     <row r="59" spans="2:7">
@@ -2416,10 +2443,10 @@
         <v>57</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>7</v>
@@ -2434,15 +2461,17 @@
         <v>58</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F60" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="G60" s="1"/>
     </row>
     <row r="61" spans="2:7">
@@ -2450,17 +2479,15 @@
         <v>59</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F61" s="1" t="s">
-        <v>34</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F61" s="1"/>
       <c r="G61" s="1"/>
     </row>
     <row r="62" spans="2:7">
@@ -2468,15 +2495,17 @@
         <v>60</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F62" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="G62" s="1"/>
     </row>
     <row r="63" spans="2:7">
@@ -2484,10 +2513,10 @@
         <v>61</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>5</v>
@@ -2500,10 +2529,10 @@
         <v>62</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E64" s="1" t="s">
         <v>5</v>
@@ -2516,10 +2545,10 @@
         <v>63</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E65" s="1" t="s">
         <v>5</v>
@@ -2532,10 +2561,10 @@
         <v>64</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E66" s="1" t="s">
         <v>5</v>
@@ -2548,10 +2577,10 @@
         <v>65</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E67" s="1" t="s">
         <v>5</v>
@@ -2564,10 +2593,10 @@
         <v>66</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>5</v>
@@ -2580,10 +2609,10 @@
         <v>67</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E69" s="1" t="s">
         <v>5</v>
@@ -2596,17 +2625,15 @@
         <v>68</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F70" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F70" s="1"/>
       <c r="G70" s="1"/>
     </row>
     <row r="71" spans="2:7">
@@ -2614,15 +2641,17 @@
         <v>69</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F71" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="G71" s="1"/>
     </row>
     <row r="72" spans="2:7">
@@ -2630,17 +2659,15 @@
         <v>70</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F72" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F72" s="1"/>
       <c r="G72" s="1"/>
     </row>
     <row r="73" spans="2:7">
@@ -2648,15 +2675,17 @@
         <v>71</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F73" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="G73" s="1"/>
     </row>
     <row r="74" spans="2:7">
@@ -2664,17 +2693,15 @@
         <v>72</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F74" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F74" s="1"/>
       <c r="G74" s="1"/>
     </row>
     <row r="75" spans="2:7">
@@ -2682,15 +2709,17 @@
         <v>73</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F75" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="G75" s="1"/>
     </row>
     <row r="76" spans="2:7">
@@ -2698,10 +2727,10 @@
         <v>74</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E76" s="1" t="s">
         <v>5</v>
@@ -2714,10 +2743,10 @@
         <v>75</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E77" s="1" t="s">
         <v>5</v>
@@ -2730,10 +2759,10 @@
         <v>76</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E78" s="1" t="s">
         <v>5</v>
@@ -2746,10 +2775,10 @@
         <v>77</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E79" s="1" t="s">
         <v>5</v>
@@ -2762,17 +2791,15 @@
         <v>78</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F80" s="1" t="s">
-        <v>34</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F80" s="1"/>
       <c r="G80" s="1"/>
     </row>
     <row r="81" spans="2:7">
@@ -2780,10 +2807,10 @@
         <v>79</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E81" s="1" t="s">
         <v>7</v>
@@ -2798,16 +2825,16 @@
         <v>80</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E82" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="G82" s="1"/>
     </row>
@@ -2816,15 +2843,17 @@
         <v>81</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F83" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="G83" s="1"/>
     </row>
     <row r="84" spans="2:7">
@@ -2832,13 +2861,13 @@
         <v>82</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F84" s="1"/>
       <c r="G84" s="1"/>
@@ -2848,13 +2877,13 @@
         <v>83</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F85" s="1"/>
       <c r="G85" s="1"/>
@@ -2864,10 +2893,10 @@
         <v>84</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E86" s="1" t="s">
         <v>5</v>
@@ -2880,10 +2909,10 @@
         <v>85</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E87" s="1" t="s">
         <v>5</v>
@@ -2896,10 +2925,10 @@
         <v>86</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E88" s="1" t="s">
         <v>5</v>
@@ -2912,10 +2941,10 @@
         <v>87</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E89" s="1" t="s">
         <v>5</v>
@@ -2928,10 +2957,10 @@
         <v>88</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E90" s="1" t="s">
         <v>5</v>
@@ -2944,10 +2973,10 @@
         <v>89</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E91" s="1" t="s">
         <v>5</v>
@@ -2960,10 +2989,10 @@
         <v>90</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E92" s="1" t="s">
         <v>5</v>
@@ -2976,10 +3005,10 @@
         <v>91</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E93" s="1" t="s">
         <v>5</v>
@@ -2992,17 +3021,15 @@
         <v>92</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F94" s="1" t="s">
-        <v>34</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F94" s="1"/>
       <c r="G94" s="1"/>
     </row>
     <row r="95" spans="2:7">
@@ -3010,15 +3037,17 @@
         <v>93</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F95" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F95" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="G95" s="1"/>
     </row>
     <row r="96" spans="2:7">
@@ -3026,10 +3055,10 @@
         <v>94</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E96" s="1" t="s">
         <v>5</v>
@@ -3042,10 +3071,10 @@
         <v>95</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E97" s="1" t="s">
         <v>5</v>
@@ -3058,10 +3087,10 @@
         <v>96</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E98" s="1" t="s">
         <v>5</v>
@@ -3074,10 +3103,10 @@
         <v>97</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E99" s="1" t="s">
         <v>5</v>
@@ -3090,10 +3119,10 @@
         <v>98</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E100" s="1" t="s">
         <v>5</v>
@@ -3106,10 +3135,10 @@
         <v>99</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E101" s="1" t="s">
         <v>5</v>
@@ -3122,10 +3151,10 @@
         <v>100</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E102" s="1" t="s">
         <v>5</v>
@@ -3138,17 +3167,15 @@
         <v>101</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F103" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F103" s="1"/>
       <c r="G103" s="1"/>
     </row>
     <row r="104" spans="2:7">
@@ -3156,15 +3183,17 @@
         <v>102</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F104" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F104" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="G104" s="1"/>
     </row>
     <row r="105" spans="2:7">
@@ -3172,10 +3201,10 @@
         <v>103</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E105" s="1" t="s">
         <v>5</v>
@@ -3188,10 +3217,10 @@
         <v>104</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="E106" s="1" t="s">
         <v>5</v>
@@ -3204,10 +3233,10 @@
         <v>105</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E107" s="1" t="s">
         <v>5</v>
@@ -3220,13 +3249,13 @@
         <v>106</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F108" s="1"/>
       <c r="G108" s="1"/>
@@ -3236,13 +3265,13 @@
         <v>107</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F109" s="1"/>
       <c r="G109" s="1"/>
@@ -3252,10 +3281,10 @@
         <v>108</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E110" s="1" t="s">
         <v>5</v>
@@ -3268,10 +3297,10 @@
         <v>109</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E111" s="1" t="s">
         <v>5</v>
@@ -3284,17 +3313,15 @@
         <v>110</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F112" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F112" s="1"/>
       <c r="G112" s="1"/>
     </row>
     <row r="113" spans="2:7">
@@ -3302,15 +3329,17 @@
         <v>111</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F113" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F113" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="G113" s="1"/>
     </row>
     <row r="114" spans="2:7">
@@ -3318,10 +3347,10 @@
         <v>112</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E114" s="1" t="s">
         <v>5</v>
@@ -3334,17 +3363,15 @@
         <v>113</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F115" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F115" s="1"/>
       <c r="G115" s="1"/>
     </row>
     <row r="116" spans="2:7">
@@ -3352,30 +3379,28 @@
         <v>114</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="E116" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F116" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G116" s="1" t="s">
-        <v>37</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="G116" s="1"/>
     </row>
     <row r="117" spans="2:7">
       <c r="B117" s="6">
         <v>115</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E117" s="1" t="s">
         <v>7</v>
@@ -3392,10 +3417,10 @@
         <v>116</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="E118" s="1" t="s">
         <v>7</v>
@@ -3404,7 +3429,7 @@
         <v>34</v>
       </c>
       <c r="G118" s="1" t="s">
-        <v>315</v>
+        <v>37</v>
       </c>
     </row>
     <row r="119" spans="2:7">
@@ -3412,10 +3437,10 @@
         <v>117</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E119" s="1" t="s">
         <v>7</v>
@@ -3423,22 +3448,26 @@
       <c r="F119" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G119" s="1"/>
+      <c r="G119" s="1" t="s">
+        <v>315</v>
+      </c>
     </row>
     <row r="120" spans="2:7">
       <c r="B120" s="6">
         <v>118</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F120" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F120" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="G120" s="1"/>
     </row>
     <row r="121" spans="2:7">
@@ -3446,10 +3475,10 @@
         <v>119</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="E121" s="1" t="s">
         <v>5</v>
@@ -3462,17 +3491,15 @@
         <v>120</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F122" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F122" s="1"/>
       <c r="G122" s="1"/>
     </row>
     <row r="123" spans="2:7">
@@ -3480,16 +3507,16 @@
         <v>121</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E123" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F123" s="1" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="G123" s="1"/>
     </row>
@@ -3498,15 +3525,17 @@
         <v>122</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F124" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F124" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="G124" s="1"/>
     </row>
     <row r="125" spans="2:7">
@@ -3514,10 +3543,10 @@
         <v>123</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="E125" s="1" t="s">
         <v>5</v>
@@ -3530,10 +3559,10 @@
         <v>124</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E126" s="1" t="s">
         <v>5</v>
@@ -3546,10 +3575,10 @@
         <v>125</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E127" s="1" t="s">
         <v>5</v>
@@ -3562,10 +3591,10 @@
         <v>126</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E128" s="1" t="s">
         <v>5</v>
@@ -3578,17 +3607,15 @@
         <v>127</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="E129" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F129" s="1" t="s">
-        <v>34</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F129" s="1"/>
       <c r="G129" s="1"/>
     </row>
     <row r="130" spans="2:7">
@@ -3596,15 +3623,17 @@
         <v>128</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="E130" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F130" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F130" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="G130" s="1"/>
     </row>
     <row r="131" spans="2:7">
@@ -3612,13 +3641,13 @@
         <v>129</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="E131" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F131" s="1"/>
       <c r="G131" s="1"/>
@@ -3628,10 +3657,10 @@
         <v>130</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="E132" s="1" t="s">
         <v>5</v>
@@ -3644,10 +3673,10 @@
         <v>131</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E133" s="1" t="s">
         <v>5</v>
@@ -3660,10 +3689,10 @@
         <v>132</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="E134" s="1" t="s">
         <v>5</v>
@@ -3676,10 +3705,10 @@
         <v>133</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E135" s="1" t="s">
         <v>5</v>
@@ -3692,10 +3721,10 @@
         <v>134</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="E136" s="1" t="s">
         <v>5</v>
@@ -3708,17 +3737,15 @@
         <v>135</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E137" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F137" s="1" t="s">
-        <v>34</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F137" s="1"/>
       <c r="G137" s="1"/>
     </row>
     <row r="138" spans="2:7">
@@ -3726,15 +3753,17 @@
         <v>136</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="E138" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F138" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F138" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="G138" s="1"/>
     </row>
     <row r="139" spans="2:7">
@@ -3742,10 +3771,10 @@
         <v>137</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E139" s="1" t="s">
         <v>5</v>
@@ -3758,17 +3787,15 @@
         <v>138</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E140" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F140" s="1" t="s">
-        <v>34</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F140" s="1"/>
       <c r="G140" s="1"/>
     </row>
     <row r="141" spans="2:7">
@@ -3776,15 +3803,17 @@
         <v>139</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E141" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F141" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F141" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="G141" s="1"/>
     </row>
     <row r="142" spans="2:7">
@@ -3792,10 +3821,10 @@
         <v>140</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="E142" s="1" t="s">
         <v>5</v>
@@ -3808,10 +3837,10 @@
         <v>141</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E143" s="1" t="s">
         <v>5</v>
@@ -3824,10 +3853,10 @@
         <v>142</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E144" s="1" t="s">
         <v>5</v>
@@ -3840,10 +3869,10 @@
         <v>143</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="E145" s="1" t="s">
         <v>5</v>
@@ -3856,10 +3885,10 @@
         <v>144</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>10</v>
+        <v>292</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E146" s="1" t="s">
         <v>5</v>
@@ -3872,17 +3901,15 @@
         <v>145</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>295</v>
+        <v>10</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="E147" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F147" s="1" t="s">
-        <v>34</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F147" s="1"/>
       <c r="G147" s="1"/>
     </row>
     <row r="148" spans="2:7">
@@ -3890,15 +3917,17 @@
         <v>146</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="E148" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F148" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F148" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="G148" s="1"/>
     </row>
     <row r="149" spans="2:7">
@@ -3906,13 +3935,13 @@
         <v>147</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="E149" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F149" s="1"/>
       <c r="G149" s="1"/>
@@ -3922,17 +3951,15 @@
         <v>148</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="E150" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F150" s="1" t="s">
-        <v>34</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="F150" s="1"/>
       <c r="G150" s="1"/>
     </row>
     <row r="151" spans="2:7">
@@ -3940,10 +3967,10 @@
         <v>149</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E151" s="1" t="s">
         <v>7</v>
@@ -3958,10 +3985,10 @@
         <v>150</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E152" s="1" t="s">
         <v>7</v>
@@ -3976,15 +4003,17 @@
         <v>151</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="E153" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F153" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F153" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="G153" s="1"/>
     </row>
     <row r="154" spans="2:7">
@@ -3992,17 +4021,15 @@
         <v>152</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E154" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F154" s="1" t="s">
-        <v>34</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F154" s="1"/>
       <c r="G154" s="1"/>
     </row>
     <row r="155" spans="2:7">
@@ -4010,15 +4037,17 @@
         <v>153</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="D155" s="1" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E155" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F155" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F155" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="G155" s="1"/>
     </row>
     <row r="156" spans="2:7">
@@ -4026,10 +4055,10 @@
         <v>154</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E156" s="1" t="s">
         <v>5</v>
@@ -4038,10 +4067,18 @@
       <c r="G156" s="1"/>
     </row>
     <row r="157" spans="2:7">
-      <c r="B157" s="6"/>
-      <c r="C157" s="1"/>
-      <c r="D157" s="1"/>
-      <c r="E157" s="1"/>
+      <c r="B157" s="6">
+        <v>155</v>
+      </c>
+      <c r="C157" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="D157" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="E157" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F157" s="1"/>
       <c r="G157" s="1"/>
     </row>
@@ -4069,12 +4106,20 @@
       <c r="F160" s="1"/>
       <c r="G160" s="1"/>
     </row>
+    <row r="161" spans="2:7">
+      <c r="B161" s="6"/>
+      <c r="C161" s="1"/>
+      <c r="D161" s="1"/>
+      <c r="E161" s="1"/>
+      <c r="F161" s="1"/>
+      <c r="G161" s="1"/>
+    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E156" xr:uid="{7E8CE32C-29D1-4006-9E0F-69B72A0F4378}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E157" xr:uid="{7E8CE32C-29D1-4006-9E0F-69B72A0F4378}">
       <formula1>"[Application],[Directory],[Script]"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F160" xr:uid="{A5D947FB-5606-4B36-88C5-81CC2B61C636}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F161" xr:uid="{A5D947FB-5606-4B36-88C5-81CC2B61C636}">
       <formula1>"[bat],[vbs]"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Repo Update: 2024-05-31 13:50:41
</commit_message>
<xml_diff>
--- a/Database/Run_shortcut_creator_aliases.xlsx
+++ b/Database/Run_shortcut_creator_aliases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\player-1\Documents\Windows-Git-Repos\win-t\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D93ECB03-A736-426C-934E-552F6AECA324}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C0DD10C-EDB2-4BC0-A35D-19EC7E77E3B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D65865D6-BB34-410C-8183-31ED199784FF}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="325">
   <si>
     <t>Number</t>
   </si>
@@ -1021,6 +1021,18 @@
   </si>
   <si>
     <t>cb</t>
+  </si>
+  <si>
+    <t>Context Menu Manager</t>
+  </si>
+  <si>
+    <t>cmm</t>
+  </si>
+  <si>
+    <t>aai</t>
+  </si>
+  <si>
+    <t>C:\MY-TOOLS\Windows Store\Alternative Windows Apps Installer\alt app installer</t>
   </si>
 </sst>
 </file>
@@ -1452,16 +1464,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58A033C2-67FB-408D-B72B-8C45836FCF74}">
-  <dimension ref="B2:G161"/>
+  <dimension ref="B2:G163"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A138" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A127" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
+      <selection activeCell="P151" sqref="P151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21"/>
   <cols>
     <col min="2" max="2" width="13.625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="90.125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="93.5" style="4" customWidth="1"/>
     <col min="4" max="4" width="19.375" style="4" customWidth="1"/>
     <col min="5" max="5" width="25.75" style="5" customWidth="1"/>
     <col min="6" max="6" width="28.25" style="5" customWidth="1"/>
@@ -1491,7 +1503,7 @@
     </row>
     <row r="3" spans="2:7" ht="24.95" customHeight="1">
       <c r="B3" s="6" cm="1">
-        <f t="array" ref="B3:B157">_xlfn.SEQUENCE(COUNTA(C:C)-1)</f>
+        <f t="array" ref="B3:B159">_xlfn.SEQUENCE(COUNTA(C:C)-1)</f>
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -1527,13 +1539,13 @@
         <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>12</v>
+        <v>324</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>13</v>
+        <v>323</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
@@ -1543,17 +1555,15 @@
         <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F6" s="1"/>
       <c r="G6" s="1"/>
     </row>
     <row r="7" spans="2:7" ht="24.95" customHeight="1">
@@ -1561,27 +1571,25 @@
         <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G7" s="1" t="s">
-        <v>17</v>
-      </c>
+      <c r="G7" s="1"/>
     </row>
     <row r="8" spans="2:7" ht="24.95" customHeight="1">
       <c r="B8" s="6">
         <v>6</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>19</v>
@@ -1589,18 +1597,22 @@
       <c r="E8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
+      <c r="F8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="9" spans="2:7" ht="24.95" customHeight="1">
       <c r="B9" s="6">
         <v>7</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>5</v>
@@ -1613,10 +1625,10 @@
         <v>8</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>316</v>
+        <v>21</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>5</v>
@@ -1629,10 +1641,10 @@
         <v>9</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>24</v>
+        <v>316</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>5</v>
@@ -1645,17 +1657,15 @@
         <v>10</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F12" s="1"/>
       <c r="G12" s="1"/>
     </row>
     <row r="13" spans="2:7" ht="24.95" customHeight="1">
@@ -1663,10 +1673,10 @@
         <v>11</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>7</v>
@@ -1681,15 +1691,17 @@
         <v>12</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F14" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="G14" s="1"/>
     </row>
     <row r="15" spans="2:7" ht="24.95" customHeight="1">
@@ -1697,30 +1709,26 @@
         <v>13</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>17</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
     </row>
     <row r="16" spans="2:7" ht="24.95" customHeight="1">
       <c r="B16" s="6">
         <v>14</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>7</v>
@@ -1729,7 +1737,7 @@
         <v>34</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="2:7" ht="24.95" customHeight="1">
@@ -1737,26 +1745,30 @@
         <v>15</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="18" spans="2:7" ht="24.95" customHeight="1">
       <c r="B18" s="6">
         <v>16</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>5</v>
@@ -1769,17 +1781,15 @@
         <v>17</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>34</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F19" s="1"/>
       <c r="G19" s="1"/>
     </row>
     <row r="20" spans="2:7" ht="24.95" customHeight="1">
@@ -1787,10 +1797,10 @@
         <v>18</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>7</v>
@@ -1805,15 +1815,17 @@
         <v>19</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F21" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="G21" s="1"/>
     </row>
     <row r="22" spans="2:7" ht="24.95" customHeight="1">
@@ -1821,13 +1833,13 @@
         <v>20</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
@@ -1837,17 +1849,15 @@
         <v>21</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="F23" s="1"/>
       <c r="G23" s="1"/>
     </row>
     <row r="24" spans="2:7" ht="24.95" customHeight="1">
@@ -1855,16 +1865,16 @@
         <v>22</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="G24" s="1"/>
     </row>
@@ -1873,15 +1883,17 @@
         <v>23</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F25" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="G25" s="1"/>
     </row>
     <row r="26" spans="2:7" ht="24.95" customHeight="1">
@@ -1889,13 +1901,13 @@
         <v>24</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>319</v>
+        <v>54</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>320</v>
+        <v>55</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
@@ -1905,17 +1917,15 @@
         <v>25</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>117</v>
+        <v>319</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>56</v>
+        <v>320</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="F27" s="1"/>
       <c r="G27" s="1"/>
     </row>
     <row r="28" spans="2:7" ht="24.95" customHeight="1">
@@ -1923,15 +1933,17 @@
         <v>26</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>57</v>
+        <v>117</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F28" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="G28" s="1"/>
     </row>
     <row r="29" spans="2:7" ht="24.95" customHeight="1">
@@ -1939,13 +1951,13 @@
         <v>27</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
@@ -1955,13 +1967,13 @@
         <v>28</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
@@ -1971,17 +1983,15 @@
         <v>29</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>64</v>
+        <v>321</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>63</v>
+        <v>322</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F31" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="F31" s="1"/>
       <c r="G31" s="1"/>
     </row>
     <row r="32" spans="2:7" ht="24.95" customHeight="1">
@@ -1989,17 +1999,15 @@
         <v>30</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F32" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="F32" s="1"/>
       <c r="G32" s="1"/>
     </row>
     <row r="33" spans="2:7" ht="24.95" customHeight="1">
@@ -2007,10 +2015,10 @@
         <v>31</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>5</v>
@@ -2025,15 +2033,17 @@
         <v>32</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F34" s="1"/>
+        <v>5</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="G34" s="1"/>
     </row>
     <row r="35" spans="2:7" ht="24.95" customHeight="1">
@@ -2041,44 +2051,44 @@
         <v>33</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F35" s="1"/>
+      <c r="F35" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="G35" s="1"/>
     </row>
-    <row r="36" spans="2:7">
+    <row r="36" spans="2:7" ht="24.95" customHeight="1">
       <c r="B36" s="6">
         <v>34</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>34</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="F36" s="1"/>
       <c r="G36" s="1"/>
     </row>
-    <row r="37" spans="2:7">
+    <row r="37" spans="2:7" ht="24.95" customHeight="1">
       <c r="B37" s="6">
         <v>35</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>5</v>
@@ -2091,10 +2101,10 @@
         <v>36</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>7</v>
@@ -2109,10 +2119,10 @@
         <v>37</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>5</v>
@@ -2125,16 +2135,16 @@
         <v>38</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="G40" s="1"/>
     </row>
@@ -2143,17 +2153,15 @@
         <v>39</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>34</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F41" s="1"/>
       <c r="G41" s="1"/>
     </row>
     <row r="42" spans="2:7">
@@ -2161,15 +2169,17 @@
         <v>40</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>317</v>
+        <v>81</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>318</v>
+        <v>82</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F42" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="G42" s="1"/>
     </row>
     <row r="43" spans="2:7">
@@ -2177,10 +2187,10 @@
         <v>41</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>7</v>
@@ -2195,17 +2205,15 @@
         <v>42</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>88</v>
+        <v>317</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>87</v>
+        <v>318</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="F44" s="1"/>
       <c r="G44" s="1"/>
     </row>
     <row r="45" spans="2:7">
@@ -2213,10 +2221,10 @@
         <v>43</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>7</v>
@@ -2231,15 +2239,17 @@
         <v>44</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F46" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="G46" s="1"/>
     </row>
     <row r="47" spans="2:7">
@@ -2247,15 +2257,17 @@
         <v>45</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F47" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="G47" s="1"/>
     </row>
     <row r="48" spans="2:7">
@@ -2263,17 +2275,15 @@
         <v>46</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F48" s="1"/>
       <c r="G48" s="1"/>
     </row>
     <row r="49" spans="2:7">
@@ -2281,17 +2291,15 @@
         <v>47</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F49" s="1"/>
       <c r="G49" s="1"/>
     </row>
     <row r="50" spans="2:7">
@@ -2299,15 +2307,17 @@
         <v>48</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F50" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="G50" s="1"/>
     </row>
     <row r="51" spans="2:7">
@@ -2315,15 +2325,17 @@
         <v>49</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F51" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="G51" s="1"/>
     </row>
     <row r="52" spans="2:7">
@@ -2331,10 +2343,10 @@
         <v>50</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>5</v>
@@ -2347,10 +2359,10 @@
         <v>51</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>5</v>
@@ -2363,10 +2375,10 @@
         <v>52</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>5</v>
@@ -2379,10 +2391,10 @@
         <v>53</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>5</v>
@@ -2395,13 +2407,13 @@
         <v>54</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F56" s="1"/>
       <c r="G56" s="1"/>
@@ -2411,10 +2423,10 @@
         <v>55</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>5</v>
@@ -2427,13 +2439,13 @@
         <v>56</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F58" s="1"/>
       <c r="G58" s="1"/>
@@ -2443,17 +2455,15 @@
         <v>57</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F59" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F59" s="1"/>
       <c r="G59" s="1"/>
     </row>
     <row r="60" spans="2:7">
@@ -2461,17 +2471,15 @@
         <v>58</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F60" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F60" s="1"/>
       <c r="G60" s="1"/>
     </row>
     <row r="61" spans="2:7">
@@ -2479,15 +2487,17 @@
         <v>59</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F61" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="G61" s="1"/>
     </row>
     <row r="62" spans="2:7">
@@ -2495,16 +2505,16 @@
         <v>60</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="G62" s="1"/>
     </row>
@@ -2513,10 +2523,10 @@
         <v>61</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>5</v>
@@ -2529,15 +2539,17 @@
         <v>62</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F64" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="G64" s="1"/>
     </row>
     <row r="65" spans="2:7">
@@ -2545,10 +2557,10 @@
         <v>63</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="E65" s="1" t="s">
         <v>5</v>
@@ -2561,10 +2573,10 @@
         <v>64</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="E66" s="1" t="s">
         <v>5</v>
@@ -2577,10 +2589,10 @@
         <v>65</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="E67" s="1" t="s">
         <v>5</v>
@@ -2593,10 +2605,10 @@
         <v>66</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>5</v>
@@ -2609,10 +2621,10 @@
         <v>67</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E69" s="1" t="s">
         <v>5</v>
@@ -2625,10 +2637,10 @@
         <v>68</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="E70" s="1" t="s">
         <v>5</v>
@@ -2641,17 +2653,15 @@
         <v>69</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F71" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F71" s="1"/>
       <c r="G71" s="1"/>
     </row>
     <row r="72" spans="2:7">
@@ -2659,10 +2669,10 @@
         <v>70</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="E72" s="1" t="s">
         <v>5</v>
@@ -2675,10 +2685,10 @@
         <v>71</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E73" s="1" t="s">
         <v>7</v>
@@ -2693,10 +2703,10 @@
         <v>72</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="E74" s="1" t="s">
         <v>5</v>
@@ -2709,10 +2719,10 @@
         <v>73</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="E75" s="1" t="s">
         <v>7</v>
@@ -2727,10 +2737,10 @@
         <v>74</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="E76" s="1" t="s">
         <v>5</v>
@@ -2743,15 +2753,17 @@
         <v>75</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F77" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="G77" s="1"/>
     </row>
     <row r="78" spans="2:7">
@@ -2759,10 +2771,10 @@
         <v>76</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="E78" s="1" t="s">
         <v>5</v>
@@ -2775,10 +2787,10 @@
         <v>77</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="E79" s="1" t="s">
         <v>5</v>
@@ -2791,10 +2803,10 @@
         <v>78</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="E80" s="1" t="s">
         <v>5</v>
@@ -2807,17 +2819,15 @@
         <v>79</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F81" s="1" t="s">
-        <v>34</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F81" s="1"/>
       <c r="G81" s="1"/>
     </row>
     <row r="82" spans="2:7">
@@ -2825,17 +2835,15 @@
         <v>80</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F82" s="1" t="s">
-        <v>34</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F82" s="1"/>
       <c r="G82" s="1"/>
     </row>
     <row r="83" spans="2:7">
@@ -2843,16 +2851,16 @@
         <v>81</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="E83" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="G83" s="1"/>
     </row>
@@ -2861,15 +2869,17 @@
         <v>82</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F84" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="G84" s="1"/>
     </row>
     <row r="85" spans="2:7">
@@ -2877,15 +2887,17 @@
         <v>83</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F85" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="G85" s="1"/>
     </row>
     <row r="86" spans="2:7">
@@ -2893,10 +2905,10 @@
         <v>84</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="E86" s="1" t="s">
         <v>5</v>
@@ -2909,13 +2921,13 @@
         <v>85</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F87" s="1"/>
       <c r="G87" s="1"/>
@@ -2925,10 +2937,10 @@
         <v>86</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="E88" s="1" t="s">
         <v>5</v>
@@ -2941,10 +2953,10 @@
         <v>87</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="E89" s="1" t="s">
         <v>5</v>
@@ -2957,10 +2969,10 @@
         <v>88</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="E90" s="1" t="s">
         <v>5</v>
@@ -2973,10 +2985,10 @@
         <v>89</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="E91" s="1" t="s">
         <v>5</v>
@@ -2989,10 +3001,10 @@
         <v>90</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="E92" s="1" t="s">
         <v>5</v>
@@ -3005,10 +3017,10 @@
         <v>91</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="E93" s="1" t="s">
         <v>5</v>
@@ -3021,10 +3033,10 @@
         <v>92</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E94" s="1" t="s">
         <v>5</v>
@@ -3037,17 +3049,15 @@
         <v>93</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F95" s="1" t="s">
-        <v>34</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F95" s="1"/>
       <c r="G95" s="1"/>
     </row>
     <row r="96" spans="2:7">
@@ -3055,10 +3065,10 @@
         <v>94</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="E96" s="1" t="s">
         <v>5</v>
@@ -3071,15 +3081,17 @@
         <v>95</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F97" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F97" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="G97" s="1"/>
     </row>
     <row r="98" spans="2:7">
@@ -3087,10 +3099,10 @@
         <v>96</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="E98" s="1" t="s">
         <v>5</v>
@@ -3103,10 +3115,10 @@
         <v>97</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="E99" s="1" t="s">
         <v>5</v>
@@ -3119,10 +3131,10 @@
         <v>98</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="E100" s="1" t="s">
         <v>5</v>
@@ -3135,10 +3147,10 @@
         <v>99</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="E101" s="1" t="s">
         <v>5</v>
@@ -3151,10 +3163,10 @@
         <v>100</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="E102" s="1" t="s">
         <v>5</v>
@@ -3167,10 +3179,10 @@
         <v>101</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="E103" s="1" t="s">
         <v>5</v>
@@ -3183,17 +3195,15 @@
         <v>102</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F104" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F104" s="1"/>
       <c r="G104" s="1"/>
     </row>
     <row r="105" spans="2:7">
@@ -3201,10 +3211,10 @@
         <v>103</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E105" s="1" t="s">
         <v>5</v>
@@ -3217,15 +3227,17 @@
         <v>104</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F106" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F106" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="G106" s="1"/>
     </row>
     <row r="107" spans="2:7">
@@ -3233,10 +3245,10 @@
         <v>105</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="E107" s="1" t="s">
         <v>5</v>
@@ -3249,10 +3261,10 @@
         <v>106</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="E108" s="1" t="s">
         <v>5</v>
@@ -3265,13 +3277,13 @@
         <v>107</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F109" s="1"/>
       <c r="G109" s="1"/>
@@ -3281,10 +3293,10 @@
         <v>108</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="E110" s="1" t="s">
         <v>5</v>
@@ -3297,13 +3309,13 @@
         <v>109</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F111" s="1"/>
       <c r="G111" s="1"/>
@@ -3313,10 +3325,10 @@
         <v>110</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="E112" s="1" t="s">
         <v>5</v>
@@ -3329,17 +3341,15 @@
         <v>111</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F113" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F113" s="1"/>
       <c r="G113" s="1"/>
     </row>
     <row r="114" spans="2:7">
@@ -3347,10 +3357,10 @@
         <v>112</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="E114" s="1" t="s">
         <v>5</v>
@@ -3363,15 +3373,17 @@
         <v>113</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F115" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F115" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="G115" s="1"/>
     </row>
     <row r="116" spans="2:7">
@@ -3379,17 +3391,15 @@
         <v>114</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F116" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F116" s="1"/>
       <c r="G116" s="1"/>
     </row>
     <row r="117" spans="2:7">
@@ -3397,50 +3407,44 @@
         <v>115</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F117" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G117" s="1" t="s">
-        <v>37</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F117" s="1"/>
+      <c r="G117" s="1"/>
     </row>
     <row r="118" spans="2:7">
       <c r="B118" s="6">
         <v>116</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="E118" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F118" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G118" s="1" t="s">
-        <v>37</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="G118" s="1"/>
     </row>
     <row r="119" spans="2:7">
       <c r="B119" s="6">
         <v>117</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="E119" s="1" t="s">
         <v>7</v>
@@ -3449,7 +3453,7 @@
         <v>34</v>
       </c>
       <c r="G119" s="1" t="s">
-        <v>315</v>
+        <v>37</v>
       </c>
     </row>
     <row r="120" spans="2:7">
@@ -3457,10 +3461,10 @@
         <v>118</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="E120" s="1" t="s">
         <v>7</v>
@@ -3468,38 +3472,46 @@
       <c r="F120" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G120" s="1"/>
+      <c r="G120" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="121" spans="2:7">
       <c r="B121" s="6">
         <v>119</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F121" s="1"/>
-      <c r="G121" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F121" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G121" s="1" t="s">
+        <v>315</v>
+      </c>
     </row>
     <row r="122" spans="2:7">
       <c r="B122" s="6">
         <v>120</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F122" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F122" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="G122" s="1"/>
     </row>
     <row r="123" spans="2:7">
@@ -3507,17 +3519,15 @@
         <v>121</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="E123" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F123" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F123" s="1"/>
       <c r="G123" s="1"/>
     </row>
     <row r="124" spans="2:7">
@@ -3525,17 +3535,15 @@
         <v>122</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F124" s="1" t="s">
-        <v>34</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F124" s="1"/>
       <c r="G124" s="1"/>
     </row>
     <row r="125" spans="2:7">
@@ -3543,15 +3551,17 @@
         <v>123</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F125" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F125" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="G125" s="1"/>
     </row>
     <row r="126" spans="2:7">
@@ -3559,15 +3569,17 @@
         <v>124</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F126" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F126" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="G126" s="1"/>
     </row>
     <row r="127" spans="2:7">
@@ -3575,10 +3587,10 @@
         <v>125</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="E127" s="1" t="s">
         <v>5</v>
@@ -3591,10 +3603,10 @@
         <v>126</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="E128" s="1" t="s">
         <v>5</v>
@@ -3607,10 +3619,10 @@
         <v>127</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="E129" s="1" t="s">
         <v>5</v>
@@ -3623,17 +3635,15 @@
         <v>128</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="E130" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F130" s="1" t="s">
-        <v>34</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F130" s="1"/>
       <c r="G130" s="1"/>
     </row>
     <row r="131" spans="2:7">
@@ -3641,13 +3651,13 @@
         <v>129</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="E131" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F131" s="1"/>
       <c r="G131" s="1"/>
@@ -3657,15 +3667,17 @@
         <v>130</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="E132" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F132" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F132" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="G132" s="1"/>
     </row>
     <row r="133" spans="2:7">
@@ -3673,13 +3685,13 @@
         <v>131</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="E133" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F133" s="1"/>
       <c r="G133" s="1"/>
@@ -3689,10 +3701,10 @@
         <v>132</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="E134" s="1" t="s">
         <v>5</v>
@@ -3705,10 +3717,10 @@
         <v>133</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="E135" s="1" t="s">
         <v>5</v>
@@ -3721,10 +3733,10 @@
         <v>134</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="E136" s="1" t="s">
         <v>5</v>
@@ -3737,10 +3749,10 @@
         <v>135</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="E137" s="1" t="s">
         <v>5</v>
@@ -3753,17 +3765,15 @@
         <v>136</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="E138" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F138" s="1" t="s">
-        <v>34</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F138" s="1"/>
       <c r="G138" s="1"/>
     </row>
     <row r="139" spans="2:7">
@@ -3771,10 +3781,10 @@
         <v>137</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="E139" s="1" t="s">
         <v>5</v>
@@ -3787,15 +3797,17 @@
         <v>138</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="E140" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F140" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F140" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="G140" s="1"/>
     </row>
     <row r="141" spans="2:7">
@@ -3803,17 +3815,15 @@
         <v>139</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="E141" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F141" s="1" t="s">
-        <v>34</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F141" s="1"/>
       <c r="G141" s="1"/>
     </row>
     <row r="142" spans="2:7">
@@ -3821,10 +3831,10 @@
         <v>140</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="E142" s="1" t="s">
         <v>5</v>
@@ -3837,15 +3847,17 @@
         <v>141</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="E143" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F143" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F143" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="G143" s="1"/>
     </row>
     <row r="144" spans="2:7">
@@ -3853,10 +3865,10 @@
         <v>142</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="E144" s="1" t="s">
         <v>5</v>
@@ -3869,10 +3881,10 @@
         <v>143</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="E145" s="1" t="s">
         <v>5</v>
@@ -3885,10 +3897,10 @@
         <v>144</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="E146" s="1" t="s">
         <v>5</v>
@@ -3901,10 +3913,10 @@
         <v>145</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>10</v>
+        <v>290</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="E147" s="1" t="s">
         <v>5</v>
@@ -3917,17 +3929,15 @@
         <v>146</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="E148" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F148" s="1" t="s">
-        <v>34</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F148" s="1"/>
       <c r="G148" s="1"/>
     </row>
     <row r="149" spans="2:7">
@@ -3935,10 +3945,10 @@
         <v>147</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>297</v>
+        <v>10</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="E149" s="1" t="s">
         <v>5</v>
@@ -3951,15 +3961,17 @@
         <v>148</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="E150" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F150" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F150" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="G150" s="1"/>
     </row>
     <row r="151" spans="2:7">
@@ -3967,17 +3979,15 @@
         <v>149</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="E151" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F151" s="1" t="s">
-        <v>34</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F151" s="1"/>
       <c r="G151" s="1"/>
     </row>
     <row r="152" spans="2:7">
@@ -3985,17 +3995,15 @@
         <v>150</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="E152" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F152" s="1" t="s">
-        <v>34</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="F152" s="1"/>
       <c r="G152" s="1"/>
     </row>
     <row r="153" spans="2:7">
@@ -4003,10 +4011,10 @@
         <v>151</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="E153" s="1" t="s">
         <v>7</v>
@@ -4021,15 +4029,17 @@
         <v>152</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="E154" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F154" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F154" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="G154" s="1"/>
     </row>
     <row r="155" spans="2:7">
@@ -4037,10 +4047,10 @@
         <v>153</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="D155" s="1" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="E155" s="1" t="s">
         <v>7</v>
@@ -4055,10 +4065,10 @@
         <v>154</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="E156" s="1" t="s">
         <v>5</v>
@@ -4071,30 +4081,48 @@
         <v>155</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="E157" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F157" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F157" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="G157" s="1"/>
     </row>
     <row r="158" spans="2:7">
-      <c r="B158" s="6"/>
-      <c r="C158" s="1"/>
-      <c r="D158" s="1"/>
-      <c r="E158" s="1"/>
+      <c r="B158" s="6">
+        <v>156</v>
+      </c>
+      <c r="C158" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="D158" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="E158" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F158" s="1"/>
       <c r="G158" s="1"/>
     </row>
     <row r="159" spans="2:7">
-      <c r="B159" s="6"/>
-      <c r="C159" s="1"/>
-      <c r="D159" s="1"/>
-      <c r="E159" s="1"/>
+      <c r="B159" s="6">
+        <v>157</v>
+      </c>
+      <c r="C159" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="D159" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="E159" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F159" s="1"/>
       <c r="G159" s="1"/>
     </row>
@@ -4114,12 +4142,28 @@
       <c r="F161" s="1"/>
       <c r="G161" s="1"/>
     </row>
+    <row r="162" spans="2:7">
+      <c r="B162" s="6"/>
+      <c r="C162" s="1"/>
+      <c r="D162" s="1"/>
+      <c r="E162" s="1"/>
+      <c r="F162" s="1"/>
+      <c r="G162" s="1"/>
+    </row>
+    <row r="163" spans="2:7">
+      <c r="B163" s="6"/>
+      <c r="C163" s="1"/>
+      <c r="D163" s="1"/>
+      <c r="E163" s="1"/>
+      <c r="F163" s="1"/>
+      <c r="G163" s="1"/>
+    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E157" xr:uid="{7E8CE32C-29D1-4006-9E0F-69B72A0F4378}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E159" xr:uid="{7E8CE32C-29D1-4006-9E0F-69B72A0F4378}">
       <formula1>"[Application],[Directory],[Script]"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F161" xr:uid="{A5D947FB-5606-4B36-88C5-81CC2B61C636}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F163" xr:uid="{A5D947FB-5606-4B36-88C5-81CC2B61C636}">
       <formula1>"[bat],[vbs]"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Repo Update: 2024-05-31 18:26:42
</commit_message>
<xml_diff>
--- a/Database/Run_shortcut_creator_aliases.xlsx
+++ b/Database/Run_shortcut_creator_aliases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\player-1\Documents\Windows-Git-Repos\win-t\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C0DD10C-EDB2-4BC0-A35D-19EC7E77E3B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C7EFBA6-2E39-404E-861A-7520011F1A6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D65865D6-BB34-410C-8183-31ED199784FF}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="327">
   <si>
     <t>Number</t>
   </si>
@@ -1033,13 +1033,19 @@
   </si>
   <si>
     <t>C:\MY-TOOLS\Windows Store\Alternative Windows Apps Installer\alt app installer</t>
+  </si>
+  <si>
+    <t>Librewolf (Mails)</t>
+  </si>
+  <si>
+    <t>mails</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1464,24 +1470,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58A033C2-67FB-408D-B72B-8C45836FCF74}">
-  <dimension ref="B2:G163"/>
+  <dimension ref="B2:G164"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A127" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
-      <selection activeCell="P151" sqref="P151"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A142" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
+      <selection activeCell="D87" sqref="D87"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="21"/>
+  <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="13.625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="93.5" style="4" customWidth="1"/>
-    <col min="4" max="4" width="19.375" style="4" customWidth="1"/>
-    <col min="5" max="5" width="25.75" style="5" customWidth="1"/>
-    <col min="6" max="6" width="28.25" style="5" customWidth="1"/>
-    <col min="7" max="7" width="22.875" style="4" customWidth="1"/>
-    <col min="8" max="8" width="15.625" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="93.42578125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="25.7109375" style="5" customWidth="1"/>
+    <col min="6" max="6" width="28.28515625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="22.85546875" style="4" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" s="3" customFormat="1" ht="24.95" customHeight="1">
+    <row r="2" spans="2:7" s="3" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1501,9 +1507,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:7" ht="24.95" customHeight="1">
+    <row r="3" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="6" cm="1">
-        <f t="array" ref="B3:B159">_xlfn.SEQUENCE(COUNTA(C:C)-1)</f>
+        <f t="array" ref="B3:B160">_xlfn.SEQUENCE(COUNTA(C:C)-1)</f>
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -1518,7 +1524,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="2:7" ht="24.95" customHeight="1">
+    <row r="4" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="6">
         <v>2</v>
       </c>
@@ -1534,7 +1540,7 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="2:7" ht="24.95" customHeight="1">
+    <row r="5" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="6">
         <v>3</v>
       </c>
@@ -1550,7 +1556,7 @@
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="2:7" ht="24.95" customHeight="1">
+    <row r="6" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="6">
         <v>4</v>
       </c>
@@ -1566,7 +1572,7 @@
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="2:7" ht="24.95" customHeight="1">
+    <row r="7" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="6">
         <v>5</v>
       </c>
@@ -1584,7 +1590,7 @@
       </c>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="2:7" ht="24.95" customHeight="1">
+    <row r="8" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="6">
         <v>6</v>
       </c>
@@ -1604,7 +1610,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="2:7" ht="24.95" customHeight="1">
+    <row r="9" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="6">
         <v>7</v>
       </c>
@@ -1620,7 +1626,7 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="2:7" ht="24.95" customHeight="1">
+    <row r="10" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="6">
         <v>8</v>
       </c>
@@ -1636,7 +1642,7 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="2:7" ht="24.95" customHeight="1">
+    <row r="11" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="6">
         <v>9</v>
       </c>
@@ -1652,7 +1658,7 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="2:7" ht="24.95" customHeight="1">
+    <row r="12" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="6">
         <v>10</v>
       </c>
@@ -1668,7 +1674,7 @@
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="2:7" ht="24.95" customHeight="1">
+    <row r="13" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="6">
         <v>11</v>
       </c>
@@ -1686,7 +1692,7 @@
       </c>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="2:7" ht="24.95" customHeight="1">
+    <row r="14" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="6">
         <v>12</v>
       </c>
@@ -1704,7 +1710,7 @@
       </c>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="2:7" ht="24.95" customHeight="1">
+    <row r="15" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="6">
         <v>13</v>
       </c>
@@ -1720,7 +1726,7 @@
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="2:7" ht="24.95" customHeight="1">
+    <row r="16" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="6">
         <v>14</v>
       </c>
@@ -1740,7 +1746,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="2:7" ht="24.95" customHeight="1">
+    <row r="17" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="6">
         <v>15</v>
       </c>
@@ -1760,7 +1766,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="2:7" ht="24.95" customHeight="1">
+    <row r="18" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="6">
         <v>16</v>
       </c>
@@ -1776,7 +1782,7 @@
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
     </row>
-    <row r="19" spans="2:7" ht="24.95" customHeight="1">
+    <row r="19" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B19" s="6">
         <v>17</v>
       </c>
@@ -1792,7 +1798,7 @@
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
     </row>
-    <row r="20" spans="2:7" ht="24.95" customHeight="1">
+    <row r="20" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B20" s="6">
         <v>18</v>
       </c>
@@ -1810,7 +1816,7 @@
       </c>
       <c r="G20" s="1"/>
     </row>
-    <row r="21" spans="2:7" ht="24.95" customHeight="1">
+    <row r="21" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B21" s="6">
         <v>19</v>
       </c>
@@ -1828,7 +1834,7 @@
       </c>
       <c r="G21" s="1"/>
     </row>
-    <row r="22" spans="2:7" ht="24.95" customHeight="1">
+    <row r="22" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B22" s="6">
         <v>20</v>
       </c>
@@ -1844,7 +1850,7 @@
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
     </row>
-    <row r="23" spans="2:7" ht="24.95" customHeight="1">
+    <row r="23" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B23" s="6">
         <v>21</v>
       </c>
@@ -1860,7 +1866,7 @@
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
     </row>
-    <row r="24" spans="2:7" ht="24.95" customHeight="1">
+    <row r="24" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B24" s="6">
         <v>22</v>
       </c>
@@ -1878,7 +1884,7 @@
       </c>
       <c r="G24" s="1"/>
     </row>
-    <row r="25" spans="2:7" ht="24.95" customHeight="1">
+    <row r="25" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B25" s="6">
         <v>23</v>
       </c>
@@ -1896,7 +1902,7 @@
       </c>
       <c r="G25" s="1"/>
     </row>
-    <row r="26" spans="2:7" ht="24.95" customHeight="1">
+    <row r="26" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B26" s="6">
         <v>24</v>
       </c>
@@ -1912,7 +1918,7 @@
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
     </row>
-    <row r="27" spans="2:7" ht="24.95" customHeight="1">
+    <row r="27" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B27" s="6">
         <v>25</v>
       </c>
@@ -1928,7 +1934,7 @@
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
     </row>
-    <row r="28" spans="2:7" ht="24.95" customHeight="1">
+    <row r="28" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B28" s="6">
         <v>26</v>
       </c>
@@ -1946,7 +1952,7 @@
       </c>
       <c r="G28" s="1"/>
     </row>
-    <row r="29" spans="2:7" ht="24.95" customHeight="1">
+    <row r="29" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B29" s="6">
         <v>27</v>
       </c>
@@ -1962,7 +1968,7 @@
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
     </row>
-    <row r="30" spans="2:7" ht="24.95" customHeight="1">
+    <row r="30" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B30" s="6">
         <v>28</v>
       </c>
@@ -1978,7 +1984,7 @@
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
     </row>
-    <row r="31" spans="2:7" ht="24.95" customHeight="1">
+    <row r="31" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B31" s="6">
         <v>29</v>
       </c>
@@ -1994,7 +2000,7 @@
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
     </row>
-    <row r="32" spans="2:7" ht="24.95" customHeight="1">
+    <row r="32" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B32" s="6">
         <v>30</v>
       </c>
@@ -2010,7 +2016,7 @@
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
     </row>
-    <row r="33" spans="2:7" ht="24.95" customHeight="1">
+    <row r="33" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B33" s="6">
         <v>31</v>
       </c>
@@ -2028,7 +2034,7 @@
       </c>
       <c r="G33" s="1"/>
     </row>
-    <row r="34" spans="2:7" ht="24.95" customHeight="1">
+    <row r="34" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B34" s="6">
         <v>32</v>
       </c>
@@ -2046,7 +2052,7 @@
       </c>
       <c r="G34" s="1"/>
     </row>
-    <row r="35" spans="2:7" ht="24.95" customHeight="1">
+    <row r="35" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B35" s="6">
         <v>33</v>
       </c>
@@ -2064,7 +2070,7 @@
       </c>
       <c r="G35" s="1"/>
     </row>
-    <row r="36" spans="2:7" ht="24.95" customHeight="1">
+    <row r="36" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B36" s="6">
         <v>34</v>
       </c>
@@ -2080,7 +2086,7 @@
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
     </row>
-    <row r="37" spans="2:7" ht="24.95" customHeight="1">
+    <row r="37" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B37" s="6">
         <v>35</v>
       </c>
@@ -2096,7 +2102,7 @@
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
     </row>
-    <row r="38" spans="2:7">
+    <row r="38" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B38" s="6">
         <v>36</v>
       </c>
@@ -2114,7 +2120,7 @@
       </c>
       <c r="G38" s="1"/>
     </row>
-    <row r="39" spans="2:7">
+    <row r="39" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B39" s="6">
         <v>37</v>
       </c>
@@ -2130,7 +2136,7 @@
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
     </row>
-    <row r="40" spans="2:7">
+    <row r="40" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B40" s="6">
         <v>38</v>
       </c>
@@ -2148,7 +2154,7 @@
       </c>
       <c r="G40" s="1"/>
     </row>
-    <row r="41" spans="2:7">
+    <row r="41" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B41" s="6">
         <v>39</v>
       </c>
@@ -2164,7 +2170,7 @@
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
     </row>
-    <row r="42" spans="2:7">
+    <row r="42" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B42" s="6">
         <v>40</v>
       </c>
@@ -2182,7 +2188,7 @@
       </c>
       <c r="G42" s="1"/>
     </row>
-    <row r="43" spans="2:7">
+    <row r="43" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B43" s="6">
         <v>41</v>
       </c>
@@ -2200,7 +2206,7 @@
       </c>
       <c r="G43" s="1"/>
     </row>
-    <row r="44" spans="2:7">
+    <row r="44" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B44" s="6">
         <v>42</v>
       </c>
@@ -2216,7 +2222,7 @@
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
     </row>
-    <row r="45" spans="2:7">
+    <row r="45" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B45" s="6">
         <v>43</v>
       </c>
@@ -2234,7 +2240,7 @@
       </c>
       <c r="G45" s="1"/>
     </row>
-    <row r="46" spans="2:7">
+    <row r="46" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B46" s="6">
         <v>44</v>
       </c>
@@ -2252,7 +2258,7 @@
       </c>
       <c r="G46" s="1"/>
     </row>
-    <row r="47" spans="2:7">
+    <row r="47" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B47" s="6">
         <v>45</v>
       </c>
@@ -2270,7 +2276,7 @@
       </c>
       <c r="G47" s="1"/>
     </row>
-    <row r="48" spans="2:7">
+    <row r="48" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B48" s="6">
         <v>46</v>
       </c>
@@ -2286,7 +2292,7 @@
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
     </row>
-    <row r="49" spans="2:7">
+    <row r="49" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B49" s="6">
         <v>47</v>
       </c>
@@ -2302,7 +2308,7 @@
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
     </row>
-    <row r="50" spans="2:7">
+    <row r="50" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B50" s="6">
         <v>48</v>
       </c>
@@ -2320,7 +2326,7 @@
       </c>
       <c r="G50" s="1"/>
     </row>
-    <row r="51" spans="2:7">
+    <row r="51" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B51" s="6">
         <v>49</v>
       </c>
@@ -2338,7 +2344,7 @@
       </c>
       <c r="G51" s="1"/>
     </row>
-    <row r="52" spans="2:7">
+    <row r="52" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B52" s="6">
         <v>50</v>
       </c>
@@ -2354,7 +2360,7 @@
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
     </row>
-    <row r="53" spans="2:7">
+    <row r="53" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B53" s="6">
         <v>51</v>
       </c>
@@ -2370,7 +2376,7 @@
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
     </row>
-    <row r="54" spans="2:7">
+    <row r="54" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B54" s="6">
         <v>52</v>
       </c>
@@ -2386,7 +2392,7 @@
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
     </row>
-    <row r="55" spans="2:7">
+    <row r="55" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B55" s="6">
         <v>53</v>
       </c>
@@ -2402,7 +2408,7 @@
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
     </row>
-    <row r="56" spans="2:7">
+    <row r="56" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B56" s="6">
         <v>54</v>
       </c>
@@ -2418,7 +2424,7 @@
       <c r="F56" s="1"/>
       <c r="G56" s="1"/>
     </row>
-    <row r="57" spans="2:7">
+    <row r="57" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B57" s="6">
         <v>55</v>
       </c>
@@ -2434,7 +2440,7 @@
       <c r="F57" s="1"/>
       <c r="G57" s="1"/>
     </row>
-    <row r="58" spans="2:7">
+    <row r="58" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B58" s="6">
         <v>56</v>
       </c>
@@ -2450,7 +2456,7 @@
       <c r="F58" s="1"/>
       <c r="G58" s="1"/>
     </row>
-    <row r="59" spans="2:7">
+    <row r="59" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B59" s="6">
         <v>57</v>
       </c>
@@ -2466,7 +2472,7 @@
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
     </row>
-    <row r="60" spans="2:7">
+    <row r="60" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B60" s="6">
         <v>58</v>
       </c>
@@ -2482,7 +2488,7 @@
       <c r="F60" s="1"/>
       <c r="G60" s="1"/>
     </row>
-    <row r="61" spans="2:7">
+    <row r="61" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B61" s="6">
         <v>59</v>
       </c>
@@ -2500,7 +2506,7 @@
       </c>
       <c r="G61" s="1"/>
     </row>
-    <row r="62" spans="2:7">
+    <row r="62" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B62" s="6">
         <v>60</v>
       </c>
@@ -2518,7 +2524,7 @@
       </c>
       <c r="G62" s="1"/>
     </row>
-    <row r="63" spans="2:7">
+    <row r="63" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B63" s="6">
         <v>61</v>
       </c>
@@ -2534,7 +2540,7 @@
       <c r="F63" s="1"/>
       <c r="G63" s="1"/>
     </row>
-    <row r="64" spans="2:7">
+    <row r="64" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B64" s="6">
         <v>62</v>
       </c>
@@ -2552,7 +2558,7 @@
       </c>
       <c r="G64" s="1"/>
     </row>
-    <row r="65" spans="2:7">
+    <row r="65" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B65" s="6">
         <v>63</v>
       </c>
@@ -2568,7 +2574,7 @@
       <c r="F65" s="1"/>
       <c r="G65" s="1"/>
     </row>
-    <row r="66" spans="2:7">
+    <row r="66" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B66" s="6">
         <v>64</v>
       </c>
@@ -2584,7 +2590,7 @@
       <c r="F66" s="1"/>
       <c r="G66" s="1"/>
     </row>
-    <row r="67" spans="2:7">
+    <row r="67" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B67" s="6">
         <v>65</v>
       </c>
@@ -2600,7 +2606,7 @@
       <c r="F67" s="1"/>
       <c r="G67" s="1"/>
     </row>
-    <row r="68" spans="2:7">
+    <row r="68" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B68" s="6">
         <v>66</v>
       </c>
@@ -2616,7 +2622,7 @@
       <c r="F68" s="1"/>
       <c r="G68" s="1"/>
     </row>
-    <row r="69" spans="2:7">
+    <row r="69" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B69" s="6">
         <v>67</v>
       </c>
@@ -2632,7 +2638,7 @@
       <c r="F69" s="1"/>
       <c r="G69" s="1"/>
     </row>
-    <row r="70" spans="2:7">
+    <row r="70" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B70" s="6">
         <v>68</v>
       </c>
@@ -2648,7 +2654,7 @@
       <c r="F70" s="1"/>
       <c r="G70" s="1"/>
     </row>
-    <row r="71" spans="2:7">
+    <row r="71" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B71" s="6">
         <v>69</v>
       </c>
@@ -2664,7 +2670,7 @@
       <c r="F71" s="1"/>
       <c r="G71" s="1"/>
     </row>
-    <row r="72" spans="2:7">
+    <row r="72" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B72" s="6">
         <v>70</v>
       </c>
@@ -2680,7 +2686,7 @@
       <c r="F72" s="1"/>
       <c r="G72" s="1"/>
     </row>
-    <row r="73" spans="2:7">
+    <row r="73" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B73" s="6">
         <v>71</v>
       </c>
@@ -2698,7 +2704,7 @@
       </c>
       <c r="G73" s="1"/>
     </row>
-    <row r="74" spans="2:7">
+    <row r="74" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B74" s="6">
         <v>72</v>
       </c>
@@ -2714,7 +2720,7 @@
       <c r="F74" s="1"/>
       <c r="G74" s="1"/>
     </row>
-    <row r="75" spans="2:7">
+    <row r="75" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B75" s="6">
         <v>73</v>
       </c>
@@ -2732,7 +2738,7 @@
       </c>
       <c r="G75" s="1"/>
     </row>
-    <row r="76" spans="2:7">
+    <row r="76" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B76" s="6">
         <v>74</v>
       </c>
@@ -2748,7 +2754,7 @@
       <c r="F76" s="1"/>
       <c r="G76" s="1"/>
     </row>
-    <row r="77" spans="2:7">
+    <row r="77" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B77" s="6">
         <v>75</v>
       </c>
@@ -2766,7 +2772,7 @@
       </c>
       <c r="G77" s="1"/>
     </row>
-    <row r="78" spans="2:7">
+    <row r="78" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B78" s="6">
         <v>76</v>
       </c>
@@ -2782,15 +2788,15 @@
       <c r="F78" s="1"/>
       <c r="G78" s="1"/>
     </row>
-    <row r="79" spans="2:7">
+    <row r="79" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B79" s="6">
         <v>77</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>154</v>
+        <v>325</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>155</v>
+        <v>326</v>
       </c>
       <c r="E79" s="1" t="s">
         <v>5</v>
@@ -2798,15 +2804,15 @@
       <c r="F79" s="1"/>
       <c r="G79" s="1"/>
     </row>
-    <row r="80" spans="2:7">
+    <row r="80" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B80" s="6">
         <v>78</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E80" s="1" t="s">
         <v>5</v>
@@ -2814,15 +2820,15 @@
       <c r="F80" s="1"/>
       <c r="G80" s="1"/>
     </row>
-    <row r="81" spans="2:7">
+    <row r="81" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B81" s="6">
         <v>79</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E81" s="1" t="s">
         <v>5</v>
@@ -2830,15 +2836,15 @@
       <c r="F81" s="1"/>
       <c r="G81" s="1"/>
     </row>
-    <row r="82" spans="2:7">
+    <row r="82" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B82" s="6">
         <v>80</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E82" s="1" t="s">
         <v>5</v>
@@ -2846,33 +2852,31 @@
       <c r="F82" s="1"/>
       <c r="G82" s="1"/>
     </row>
-    <row r="83" spans="2:7">
+    <row r="83" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B83" s="6">
         <v>81</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F83" s="1" t="s">
-        <v>34</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F83" s="1"/>
       <c r="G83" s="1"/>
     </row>
-    <row r="84" spans="2:7">
+    <row r="84" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B84" s="6">
         <v>82</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E84" s="1" t="s">
         <v>7</v>
@@ -2882,81 +2886,83 @@
       </c>
       <c r="G84" s="1"/>
     </row>
-    <row r="85" spans="2:7">
+    <row r="85" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B85" s="6">
         <v>83</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E85" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="G85" s="1"/>
     </row>
-    <row r="86" spans="2:7">
+    <row r="86" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B86" s="6">
         <v>84</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F86" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F86" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="G86" s="1"/>
     </row>
-    <row r="87" spans="2:7">
+    <row r="87" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B87" s="6">
         <v>85</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F87" s="1"/>
       <c r="G87" s="1"/>
     </row>
-    <row r="88" spans="2:7">
+    <row r="88" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B88" s="6">
         <v>86</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F88" s="1"/>
       <c r="G88" s="1"/>
     </row>
-    <row r="89" spans="2:7">
+    <row r="89" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B89" s="6">
         <v>87</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E89" s="1" t="s">
         <v>5</v>
@@ -2964,15 +2970,15 @@
       <c r="F89" s="1"/>
       <c r="G89" s="1"/>
     </row>
-    <row r="90" spans="2:7">
+    <row r="90" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B90" s="6">
         <v>88</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E90" s="1" t="s">
         <v>5</v>
@@ -2980,15 +2986,15 @@
       <c r="F90" s="1"/>
       <c r="G90" s="1"/>
     </row>
-    <row r="91" spans="2:7">
+    <row r="91" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B91" s="6">
         <v>89</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E91" s="1" t="s">
         <v>5</v>
@@ -2996,15 +3002,15 @@
       <c r="F91" s="1"/>
       <c r="G91" s="1"/>
     </row>
-    <row r="92" spans="2:7">
+    <row r="92" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B92" s="6">
         <v>90</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E92" s="1" t="s">
         <v>5</v>
@@ -3012,15 +3018,15 @@
       <c r="F92" s="1"/>
       <c r="G92" s="1"/>
     </row>
-    <row r="93" spans="2:7">
+    <row r="93" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B93" s="6">
         <v>91</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E93" s="1" t="s">
         <v>5</v>
@@ -3028,15 +3034,15 @@
       <c r="F93" s="1"/>
       <c r="G93" s="1"/>
     </row>
-    <row r="94" spans="2:7">
+    <row r="94" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B94" s="6">
         <v>92</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E94" s="1" t="s">
         <v>5</v>
@@ -3044,15 +3050,15 @@
       <c r="F94" s="1"/>
       <c r="G94" s="1"/>
     </row>
-    <row r="95" spans="2:7">
+    <row r="95" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B95" s="6">
         <v>93</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E95" s="1" t="s">
         <v>5</v>
@@ -3060,15 +3066,15 @@
       <c r="F95" s="1"/>
       <c r="G95" s="1"/>
     </row>
-    <row r="96" spans="2:7">
+    <row r="96" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B96" s="6">
         <v>94</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E96" s="1" t="s">
         <v>5</v>
@@ -3076,49 +3082,49 @@
       <c r="F96" s="1"/>
       <c r="G96" s="1"/>
     </row>
-    <row r="97" spans="2:7">
+    <row r="97" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B97" s="6">
         <v>95</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F97" s="1" t="s">
-        <v>34</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F97" s="1"/>
       <c r="G97" s="1"/>
     </row>
-    <row r="98" spans="2:7">
+    <row r="98" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B98" s="6">
         <v>96</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F98" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F98" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="G98" s="1"/>
     </row>
-    <row r="99" spans="2:7">
+    <row r="99" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B99" s="6">
         <v>97</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E99" s="1" t="s">
         <v>5</v>
@@ -3126,15 +3132,15 @@
       <c r="F99" s="1"/>
       <c r="G99" s="1"/>
     </row>
-    <row r="100" spans="2:7">
+    <row r="100" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B100" s="6">
         <v>98</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E100" s="1" t="s">
         <v>5</v>
@@ -3142,15 +3148,15 @@
       <c r="F100" s="1"/>
       <c r="G100" s="1"/>
     </row>
-    <row r="101" spans="2:7">
+    <row r="101" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B101" s="6">
         <v>99</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E101" s="1" t="s">
         <v>5</v>
@@ -3158,15 +3164,15 @@
       <c r="F101" s="1"/>
       <c r="G101" s="1"/>
     </row>
-    <row r="102" spans="2:7">
+    <row r="102" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B102" s="6">
         <v>100</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E102" s="1" t="s">
         <v>5</v>
@@ -3174,15 +3180,15 @@
       <c r="F102" s="1"/>
       <c r="G102" s="1"/>
     </row>
-    <row r="103" spans="2:7">
+    <row r="103" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B103" s="6">
         <v>101</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E103" s="1" t="s">
         <v>5</v>
@@ -3190,15 +3196,15 @@
       <c r="F103" s="1"/>
       <c r="G103" s="1"/>
     </row>
-    <row r="104" spans="2:7">
+    <row r="104" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B104" s="6">
         <v>102</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E104" s="1" t="s">
         <v>5</v>
@@ -3206,15 +3212,15 @@
       <c r="F104" s="1"/>
       <c r="G104" s="1"/>
     </row>
-    <row r="105" spans="2:7">
+    <row r="105" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B105" s="6">
         <v>103</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E105" s="1" t="s">
         <v>5</v>
@@ -3222,49 +3228,49 @@
       <c r="F105" s="1"/>
       <c r="G105" s="1"/>
     </row>
-    <row r="106" spans="2:7">
+    <row r="106" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B106" s="6">
         <v>104</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F106" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F106" s="1"/>
       <c r="G106" s="1"/>
     </row>
-    <row r="107" spans="2:7">
+    <row r="107" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B107" s="6">
         <v>105</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F107" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F107" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="G107" s="1"/>
     </row>
-    <row r="108" spans="2:7">
+    <row r="108" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B108" s="6">
         <v>106</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E108" s="1" t="s">
         <v>5</v>
@@ -3272,15 +3278,15 @@
       <c r="F108" s="1"/>
       <c r="G108" s="1"/>
     </row>
-    <row r="109" spans="2:7">
+    <row r="109" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B109" s="6">
         <v>107</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="E109" s="1" t="s">
         <v>5</v>
@@ -3288,15 +3294,15 @@
       <c r="F109" s="1"/>
       <c r="G109" s="1"/>
     </row>
-    <row r="110" spans="2:7">
+    <row r="110" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B110" s="6">
         <v>108</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E110" s="1" t="s">
         <v>5</v>
@@ -3304,47 +3310,47 @@
       <c r="F110" s="1"/>
       <c r="G110" s="1"/>
     </row>
-    <row r="111" spans="2:7">
+    <row r="111" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B111" s="6">
         <v>109</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F111" s="1"/>
       <c r="G111" s="1"/>
     </row>
-    <row r="112" spans="2:7">
+    <row r="112" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B112" s="6">
         <v>110</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F112" s="1"/>
       <c r="G112" s="1"/>
     </row>
-    <row r="113" spans="2:7">
+    <row r="113" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B113" s="6">
         <v>111</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E113" s="1" t="s">
         <v>5</v>
@@ -3352,15 +3358,15 @@
       <c r="F113" s="1"/>
       <c r="G113" s="1"/>
     </row>
-    <row r="114" spans="2:7">
+    <row r="114" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B114" s="6">
         <v>112</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E114" s="1" t="s">
         <v>5</v>
@@ -3368,49 +3374,49 @@
       <c r="F114" s="1"/>
       <c r="G114" s="1"/>
     </row>
-    <row r="115" spans="2:7">
+    <row r="115" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B115" s="6">
         <v>113</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F115" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F115" s="1"/>
       <c r="G115" s="1"/>
     </row>
-    <row r="116" spans="2:7">
+    <row r="116" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B116" s="6">
         <v>114</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F116" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F116" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="G116" s="1"/>
     </row>
-    <row r="117" spans="2:7">
+    <row r="117" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B117" s="6">
         <v>115</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E117" s="1" t="s">
         <v>5</v>
@@ -3418,53 +3424,49 @@
       <c r="F117" s="1"/>
       <c r="G117" s="1"/>
     </row>
-    <row r="118" spans="2:7">
+    <row r="118" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B118" s="6">
         <v>116</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F118" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F118" s="1"/>
       <c r="G118" s="1"/>
     </row>
-    <row r="119" spans="2:7">
+    <row r="119" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B119" s="6">
         <v>117</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="E119" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F119" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G119" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="120" spans="2:7">
+        <v>16</v>
+      </c>
+      <c r="G119" s="1"/>
+    </row>
+    <row r="120" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B120" s="6">
         <v>118</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E120" s="1" t="s">
         <v>7</v>
@@ -3476,15 +3478,15 @@
         <v>37</v>
       </c>
     </row>
-    <row r="121" spans="2:7">
+    <row r="121" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B121" s="6">
         <v>119</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="E121" s="1" t="s">
         <v>7</v>
@@ -3493,18 +3495,18 @@
         <v>34</v>
       </c>
       <c r="G121" s="1" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="122" spans="2:7">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="122" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B122" s="6">
         <v>120</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E122" s="1" t="s">
         <v>7</v>
@@ -3512,33 +3514,37 @@
       <c r="F122" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G122" s="1"/>
-    </row>
-    <row r="123" spans="2:7">
+      <c r="G122" s="1" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="123" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B123" s="6">
         <v>121</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="E123" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F123" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F123" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="G123" s="1"/>
     </row>
-    <row r="124" spans="2:7">
+    <row r="124" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B124" s="6">
         <v>122</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="E124" s="1" t="s">
         <v>5</v>
@@ -3546,67 +3552,67 @@
       <c r="F124" s="1"/>
       <c r="G124" s="1"/>
     </row>
-    <row r="125" spans="2:7">
+    <row r="125" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B125" s="6">
         <v>123</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F125" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F125" s="1"/>
       <c r="G125" s="1"/>
     </row>
-    <row r="126" spans="2:7">
+    <row r="126" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B126" s="6">
         <v>124</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E126" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F126" s="1" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="G126" s="1"/>
     </row>
-    <row r="127" spans="2:7">
+    <row r="127" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B127" s="6">
         <v>125</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F127" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F127" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="G127" s="1"/>
     </row>
-    <row r="128" spans="2:7">
+    <row r="128" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B128" s="6">
         <v>126</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="E128" s="1" t="s">
         <v>5</v>
@@ -3614,15 +3620,15 @@
       <c r="F128" s="1"/>
       <c r="G128" s="1"/>
     </row>
-    <row r="129" spans="2:7">
+    <row r="129" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B129" s="6">
         <v>127</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E129" s="1" t="s">
         <v>5</v>
@@ -3630,15 +3636,15 @@
       <c r="F129" s="1"/>
       <c r="G129" s="1"/>
     </row>
-    <row r="130" spans="2:7">
+    <row r="130" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B130" s="6">
         <v>128</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E130" s="1" t="s">
         <v>5</v>
@@ -3646,15 +3652,15 @@
       <c r="F130" s="1"/>
       <c r="G130" s="1"/>
     </row>
-    <row r="131" spans="2:7">
+    <row r="131" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B131" s="6">
         <v>129</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E131" s="1" t="s">
         <v>5</v>
@@ -3662,65 +3668,65 @@
       <c r="F131" s="1"/>
       <c r="G131" s="1"/>
     </row>
-    <row r="132" spans="2:7">
+    <row r="132" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B132" s="6">
         <v>130</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="E132" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F132" s="1" t="s">
-        <v>34</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F132" s="1"/>
       <c r="G132" s="1"/>
     </row>
-    <row r="133" spans="2:7">
+    <row r="133" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B133" s="6">
         <v>131</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="E133" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F133" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F133" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="G133" s="1"/>
     </row>
-    <row r="134" spans="2:7">
+    <row r="134" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B134" s="6">
         <v>132</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="E134" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F134" s="1"/>
       <c r="G134" s="1"/>
     </row>
-    <row r="135" spans="2:7">
+    <row r="135" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B135" s="6">
         <v>133</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="E135" s="1" t="s">
         <v>5</v>
@@ -3728,15 +3734,15 @@
       <c r="F135" s="1"/>
       <c r="G135" s="1"/>
     </row>
-    <row r="136" spans="2:7">
+    <row r="136" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B136" s="6">
         <v>134</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E136" s="1" t="s">
         <v>5</v>
@@ -3744,15 +3750,15 @@
       <c r="F136" s="1"/>
       <c r="G136" s="1"/>
     </row>
-    <row r="137" spans="2:7">
+    <row r="137" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B137" s="6">
         <v>135</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="E137" s="1" t="s">
         <v>5</v>
@@ -3760,15 +3766,15 @@
       <c r="F137" s="1"/>
       <c r="G137" s="1"/>
     </row>
-    <row r="138" spans="2:7">
+    <row r="138" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B138" s="6">
         <v>136</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E138" s="1" t="s">
         <v>5</v>
@@ -3776,15 +3782,15 @@
       <c r="F138" s="1"/>
       <c r="G138" s="1"/>
     </row>
-    <row r="139" spans="2:7">
+    <row r="139" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B139" s="6">
         <v>137</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="E139" s="1" t="s">
         <v>5</v>
@@ -3792,49 +3798,49 @@
       <c r="F139" s="1"/>
       <c r="G139" s="1"/>
     </row>
-    <row r="140" spans="2:7">
+    <row r="140" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B140" s="6">
         <v>138</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E140" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F140" s="1" t="s">
-        <v>34</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F140" s="1"/>
       <c r="G140" s="1"/>
     </row>
-    <row r="141" spans="2:7">
+    <row r="141" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B141" s="6">
         <v>139</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="E141" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F141" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F141" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="G141" s="1"/>
     </row>
-    <row r="142" spans="2:7">
+    <row r="142" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B142" s="6">
         <v>140</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E142" s="1" t="s">
         <v>5</v>
@@ -3842,49 +3848,49 @@
       <c r="F142" s="1"/>
       <c r="G142" s="1"/>
     </row>
-    <row r="143" spans="2:7">
+    <row r="143" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B143" s="6">
         <v>141</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E143" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F143" s="1" t="s">
-        <v>34</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F143" s="1"/>
       <c r="G143" s="1"/>
     </row>
-    <row r="144" spans="2:7">
+    <row r="144" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B144" s="6">
         <v>142</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E144" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F144" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F144" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="G144" s="1"/>
     </row>
-    <row r="145" spans="2:7">
+    <row r="145" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B145" s="6">
         <v>143</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="E145" s="1" t="s">
         <v>5</v>
@@ -3892,15 +3898,15 @@
       <c r="F145" s="1"/>
       <c r="G145" s="1"/>
     </row>
-    <row r="146" spans="2:7">
+    <row r="146" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B146" s="6">
         <v>144</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E146" s="1" t="s">
         <v>5</v>
@@ -3908,15 +3914,15 @@
       <c r="F146" s="1"/>
       <c r="G146" s="1"/>
     </row>
-    <row r="147" spans="2:7">
+    <row r="147" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B147" s="6">
         <v>145</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E147" s="1" t="s">
         <v>5</v>
@@ -3924,15 +3930,15 @@
       <c r="F147" s="1"/>
       <c r="G147" s="1"/>
     </row>
-    <row r="148" spans="2:7">
+    <row r="148" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B148" s="6">
         <v>146</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="E148" s="1" t="s">
         <v>5</v>
@@ -3940,15 +3946,15 @@
       <c r="F148" s="1"/>
       <c r="G148" s="1"/>
     </row>
-    <row r="149" spans="2:7">
+    <row r="149" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B149" s="6">
         <v>147</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>10</v>
+        <v>292</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E149" s="1" t="s">
         <v>5</v>
@@ -3956,83 +3962,81 @@
       <c r="F149" s="1"/>
       <c r="G149" s="1"/>
     </row>
-    <row r="150" spans="2:7">
+    <row r="150" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B150" s="6">
         <v>148</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>295</v>
+        <v>10</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="E150" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F150" s="1" t="s">
-        <v>34</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F150" s="1"/>
       <c r="G150" s="1"/>
     </row>
-    <row r="151" spans="2:7">
+    <row r="151" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B151" s="6">
         <v>149</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="E151" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F151" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F151" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="G151" s="1"/>
     </row>
-    <row r="152" spans="2:7">
+    <row r="152" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B152" s="6">
         <v>150</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="E152" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F152" s="1"/>
       <c r="G152" s="1"/>
     </row>
-    <row r="153" spans="2:7">
+    <row r="153" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B153" s="6">
         <v>151</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="E153" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F153" s="1" t="s">
-        <v>34</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="F153" s="1"/>
       <c r="G153" s="1"/>
     </row>
-    <row r="154" spans="2:7">
+    <row r="154" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B154" s="6">
         <v>152</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E154" s="1" t="s">
         <v>7</v>
@@ -4042,15 +4046,15 @@
       </c>
       <c r="G154" s="1"/>
     </row>
-    <row r="155" spans="2:7">
+    <row r="155" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B155" s="6">
         <v>153</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D155" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E155" s="1" t="s">
         <v>7</v>
@@ -4060,65 +4064,67 @@
       </c>
       <c r="G155" s="1"/>
     </row>
-    <row r="156" spans="2:7">
+    <row r="156" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B156" s="6">
         <v>154</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="E156" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F156" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F156" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="G156" s="1"/>
     </row>
-    <row r="157" spans="2:7">
+    <row r="157" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B157" s="6">
         <v>155</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E157" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F157" s="1" t="s">
-        <v>34</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F157" s="1"/>
       <c r="G157" s="1"/>
     </row>
-    <row r="158" spans="2:7">
+    <row r="158" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B158" s="6">
         <v>156</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="D158" s="1" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E158" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F158" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F158" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="G158" s="1"/>
     </row>
-    <row r="159" spans="2:7">
+    <row r="159" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B159" s="6">
         <v>157</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E159" s="1" t="s">
         <v>5</v>
@@ -4126,15 +4132,23 @@
       <c r="F159" s="1"/>
       <c r="G159" s="1"/>
     </row>
-    <row r="160" spans="2:7">
-      <c r="B160" s="6"/>
-      <c r="C160" s="1"/>
-      <c r="D160" s="1"/>
-      <c r="E160" s="1"/>
+    <row r="160" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B160" s="6">
+        <v>158</v>
+      </c>
+      <c r="C160" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="D160" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="E160" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F160" s="1"/>
       <c r="G160" s="1"/>
     </row>
-    <row r="161" spans="2:7">
+    <row r="161" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B161" s="6"/>
       <c r="C161" s="1"/>
       <c r="D161" s="1"/>
@@ -4142,7 +4156,7 @@
       <c r="F161" s="1"/>
       <c r="G161" s="1"/>
     </row>
-    <row r="162" spans="2:7">
+    <row r="162" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B162" s="6"/>
       <c r="C162" s="1"/>
       <c r="D162" s="1"/>
@@ -4150,7 +4164,7 @@
       <c r="F162" s="1"/>
       <c r="G162" s="1"/>
     </row>
-    <row r="163" spans="2:7">
+    <row r="163" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B163" s="6"/>
       <c r="C163" s="1"/>
       <c r="D163" s="1"/>
@@ -4158,12 +4172,20 @@
       <c r="F163" s="1"/>
       <c r="G163" s="1"/>
     </row>
+    <row r="164" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B164" s="6"/>
+      <c r="C164" s="1"/>
+      <c r="D164" s="1"/>
+      <c r="E164" s="1"/>
+      <c r="F164" s="1"/>
+      <c r="G164" s="1"/>
+    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E159" xr:uid="{7E8CE32C-29D1-4006-9E0F-69B72A0F4378}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E160" xr:uid="{7E8CE32C-29D1-4006-9E0F-69B72A0F4378}">
       <formula1>"[Application],[Directory],[Script]"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F163" xr:uid="{A5D947FB-5606-4B36-88C5-81CC2B61C636}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F164" xr:uid="{A5D947FB-5606-4B36-88C5-81CC2B61C636}">
       <formula1>"[bat],[vbs]"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Repo Update: 2024-05-31 21:11:42
</commit_message>
<xml_diff>
--- a/Database/Run_shortcut_creator_aliases.xlsx
+++ b/Database/Run_shortcut_creator_aliases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\player-1\Documents\Windows-Git-Repos\win-t\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C7EFBA6-2E39-404E-861A-7520011F1A6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F249477D-AFCC-4E3C-9374-DB3CBA5E9E8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D65865D6-BB34-410C-8183-31ED199784FF}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="329">
   <si>
     <t>Number</t>
   </si>
@@ -1039,13 +1039,19 @@
   </si>
   <si>
     <t>mails</t>
+  </si>
+  <si>
+    <t>Obsidian</t>
+  </si>
+  <si>
+    <t>ob</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1470,24 +1476,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58A033C2-67FB-408D-B72B-8C45836FCF74}">
-  <dimension ref="B2:G164"/>
+  <dimension ref="B2:G165"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A142" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
-      <selection activeCell="D87" sqref="D87"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A73" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
+      <selection activeCell="E91" sqref="E91"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="21"/>
   <cols>
-    <col min="2" max="2" width="13.5703125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="93.42578125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="19.42578125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="25.7109375" style="5" customWidth="1"/>
-    <col min="6" max="6" width="28.28515625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="22.85546875" style="4" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" customWidth="1"/>
+    <col min="2" max="2" width="13.625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="93.375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="19.375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="25.75" style="5" customWidth="1"/>
+    <col min="6" max="6" width="28.25" style="5" customWidth="1"/>
+    <col min="7" max="7" width="22.875" style="4" customWidth="1"/>
+    <col min="8" max="8" width="15.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" s="3" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:7" s="3" customFormat="1" ht="24.95" customHeight="1">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1507,9 +1513,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:7" ht="24.95" customHeight="1">
       <c r="B3" s="6" cm="1">
-        <f t="array" ref="B3:B160">_xlfn.SEQUENCE(COUNTA(C:C)-1)</f>
+        <f t="array" ref="B3:B161">_xlfn.SEQUENCE(COUNTA(C:C)-1)</f>
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -1524,7 +1530,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:7" ht="24.95" customHeight="1">
       <c r="B4" s="6">
         <v>2</v>
       </c>
@@ -1540,7 +1546,7 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:7" ht="24.95" customHeight="1">
       <c r="B5" s="6">
         <v>3</v>
       </c>
@@ -1556,7 +1562,7 @@
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:7" ht="24.95" customHeight="1">
       <c r="B6" s="6">
         <v>4</v>
       </c>
@@ -1572,7 +1578,7 @@
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:7" ht="24.95" customHeight="1">
       <c r="B7" s="6">
         <v>5</v>
       </c>
@@ -1590,7 +1596,7 @@
       </c>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:7" ht="24.95" customHeight="1">
       <c r="B8" s="6">
         <v>6</v>
       </c>
@@ -1610,7 +1616,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:7" ht="24.95" customHeight="1">
       <c r="B9" s="6">
         <v>7</v>
       </c>
@@ -1626,7 +1632,7 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:7" ht="24.95" customHeight="1">
       <c r="B10" s="6">
         <v>8</v>
       </c>
@@ -1642,7 +1648,7 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:7" ht="24.95" customHeight="1">
       <c r="B11" s="6">
         <v>9</v>
       </c>
@@ -1658,7 +1664,7 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:7" ht="24.95" customHeight="1">
       <c r="B12" s="6">
         <v>10</v>
       </c>
@@ -1674,7 +1680,7 @@
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:7" ht="24.95" customHeight="1">
       <c r="B13" s="6">
         <v>11</v>
       </c>
@@ -1692,7 +1698,7 @@
       </c>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:7" ht="24.95" customHeight="1">
       <c r="B14" s="6">
         <v>12</v>
       </c>
@@ -1710,7 +1716,7 @@
       </c>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:7" ht="24.95" customHeight="1">
       <c r="B15" s="6">
         <v>13</v>
       </c>
@@ -1726,7 +1732,7 @@
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:7" ht="24.95" customHeight="1">
       <c r="B16" s="6">
         <v>14</v>
       </c>
@@ -1746,7 +1752,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:7" ht="24.95" customHeight="1">
       <c r="B17" s="6">
         <v>15</v>
       </c>
@@ -1766,7 +1772,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:7" ht="24.95" customHeight="1">
       <c r="B18" s="6">
         <v>16</v>
       </c>
@@ -1782,7 +1788,7 @@
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
     </row>
-    <row r="19" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:7" ht="24.95" customHeight="1">
       <c r="B19" s="6">
         <v>17</v>
       </c>
@@ -1798,7 +1804,7 @@
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
     </row>
-    <row r="20" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:7" ht="24.95" customHeight="1">
       <c r="B20" s="6">
         <v>18</v>
       </c>
@@ -1816,7 +1822,7 @@
       </c>
       <c r="G20" s="1"/>
     </row>
-    <row r="21" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:7" ht="24.95" customHeight="1">
       <c r="B21" s="6">
         <v>19</v>
       </c>
@@ -1834,7 +1840,7 @@
       </c>
       <c r="G21" s="1"/>
     </row>
-    <row r="22" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:7" ht="24.95" customHeight="1">
       <c r="B22" s="6">
         <v>20</v>
       </c>
@@ -1850,7 +1856,7 @@
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
     </row>
-    <row r="23" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:7" ht="24.95" customHeight="1">
       <c r="B23" s="6">
         <v>21</v>
       </c>
@@ -1866,7 +1872,7 @@
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
     </row>
-    <row r="24" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:7" ht="24.95" customHeight="1">
       <c r="B24" s="6">
         <v>22</v>
       </c>
@@ -1884,7 +1890,7 @@
       </c>
       <c r="G24" s="1"/>
     </row>
-    <row r="25" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:7" ht="24.95" customHeight="1">
       <c r="B25" s="6">
         <v>23</v>
       </c>
@@ -1902,7 +1908,7 @@
       </c>
       <c r="G25" s="1"/>
     </row>
-    <row r="26" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:7" ht="24.95" customHeight="1">
       <c r="B26" s="6">
         <v>24</v>
       </c>
@@ -1918,7 +1924,7 @@
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
     </row>
-    <row r="27" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:7" ht="24.95" customHeight="1">
       <c r="B27" s="6">
         <v>25</v>
       </c>
@@ -1934,7 +1940,7 @@
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
     </row>
-    <row r="28" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:7" ht="24.95" customHeight="1">
       <c r="B28" s="6">
         <v>26</v>
       </c>
@@ -1952,7 +1958,7 @@
       </c>
       <c r="G28" s="1"/>
     </row>
-    <row r="29" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:7" ht="24.95" customHeight="1">
       <c r="B29" s="6">
         <v>27</v>
       </c>
@@ -1968,7 +1974,7 @@
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
     </row>
-    <row r="30" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:7" ht="24.95" customHeight="1">
       <c r="B30" s="6">
         <v>28</v>
       </c>
@@ -1984,7 +1990,7 @@
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
     </row>
-    <row r="31" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:7" ht="24.95" customHeight="1">
       <c r="B31" s="6">
         <v>29</v>
       </c>
@@ -2000,7 +2006,7 @@
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
     </row>
-    <row r="32" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:7" ht="24.95" customHeight="1">
       <c r="B32" s="6">
         <v>30</v>
       </c>
@@ -2016,7 +2022,7 @@
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
     </row>
-    <row r="33" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:7" ht="24.95" customHeight="1">
       <c r="B33" s="6">
         <v>31</v>
       </c>
@@ -2034,7 +2040,7 @@
       </c>
       <c r="G33" s="1"/>
     </row>
-    <row r="34" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:7" ht="24.95" customHeight="1">
       <c r="B34" s="6">
         <v>32</v>
       </c>
@@ -2052,7 +2058,7 @@
       </c>
       <c r="G34" s="1"/>
     </row>
-    <row r="35" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:7" ht="24.95" customHeight="1">
       <c r="B35" s="6">
         <v>33</v>
       </c>
@@ -2070,7 +2076,7 @@
       </c>
       <c r="G35" s="1"/>
     </row>
-    <row r="36" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:7" ht="24.95" customHeight="1">
       <c r="B36" s="6">
         <v>34</v>
       </c>
@@ -2086,7 +2092,7 @@
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
     </row>
-    <row r="37" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:7" ht="24.95" customHeight="1">
       <c r="B37" s="6">
         <v>35</v>
       </c>
@@ -2102,7 +2108,7 @@
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
     </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:7">
       <c r="B38" s="6">
         <v>36</v>
       </c>
@@ -2120,7 +2126,7 @@
       </c>
       <c r="G38" s="1"/>
     </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:7">
       <c r="B39" s="6">
         <v>37</v>
       </c>
@@ -2136,7 +2142,7 @@
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
     </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:7">
       <c r="B40" s="6">
         <v>38</v>
       </c>
@@ -2154,7 +2160,7 @@
       </c>
       <c r="G40" s="1"/>
     </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:7">
       <c r="B41" s="6">
         <v>39</v>
       </c>
@@ -2170,7 +2176,7 @@
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
     </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:7">
       <c r="B42" s="6">
         <v>40</v>
       </c>
@@ -2188,7 +2194,7 @@
       </c>
       <c r="G42" s="1"/>
     </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:7">
       <c r="B43" s="6">
         <v>41</v>
       </c>
@@ -2206,7 +2212,7 @@
       </c>
       <c r="G43" s="1"/>
     </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:7">
       <c r="B44" s="6">
         <v>42</v>
       </c>
@@ -2222,7 +2228,7 @@
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
     </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:7">
       <c r="B45" s="6">
         <v>43</v>
       </c>
@@ -2240,7 +2246,7 @@
       </c>
       <c r="G45" s="1"/>
     </row>
-    <row r="46" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:7">
       <c r="B46" s="6">
         <v>44</v>
       </c>
@@ -2258,7 +2264,7 @@
       </c>
       <c r="G46" s="1"/>
     </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:7">
       <c r="B47" s="6">
         <v>45</v>
       </c>
@@ -2276,7 +2282,7 @@
       </c>
       <c r="G47" s="1"/>
     </row>
-    <row r="48" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:7">
       <c r="B48" s="6">
         <v>46</v>
       </c>
@@ -2292,7 +2298,7 @@
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
     </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:7">
       <c r="B49" s="6">
         <v>47</v>
       </c>
@@ -2308,7 +2314,7 @@
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
     </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:7">
       <c r="B50" s="6">
         <v>48</v>
       </c>
@@ -2326,7 +2332,7 @@
       </c>
       <c r="G50" s="1"/>
     </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:7">
       <c r="B51" s="6">
         <v>49</v>
       </c>
@@ -2344,7 +2350,7 @@
       </c>
       <c r="G51" s="1"/>
     </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:7">
       <c r="B52" s="6">
         <v>50</v>
       </c>
@@ -2360,7 +2366,7 @@
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
     </row>
-    <row r="53" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:7">
       <c r="B53" s="6">
         <v>51</v>
       </c>
@@ -2376,7 +2382,7 @@
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
     </row>
-    <row r="54" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:7">
       <c r="B54" s="6">
         <v>52</v>
       </c>
@@ -2392,7 +2398,7 @@
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
     </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:7">
       <c r="B55" s="6">
         <v>53</v>
       </c>
@@ -2408,7 +2414,7 @@
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
     </row>
-    <row r="56" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:7">
       <c r="B56" s="6">
         <v>54</v>
       </c>
@@ -2424,7 +2430,7 @@
       <c r="F56" s="1"/>
       <c r="G56" s="1"/>
     </row>
-    <row r="57" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:7">
       <c r="B57" s="6">
         <v>55</v>
       </c>
@@ -2440,7 +2446,7 @@
       <c r="F57" s="1"/>
       <c r="G57" s="1"/>
     </row>
-    <row r="58" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:7">
       <c r="B58" s="6">
         <v>56</v>
       </c>
@@ -2456,7 +2462,7 @@
       <c r="F58" s="1"/>
       <c r="G58" s="1"/>
     </row>
-    <row r="59" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:7">
       <c r="B59" s="6">
         <v>57</v>
       </c>
@@ -2472,7 +2478,7 @@
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
     </row>
-    <row r="60" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:7">
       <c r="B60" s="6">
         <v>58</v>
       </c>
@@ -2488,7 +2494,7 @@
       <c r="F60" s="1"/>
       <c r="G60" s="1"/>
     </row>
-    <row r="61" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:7">
       <c r="B61" s="6">
         <v>59</v>
       </c>
@@ -2506,7 +2512,7 @@
       </c>
       <c r="G61" s="1"/>
     </row>
-    <row r="62" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:7">
       <c r="B62" s="6">
         <v>60</v>
       </c>
@@ -2524,7 +2530,7 @@
       </c>
       <c r="G62" s="1"/>
     </row>
-    <row r="63" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:7">
       <c r="B63" s="6">
         <v>61</v>
       </c>
@@ -2540,7 +2546,7 @@
       <c r="F63" s="1"/>
       <c r="G63" s="1"/>
     </row>
-    <row r="64" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="64" spans="2:7">
       <c r="B64" s="6">
         <v>62</v>
       </c>
@@ -2558,7 +2564,7 @@
       </c>
       <c r="G64" s="1"/>
     </row>
-    <row r="65" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:7">
       <c r="B65" s="6">
         <v>63</v>
       </c>
@@ -2574,7 +2580,7 @@
       <c r="F65" s="1"/>
       <c r="G65" s="1"/>
     </row>
-    <row r="66" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:7">
       <c r="B66" s="6">
         <v>64</v>
       </c>
@@ -2590,7 +2596,7 @@
       <c r="F66" s="1"/>
       <c r="G66" s="1"/>
     </row>
-    <row r="67" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="67" spans="2:7">
       <c r="B67" s="6">
         <v>65</v>
       </c>
@@ -2606,7 +2612,7 @@
       <c r="F67" s="1"/>
       <c r="G67" s="1"/>
     </row>
-    <row r="68" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="68" spans="2:7">
       <c r="B68" s="6">
         <v>66</v>
       </c>
@@ -2622,7 +2628,7 @@
       <c r="F68" s="1"/>
       <c r="G68" s="1"/>
     </row>
-    <row r="69" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="69" spans="2:7">
       <c r="B69" s="6">
         <v>67</v>
       </c>
@@ -2638,7 +2644,7 @@
       <c r="F69" s="1"/>
       <c r="G69" s="1"/>
     </row>
-    <row r="70" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="70" spans="2:7">
       <c r="B70" s="6">
         <v>68</v>
       </c>
@@ -2654,7 +2660,7 @@
       <c r="F70" s="1"/>
       <c r="G70" s="1"/>
     </row>
-    <row r="71" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="71" spans="2:7">
       <c r="B71" s="6">
         <v>69</v>
       </c>
@@ -2670,7 +2676,7 @@
       <c r="F71" s="1"/>
       <c r="G71" s="1"/>
     </row>
-    <row r="72" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="72" spans="2:7">
       <c r="B72" s="6">
         <v>70</v>
       </c>
@@ -2686,7 +2692,7 @@
       <c r="F72" s="1"/>
       <c r="G72" s="1"/>
     </row>
-    <row r="73" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="73" spans="2:7">
       <c r="B73" s="6">
         <v>71</v>
       </c>
@@ -2704,7 +2710,7 @@
       </c>
       <c r="G73" s="1"/>
     </row>
-    <row r="74" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="74" spans="2:7">
       <c r="B74" s="6">
         <v>72</v>
       </c>
@@ -2720,7 +2726,7 @@
       <c r="F74" s="1"/>
       <c r="G74" s="1"/>
     </row>
-    <row r="75" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="75" spans="2:7">
       <c r="B75" s="6">
         <v>73</v>
       </c>
@@ -2738,7 +2744,7 @@
       </c>
       <c r="G75" s="1"/>
     </row>
-    <row r="76" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="76" spans="2:7">
       <c r="B76" s="6">
         <v>74</v>
       </c>
@@ -2754,7 +2760,7 @@
       <c r="F76" s="1"/>
       <c r="G76" s="1"/>
     </row>
-    <row r="77" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="77" spans="2:7">
       <c r="B77" s="6">
         <v>75</v>
       </c>
@@ -2772,7 +2778,7 @@
       </c>
       <c r="G77" s="1"/>
     </row>
-    <row r="78" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="78" spans="2:7">
       <c r="B78" s="6">
         <v>76</v>
       </c>
@@ -2788,7 +2794,7 @@
       <c r="F78" s="1"/>
       <c r="G78" s="1"/>
     </row>
-    <row r="79" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="79" spans="2:7">
       <c r="B79" s="6">
         <v>77</v>
       </c>
@@ -2804,7 +2810,7 @@
       <c r="F79" s="1"/>
       <c r="G79" s="1"/>
     </row>
-    <row r="80" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="80" spans="2:7">
       <c r="B80" s="6">
         <v>78</v>
       </c>
@@ -2820,7 +2826,7 @@
       <c r="F80" s="1"/>
       <c r="G80" s="1"/>
     </row>
-    <row r="81" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="81" spans="2:7">
       <c r="B81" s="6">
         <v>79</v>
       </c>
@@ -2836,7 +2842,7 @@
       <c r="F81" s="1"/>
       <c r="G81" s="1"/>
     </row>
-    <row r="82" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="82" spans="2:7">
       <c r="B82" s="6">
         <v>80</v>
       </c>
@@ -2852,7 +2858,7 @@
       <c r="F82" s="1"/>
       <c r="G82" s="1"/>
     </row>
-    <row r="83" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="83" spans="2:7">
       <c r="B83" s="6">
         <v>81</v>
       </c>
@@ -2868,7 +2874,7 @@
       <c r="F83" s="1"/>
       <c r="G83" s="1"/>
     </row>
-    <row r="84" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="84" spans="2:7">
       <c r="B84" s="6">
         <v>82</v>
       </c>
@@ -2886,7 +2892,7 @@
       </c>
       <c r="G84" s="1"/>
     </row>
-    <row r="85" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="85" spans="2:7">
       <c r="B85" s="6">
         <v>83</v>
       </c>
@@ -2904,7 +2910,7 @@
       </c>
       <c r="G85" s="1"/>
     </row>
-    <row r="86" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="86" spans="2:7">
       <c r="B86" s="6">
         <v>84</v>
       </c>
@@ -2922,7 +2928,7 @@
       </c>
       <c r="G86" s="1"/>
     </row>
-    <row r="87" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="87" spans="2:7">
       <c r="B87" s="6">
         <v>85</v>
       </c>
@@ -2938,7 +2944,7 @@
       <c r="F87" s="1"/>
       <c r="G87" s="1"/>
     </row>
-    <row r="88" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="88" spans="2:7">
       <c r="B88" s="6">
         <v>86</v>
       </c>
@@ -2954,7 +2960,7 @@
       <c r="F88" s="1"/>
       <c r="G88" s="1"/>
     </row>
-    <row r="89" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="89" spans="2:7">
       <c r="B89" s="6">
         <v>87</v>
       </c>
@@ -2970,7 +2976,7 @@
       <c r="F89" s="1"/>
       <c r="G89" s="1"/>
     </row>
-    <row r="90" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="90" spans="2:7">
       <c r="B90" s="6">
         <v>88</v>
       </c>
@@ -2986,15 +2992,15 @@
       <c r="F90" s="1"/>
       <c r="G90" s="1"/>
     </row>
-    <row r="91" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="91" spans="2:7">
       <c r="B91" s="6">
         <v>89</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>176</v>
+        <v>327</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>177</v>
+        <v>328</v>
       </c>
       <c r="E91" s="1" t="s">
         <v>5</v>
@@ -3002,15 +3008,15 @@
       <c r="F91" s="1"/>
       <c r="G91" s="1"/>
     </row>
-    <row r="92" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="92" spans="2:7">
       <c r="B92" s="6">
         <v>90</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E92" s="1" t="s">
         <v>5</v>
@@ -3018,15 +3024,15 @@
       <c r="F92" s="1"/>
       <c r="G92" s="1"/>
     </row>
-    <row r="93" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="93" spans="2:7">
       <c r="B93" s="6">
         <v>91</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E93" s="1" t="s">
         <v>5</v>
@@ -3034,15 +3040,15 @@
       <c r="F93" s="1"/>
       <c r="G93" s="1"/>
     </row>
-    <row r="94" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="94" spans="2:7">
       <c r="B94" s="6">
         <v>92</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E94" s="1" t="s">
         <v>5</v>
@@ -3050,15 +3056,15 @@
       <c r="F94" s="1"/>
       <c r="G94" s="1"/>
     </row>
-    <row r="95" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="95" spans="2:7">
       <c r="B95" s="6">
         <v>93</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E95" s="1" t="s">
         <v>5</v>
@@ -3066,15 +3072,15 @@
       <c r="F95" s="1"/>
       <c r="G95" s="1"/>
     </row>
-    <row r="96" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="96" spans="2:7">
       <c r="B96" s="6">
         <v>94</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E96" s="1" t="s">
         <v>5</v>
@@ -3082,15 +3088,15 @@
       <c r="F96" s="1"/>
       <c r="G96" s="1"/>
     </row>
-    <row r="97" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="97" spans="2:7">
       <c r="B97" s="6">
         <v>95</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E97" s="1" t="s">
         <v>5</v>
@@ -3098,49 +3104,49 @@
       <c r="F97" s="1"/>
       <c r="G97" s="1"/>
     </row>
-    <row r="98" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="98" spans="2:7">
       <c r="B98" s="6">
         <v>96</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F98" s="1" t="s">
-        <v>34</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F98" s="1"/>
       <c r="G98" s="1"/>
     </row>
-    <row r="99" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="99" spans="2:7">
       <c r="B99" s="6">
         <v>97</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F99" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F99" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="G99" s="1"/>
     </row>
-    <row r="100" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="100" spans="2:7">
       <c r="B100" s="6">
         <v>98</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E100" s="1" t="s">
         <v>5</v>
@@ -3148,15 +3154,15 @@
       <c r="F100" s="1"/>
       <c r="G100" s="1"/>
     </row>
-    <row r="101" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="101" spans="2:7">
       <c r="B101" s="6">
         <v>99</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E101" s="1" t="s">
         <v>5</v>
@@ -3164,15 +3170,15 @@
       <c r="F101" s="1"/>
       <c r="G101" s="1"/>
     </row>
-    <row r="102" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="102" spans="2:7">
       <c r="B102" s="6">
         <v>100</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E102" s="1" t="s">
         <v>5</v>
@@ -3180,15 +3186,15 @@
       <c r="F102" s="1"/>
       <c r="G102" s="1"/>
     </row>
-    <row r="103" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="103" spans="2:7">
       <c r="B103" s="6">
         <v>101</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E103" s="1" t="s">
         <v>5</v>
@@ -3196,15 +3202,15 @@
       <c r="F103" s="1"/>
       <c r="G103" s="1"/>
     </row>
-    <row r="104" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="104" spans="2:7">
       <c r="B104" s="6">
         <v>102</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E104" s="1" t="s">
         <v>5</v>
@@ -3212,15 +3218,15 @@
       <c r="F104" s="1"/>
       <c r="G104" s="1"/>
     </row>
-    <row r="105" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="105" spans="2:7">
       <c r="B105" s="6">
         <v>103</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E105" s="1" t="s">
         <v>5</v>
@@ -3228,15 +3234,15 @@
       <c r="F105" s="1"/>
       <c r="G105" s="1"/>
     </row>
-    <row r="106" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="106" spans="2:7">
       <c r="B106" s="6">
         <v>104</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E106" s="1" t="s">
         <v>5</v>
@@ -3244,49 +3250,49 @@
       <c r="F106" s="1"/>
       <c r="G106" s="1"/>
     </row>
-    <row r="107" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="107" spans="2:7">
       <c r="B107" s="6">
         <v>105</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F107" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F107" s="1"/>
       <c r="G107" s="1"/>
     </row>
-    <row r="108" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="108" spans="2:7">
       <c r="B108" s="6">
         <v>106</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F108" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F108" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="G108" s="1"/>
     </row>
-    <row r="109" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="109" spans="2:7">
       <c r="B109" s="6">
         <v>107</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E109" s="1" t="s">
         <v>5</v>
@@ -3294,15 +3300,15 @@
       <c r="F109" s="1"/>
       <c r="G109" s="1"/>
     </row>
-    <row r="110" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="110" spans="2:7">
       <c r="B110" s="6">
         <v>108</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="E110" s="1" t="s">
         <v>5</v>
@@ -3310,15 +3316,15 @@
       <c r="F110" s="1"/>
       <c r="G110" s="1"/>
     </row>
-    <row r="111" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="111" spans="2:7">
       <c r="B111" s="6">
         <v>109</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E111" s="1" t="s">
         <v>5</v>
@@ -3326,47 +3332,47 @@
       <c r="F111" s="1"/>
       <c r="G111" s="1"/>
     </row>
-    <row r="112" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="112" spans="2:7">
       <c r="B112" s="6">
         <v>110</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F112" s="1"/>
       <c r="G112" s="1"/>
     </row>
-    <row r="113" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="113" spans="2:7">
       <c r="B113" s="6">
         <v>111</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F113" s="1"/>
       <c r="G113" s="1"/>
     </row>
-    <row r="114" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="114" spans="2:7">
       <c r="B114" s="6">
         <v>112</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E114" s="1" t="s">
         <v>5</v>
@@ -3374,15 +3380,15 @@
       <c r="F114" s="1"/>
       <c r="G114" s="1"/>
     </row>
-    <row r="115" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="115" spans="2:7">
       <c r="B115" s="6">
         <v>113</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E115" s="1" t="s">
         <v>5</v>
@@ -3390,49 +3396,49 @@
       <c r="F115" s="1"/>
       <c r="G115" s="1"/>
     </row>
-    <row r="116" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="116" spans="2:7">
       <c r="B116" s="6">
         <v>114</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F116" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F116" s="1"/>
       <c r="G116" s="1"/>
     </row>
-    <row r="117" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="117" spans="2:7">
       <c r="B117" s="6">
         <v>115</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F117" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F117" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="G117" s="1"/>
     </row>
-    <row r="118" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="118" spans="2:7">
       <c r="B118" s="6">
         <v>116</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E118" s="1" t="s">
         <v>5</v>
@@ -3440,53 +3446,49 @@
       <c r="F118" s="1"/>
       <c r="G118" s="1"/>
     </row>
-    <row r="119" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="119" spans="2:7">
       <c r="B119" s="6">
         <v>117</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F119" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F119" s="1"/>
       <c r="G119" s="1"/>
     </row>
-    <row r="120" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="120" spans="2:7">
       <c r="B120" s="6">
         <v>118</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="E120" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F120" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G120" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="121" spans="2:7" x14ac:dyDescent="0.35">
+        <v>16</v>
+      </c>
+      <c r="G120" s="1"/>
+    </row>
+    <row r="121" spans="2:7">
       <c r="B121" s="6">
         <v>119</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E121" s="1" t="s">
         <v>7</v>
@@ -3498,15 +3500,15 @@
         <v>37</v>
       </c>
     </row>
-    <row r="122" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="122" spans="2:7">
       <c r="B122" s="6">
         <v>120</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="E122" s="1" t="s">
         <v>7</v>
@@ -3515,18 +3517,18 @@
         <v>34</v>
       </c>
       <c r="G122" s="1" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="123" spans="2:7" x14ac:dyDescent="0.35">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="123" spans="2:7">
       <c r="B123" s="6">
         <v>121</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E123" s="1" t="s">
         <v>7</v>
@@ -3534,33 +3536,37 @@
       <c r="F123" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G123" s="1"/>
-    </row>
-    <row r="124" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="G123" s="1" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="124" spans="2:7">
       <c r="B124" s="6">
         <v>122</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F124" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F124" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="G124" s="1"/>
     </row>
-    <row r="125" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="125" spans="2:7">
       <c r="B125" s="6">
         <v>123</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="E125" s="1" t="s">
         <v>5</v>
@@ -3568,67 +3574,67 @@
       <c r="F125" s="1"/>
       <c r="G125" s="1"/>
     </row>
-    <row r="126" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="126" spans="2:7">
       <c r="B126" s="6">
         <v>124</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F126" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F126" s="1"/>
       <c r="G126" s="1"/>
     </row>
-    <row r="127" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="127" spans="2:7">
       <c r="B127" s="6">
         <v>125</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E127" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F127" s="1" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="G127" s="1"/>
     </row>
-    <row r="128" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="128" spans="2:7">
       <c r="B128" s="6">
         <v>126</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="E128" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F128" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F128" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="G128" s="1"/>
     </row>
-    <row r="129" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="129" spans="2:7">
       <c r="B129" s="6">
         <v>127</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="E129" s="1" t="s">
         <v>5</v>
@@ -3636,15 +3642,15 @@
       <c r="F129" s="1"/>
       <c r="G129" s="1"/>
     </row>
-    <row r="130" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="130" spans="2:7">
       <c r="B130" s="6">
         <v>128</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E130" s="1" t="s">
         <v>5</v>
@@ -3652,15 +3658,15 @@
       <c r="F130" s="1"/>
       <c r="G130" s="1"/>
     </row>
-    <row r="131" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="131" spans="2:7">
       <c r="B131" s="6">
         <v>129</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E131" s="1" t="s">
         <v>5</v>
@@ -3668,15 +3674,15 @@
       <c r="F131" s="1"/>
       <c r="G131" s="1"/>
     </row>
-    <row r="132" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="132" spans="2:7">
       <c r="B132" s="6">
         <v>130</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E132" s="1" t="s">
         <v>5</v>
@@ -3684,65 +3690,65 @@
       <c r="F132" s="1"/>
       <c r="G132" s="1"/>
     </row>
-    <row r="133" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="133" spans="2:7">
       <c r="B133" s="6">
         <v>131</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="E133" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F133" s="1" t="s">
-        <v>34</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F133" s="1"/>
       <c r="G133" s="1"/>
     </row>
-    <row r="134" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="134" spans="2:7">
       <c r="B134" s="6">
         <v>132</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="E134" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F134" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F134" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="G134" s="1"/>
     </row>
-    <row r="135" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="135" spans="2:7">
       <c r="B135" s="6">
         <v>133</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="E135" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F135" s="1"/>
       <c r="G135" s="1"/>
     </row>
-    <row r="136" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="136" spans="2:7">
       <c r="B136" s="6">
         <v>134</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="E136" s="1" t="s">
         <v>5</v>
@@ -3750,15 +3756,15 @@
       <c r="F136" s="1"/>
       <c r="G136" s="1"/>
     </row>
-    <row r="137" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="137" spans="2:7">
       <c r="B137" s="6">
         <v>135</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E137" s="1" t="s">
         <v>5</v>
@@ -3766,15 +3772,15 @@
       <c r="F137" s="1"/>
       <c r="G137" s="1"/>
     </row>
-    <row r="138" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="138" spans="2:7">
       <c r="B138" s="6">
         <v>136</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="E138" s="1" t="s">
         <v>5</v>
@@ -3782,15 +3788,15 @@
       <c r="F138" s="1"/>
       <c r="G138" s="1"/>
     </row>
-    <row r="139" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="139" spans="2:7">
       <c r="B139" s="6">
         <v>137</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E139" s="1" t="s">
         <v>5</v>
@@ -3798,15 +3804,15 @@
       <c r="F139" s="1"/>
       <c r="G139" s="1"/>
     </row>
-    <row r="140" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="140" spans="2:7">
       <c r="B140" s="6">
         <v>138</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="E140" s="1" t="s">
         <v>5</v>
@@ -3814,49 +3820,49 @@
       <c r="F140" s="1"/>
       <c r="G140" s="1"/>
     </row>
-    <row r="141" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="141" spans="2:7">
       <c r="B141" s="6">
         <v>139</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E141" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F141" s="1" t="s">
-        <v>34</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F141" s="1"/>
       <c r="G141" s="1"/>
     </row>
-    <row r="142" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="142" spans="2:7">
       <c r="B142" s="6">
         <v>140</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="E142" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F142" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F142" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="G142" s="1"/>
     </row>
-    <row r="143" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="143" spans="2:7">
       <c r="B143" s="6">
         <v>141</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E143" s="1" t="s">
         <v>5</v>
@@ -3864,49 +3870,49 @@
       <c r="F143" s="1"/>
       <c r="G143" s="1"/>
     </row>
-    <row r="144" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="144" spans="2:7">
       <c r="B144" s="6">
         <v>142</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E144" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F144" s="1" t="s">
-        <v>34</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F144" s="1"/>
       <c r="G144" s="1"/>
     </row>
-    <row r="145" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="145" spans="2:7">
       <c r="B145" s="6">
         <v>143</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E145" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F145" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F145" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="G145" s="1"/>
     </row>
-    <row r="146" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="146" spans="2:7">
       <c r="B146" s="6">
         <v>144</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="E146" s="1" t="s">
         <v>5</v>
@@ -3914,15 +3920,15 @@
       <c r="F146" s="1"/>
       <c r="G146" s="1"/>
     </row>
-    <row r="147" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="147" spans="2:7">
       <c r="B147" s="6">
         <v>145</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E147" s="1" t="s">
         <v>5</v>
@@ -3930,15 +3936,15 @@
       <c r="F147" s="1"/>
       <c r="G147" s="1"/>
     </row>
-    <row r="148" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="148" spans="2:7">
       <c r="B148" s="6">
         <v>146</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E148" s="1" t="s">
         <v>5</v>
@@ -3946,15 +3952,15 @@
       <c r="F148" s="1"/>
       <c r="G148" s="1"/>
     </row>
-    <row r="149" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="149" spans="2:7">
       <c r="B149" s="6">
         <v>147</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="E149" s="1" t="s">
         <v>5</v>
@@ -3962,15 +3968,15 @@
       <c r="F149" s="1"/>
       <c r="G149" s="1"/>
     </row>
-    <row r="150" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="150" spans="2:7">
       <c r="B150" s="6">
         <v>148</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>10</v>
+        <v>292</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E150" s="1" t="s">
         <v>5</v>
@@ -3978,83 +3984,81 @@
       <c r="F150" s="1"/>
       <c r="G150" s="1"/>
     </row>
-    <row r="151" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="151" spans="2:7">
       <c r="B151" s="6">
         <v>149</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>295</v>
+        <v>10</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="E151" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F151" s="1" t="s">
-        <v>34</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F151" s="1"/>
       <c r="G151" s="1"/>
     </row>
-    <row r="152" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="152" spans="2:7">
       <c r="B152" s="6">
         <v>150</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="E152" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F152" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F152" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="G152" s="1"/>
     </row>
-    <row r="153" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="153" spans="2:7">
       <c r="B153" s="6">
         <v>151</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="E153" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F153" s="1"/>
       <c r="G153" s="1"/>
     </row>
-    <row r="154" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="154" spans="2:7">
       <c r="B154" s="6">
         <v>152</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="E154" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F154" s="1" t="s">
-        <v>34</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="F154" s="1"/>
       <c r="G154" s="1"/>
     </row>
-    <row r="155" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="155" spans="2:7">
       <c r="B155" s="6">
         <v>153</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D155" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E155" s="1" t="s">
         <v>7</v>
@@ -4064,15 +4068,15 @@
       </c>
       <c r="G155" s="1"/>
     </row>
-    <row r="156" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="156" spans="2:7">
       <c r="B156" s="6">
         <v>154</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E156" s="1" t="s">
         <v>7</v>
@@ -4082,65 +4086,67 @@
       </c>
       <c r="G156" s="1"/>
     </row>
-    <row r="157" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="157" spans="2:7">
       <c r="B157" s="6">
         <v>155</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="E157" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F157" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F157" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="G157" s="1"/>
     </row>
-    <row r="158" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="158" spans="2:7">
       <c r="B158" s="6">
         <v>156</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D158" s="1" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E158" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F158" s="1" t="s">
-        <v>34</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F158" s="1"/>
       <c r="G158" s="1"/>
     </row>
-    <row r="159" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="159" spans="2:7">
       <c r="B159" s="6">
         <v>157</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E159" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F159" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F159" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="G159" s="1"/>
     </row>
-    <row r="160" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="160" spans="2:7">
       <c r="B160" s="6">
         <v>158</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D160" s="1" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E160" s="1" t="s">
         <v>5</v>
@@ -4148,15 +4154,23 @@
       <c r="F160" s="1"/>
       <c r="G160" s="1"/>
     </row>
-    <row r="161" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B161" s="6"/>
-      <c r="C161" s="1"/>
-      <c r="D161" s="1"/>
-      <c r="E161" s="1"/>
+    <row r="161" spans="2:7">
+      <c r="B161" s="6">
+        <v>159</v>
+      </c>
+      <c r="C161" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="D161" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="E161" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F161" s="1"/>
       <c r="G161" s="1"/>
     </row>
-    <row r="162" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="162" spans="2:7">
       <c r="B162" s="6"/>
       <c r="C162" s="1"/>
       <c r="D162" s="1"/>
@@ -4164,7 +4178,7 @@
       <c r="F162" s="1"/>
       <c r="G162" s="1"/>
     </row>
-    <row r="163" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="163" spans="2:7">
       <c r="B163" s="6"/>
       <c r="C163" s="1"/>
       <c r="D163" s="1"/>
@@ -4172,7 +4186,7 @@
       <c r="F163" s="1"/>
       <c r="G163" s="1"/>
     </row>
-    <row r="164" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="164" spans="2:7">
       <c r="B164" s="6"/>
       <c r="C164" s="1"/>
       <c r="D164" s="1"/>
@@ -4180,12 +4194,20 @@
       <c r="F164" s="1"/>
       <c r="G164" s="1"/>
     </row>
+    <row r="165" spans="2:7">
+      <c r="B165" s="6"/>
+      <c r="C165" s="1"/>
+      <c r="D165" s="1"/>
+      <c r="E165" s="1"/>
+      <c r="F165" s="1"/>
+      <c r="G165" s="1"/>
+    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E160" xr:uid="{7E8CE32C-29D1-4006-9E0F-69B72A0F4378}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E161" xr:uid="{7E8CE32C-29D1-4006-9E0F-69B72A0F4378}">
       <formula1>"[Application],[Directory],[Script]"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F164" xr:uid="{A5D947FB-5606-4B36-88C5-81CC2B61C636}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F165" xr:uid="{A5D947FB-5606-4B36-88C5-81CC2B61C636}">
       <formula1>"[bat],[vbs]"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Repo Update: 2024-06-06 19:22:41
</commit_message>
<xml_diff>
--- a/Database/Run_shortcut_creator_aliases.xlsx
+++ b/Database/Run_shortcut_creator_aliases.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\player-1\Documents\Windows-Git-Repos\win-t\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F249477D-AFCC-4E3C-9374-DB3CBA5E9E8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41F18080-3E85-4AC1-AAFB-7C33E7F58BF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D65865D6-BB34-410C-8183-31ED199784FF}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="331">
   <si>
     <t>Number</t>
   </si>
@@ -1045,6 +1045,12 @@
   </si>
   <si>
     <t>ob</t>
+  </si>
+  <si>
+    <t>ntl</t>
+  </si>
+  <si>
+    <t>NTLite</t>
   </si>
 </sst>
 </file>
@@ -1476,10 +1482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58A033C2-67FB-408D-B72B-8C45836FCF74}">
-  <dimension ref="B2:G165"/>
+  <dimension ref="B2:G166"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A73" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
-      <selection activeCell="E91" sqref="E91"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A72" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
+      <selection activeCell="C91" sqref="C91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21"/>
@@ -1515,7 +1521,7 @@
     </row>
     <row r="3" spans="2:7" ht="24.95" customHeight="1">
       <c r="B3" s="6" cm="1">
-        <f t="array" ref="B3:B161">_xlfn.SEQUENCE(COUNTA(C:C)-1)</f>
+        <f t="array" ref="B3:B162">_xlfn.SEQUENCE(COUNTA(C:C)-1)</f>
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -2997,10 +3003,10 @@
         <v>89</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="E91" s="1" t="s">
         <v>5</v>
@@ -3013,10 +3019,10 @@
         <v>90</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>176</v>
+        <v>327</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>177</v>
+        <v>328</v>
       </c>
       <c r="E92" s="1" t="s">
         <v>5</v>
@@ -3029,10 +3035,10 @@
         <v>91</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E93" s="1" t="s">
         <v>5</v>
@@ -3045,10 +3051,10 @@
         <v>92</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E94" s="1" t="s">
         <v>5</v>
@@ -3061,10 +3067,10 @@
         <v>93</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E95" s="1" t="s">
         <v>5</v>
@@ -3077,10 +3083,10 @@
         <v>94</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E96" s="1" t="s">
         <v>5</v>
@@ -3093,10 +3099,10 @@
         <v>95</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E97" s="1" t="s">
         <v>5</v>
@@ -3109,10 +3115,10 @@
         <v>96</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E98" s="1" t="s">
         <v>5</v>
@@ -3125,17 +3131,15 @@
         <v>97</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F99" s="1" t="s">
-        <v>34</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F99" s="1"/>
       <c r="G99" s="1"/>
     </row>
     <row r="100" spans="2:7">
@@ -3143,15 +3147,17 @@
         <v>98</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F100" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F100" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="G100" s="1"/>
     </row>
     <row r="101" spans="2:7">
@@ -3159,10 +3165,10 @@
         <v>99</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E101" s="1" t="s">
         <v>5</v>
@@ -3175,10 +3181,10 @@
         <v>100</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E102" s="1" t="s">
         <v>5</v>
@@ -3191,10 +3197,10 @@
         <v>101</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E103" s="1" t="s">
         <v>5</v>
@@ -3207,10 +3213,10 @@
         <v>102</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E104" s="1" t="s">
         <v>5</v>
@@ -3223,10 +3229,10 @@
         <v>103</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E105" s="1" t="s">
         <v>5</v>
@@ -3239,10 +3245,10 @@
         <v>104</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E106" s="1" t="s">
         <v>5</v>
@@ -3255,10 +3261,10 @@
         <v>105</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E107" s="1" t="s">
         <v>5</v>
@@ -3271,17 +3277,15 @@
         <v>106</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F108" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F108" s="1"/>
       <c r="G108" s="1"/>
     </row>
     <row r="109" spans="2:7">
@@ -3289,15 +3293,17 @@
         <v>107</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F109" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F109" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="G109" s="1"/>
     </row>
     <row r="110" spans="2:7">
@@ -3305,10 +3311,10 @@
         <v>108</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E110" s="1" t="s">
         <v>5</v>
@@ -3321,10 +3327,10 @@
         <v>109</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="E111" s="1" t="s">
         <v>5</v>
@@ -3337,10 +3343,10 @@
         <v>110</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E112" s="1" t="s">
         <v>5</v>
@@ -3353,13 +3359,13 @@
         <v>111</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F113" s="1"/>
       <c r="G113" s="1"/>
@@ -3369,13 +3375,13 @@
         <v>112</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F114" s="1"/>
       <c r="G114" s="1"/>
@@ -3385,10 +3391,10 @@
         <v>113</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E115" s="1" t="s">
         <v>5</v>
@@ -3401,10 +3407,10 @@
         <v>114</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E116" s="1" t="s">
         <v>5</v>
@@ -3417,17 +3423,15 @@
         <v>115</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F117" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F117" s="1"/>
       <c r="G117" s="1"/>
     </row>
     <row r="118" spans="2:7">
@@ -3435,15 +3439,17 @@
         <v>116</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F118" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F118" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="G118" s="1"/>
     </row>
     <row r="119" spans="2:7">
@@ -3451,10 +3457,10 @@
         <v>117</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E119" s="1" t="s">
         <v>5</v>
@@ -3467,17 +3473,15 @@
         <v>118</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F120" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F120" s="1"/>
       <c r="G120" s="1"/>
     </row>
     <row r="121" spans="2:7">
@@ -3485,30 +3489,28 @@
         <v>119</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="E121" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F121" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G121" s="1" t="s">
-        <v>37</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="G121" s="1"/>
     </row>
     <row r="122" spans="2:7">
       <c r="B122" s="6">
         <v>120</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E122" s="1" t="s">
         <v>7</v>
@@ -3525,10 +3527,10 @@
         <v>121</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="E123" s="1" t="s">
         <v>7</v>
@@ -3537,7 +3539,7 @@
         <v>34</v>
       </c>
       <c r="G123" s="1" t="s">
-        <v>315</v>
+        <v>37</v>
       </c>
     </row>
     <row r="124" spans="2:7">
@@ -3545,10 +3547,10 @@
         <v>122</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E124" s="1" t="s">
         <v>7</v>
@@ -3556,22 +3558,26 @@
       <c r="F124" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G124" s="1"/>
+      <c r="G124" s="1" t="s">
+        <v>315</v>
+      </c>
     </row>
     <row r="125" spans="2:7">
       <c r="B125" s="6">
         <v>123</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F125" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F125" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="G125" s="1"/>
     </row>
     <row r="126" spans="2:7">
@@ -3579,10 +3585,10 @@
         <v>124</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="E126" s="1" t="s">
         <v>5</v>
@@ -3595,17 +3601,15 @@
         <v>125</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F127" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F127" s="1"/>
       <c r="G127" s="1"/>
     </row>
     <row r="128" spans="2:7">
@@ -3613,16 +3617,16 @@
         <v>126</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E128" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F128" s="1" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="G128" s="1"/>
     </row>
@@ -3631,15 +3635,17 @@
         <v>127</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="E129" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F129" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F129" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="G129" s="1"/>
     </row>
     <row r="130" spans="2:7">
@@ -3647,10 +3653,10 @@
         <v>128</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="E130" s="1" t="s">
         <v>5</v>
@@ -3663,10 +3669,10 @@
         <v>129</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E131" s="1" t="s">
         <v>5</v>
@@ -3679,10 +3685,10 @@
         <v>130</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E132" s="1" t="s">
         <v>5</v>
@@ -3695,10 +3701,10 @@
         <v>131</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E133" s="1" t="s">
         <v>5</v>
@@ -3711,17 +3717,15 @@
         <v>132</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="E134" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F134" s="1" t="s">
-        <v>34</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F134" s="1"/>
       <c r="G134" s="1"/>
     </row>
     <row r="135" spans="2:7">
@@ -3729,15 +3733,17 @@
         <v>133</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="E135" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F135" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F135" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="G135" s="1"/>
     </row>
     <row r="136" spans="2:7">
@@ -3745,13 +3751,13 @@
         <v>134</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="E136" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F136" s="1"/>
       <c r="G136" s="1"/>
@@ -3761,10 +3767,10 @@
         <v>135</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="E137" s="1" t="s">
         <v>5</v>
@@ -3777,10 +3783,10 @@
         <v>136</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E138" s="1" t="s">
         <v>5</v>
@@ -3793,10 +3799,10 @@
         <v>137</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="E139" s="1" t="s">
         <v>5</v>
@@ -3809,10 +3815,10 @@
         <v>138</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E140" s="1" t="s">
         <v>5</v>
@@ -3825,10 +3831,10 @@
         <v>139</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="E141" s="1" t="s">
         <v>5</v>
@@ -3841,17 +3847,15 @@
         <v>140</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E142" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F142" s="1" t="s">
-        <v>34</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F142" s="1"/>
       <c r="G142" s="1"/>
     </row>
     <row r="143" spans="2:7">
@@ -3859,15 +3863,17 @@
         <v>141</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="E143" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F143" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F143" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="G143" s="1"/>
     </row>
     <row r="144" spans="2:7">
@@ -3875,10 +3881,10 @@
         <v>142</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E144" s="1" t="s">
         <v>5</v>
@@ -3891,17 +3897,15 @@
         <v>143</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E145" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F145" s="1" t="s">
-        <v>34</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F145" s="1"/>
       <c r="G145" s="1"/>
     </row>
     <row r="146" spans="2:7">
@@ -3909,15 +3913,17 @@
         <v>144</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E146" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F146" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F146" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="G146" s="1"/>
     </row>
     <row r="147" spans="2:7">
@@ -3925,10 +3931,10 @@
         <v>145</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="E147" s="1" t="s">
         <v>5</v>
@@ -3941,10 +3947,10 @@
         <v>146</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E148" s="1" t="s">
         <v>5</v>
@@ -3957,10 +3963,10 @@
         <v>147</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E149" s="1" t="s">
         <v>5</v>
@@ -3973,10 +3979,10 @@
         <v>148</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="E150" s="1" t="s">
         <v>5</v>
@@ -3989,10 +3995,10 @@
         <v>149</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>10</v>
+        <v>292</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E151" s="1" t="s">
         <v>5</v>
@@ -4005,17 +4011,15 @@
         <v>150</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>295</v>
+        <v>10</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="E152" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F152" s="1" t="s">
-        <v>34</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F152" s="1"/>
       <c r="G152" s="1"/>
     </row>
     <row r="153" spans="2:7">
@@ -4023,15 +4027,17 @@
         <v>151</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="E153" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F153" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F153" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="G153" s="1"/>
     </row>
     <row r="154" spans="2:7">
@@ -4039,13 +4045,13 @@
         <v>152</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="E154" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F154" s="1"/>
       <c r="G154" s="1"/>
@@ -4055,17 +4061,15 @@
         <v>153</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D155" s="1" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="E155" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F155" s="1" t="s">
-        <v>34</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="F155" s="1"/>
       <c r="G155" s="1"/>
     </row>
     <row r="156" spans="2:7">
@@ -4073,10 +4077,10 @@
         <v>154</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E156" s="1" t="s">
         <v>7</v>
@@ -4091,10 +4095,10 @@
         <v>155</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E157" s="1" t="s">
         <v>7</v>
@@ -4109,15 +4113,17 @@
         <v>156</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="D158" s="1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="E158" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F158" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F158" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="G158" s="1"/>
     </row>
     <row r="159" spans="2:7">
@@ -4125,17 +4131,15 @@
         <v>157</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E159" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F159" s="1" t="s">
-        <v>34</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F159" s="1"/>
       <c r="G159" s="1"/>
     </row>
     <row r="160" spans="2:7">
@@ -4143,15 +4147,17 @@
         <v>158</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="D160" s="1" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E160" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F160" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F160" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="G160" s="1"/>
     </row>
     <row r="161" spans="2:7">
@@ -4159,10 +4165,10 @@
         <v>159</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D161" s="1" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E161" s="1" t="s">
         <v>5</v>
@@ -4171,10 +4177,18 @@
       <c r="G161" s="1"/>
     </row>
     <row r="162" spans="2:7">
-      <c r="B162" s="6"/>
-      <c r="C162" s="1"/>
-      <c r="D162" s="1"/>
-      <c r="E162" s="1"/>
+      <c r="B162" s="6">
+        <v>160</v>
+      </c>
+      <c r="C162" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="D162" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="E162" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F162" s="1"/>
       <c r="G162" s="1"/>
     </row>
@@ -4202,12 +4216,20 @@
       <c r="F165" s="1"/>
       <c r="G165" s="1"/>
     </row>
+    <row r="166" spans="2:7">
+      <c r="B166" s="6"/>
+      <c r="C166" s="1"/>
+      <c r="D166" s="1"/>
+      <c r="E166" s="1"/>
+      <c r="F166" s="1"/>
+      <c r="G166" s="1"/>
+    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E161" xr:uid="{7E8CE32C-29D1-4006-9E0F-69B72A0F4378}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E162" xr:uid="{7E8CE32C-29D1-4006-9E0F-69B72A0F4378}">
       <formula1>"[Application],[Directory],[Script]"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F165" xr:uid="{A5D947FB-5606-4B36-88C5-81CC2B61C636}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F166" xr:uid="{A5D947FB-5606-4B36-88C5-81CC2B61C636}">
       <formula1>"[bat],[vbs]"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Repo Update: 2024-06-16 13:18:33
</commit_message>
<xml_diff>
--- a/Database/Run_shortcut_creator_aliases.xlsx
+++ b/Database/Run_shortcut_creator_aliases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\player-1\Documents\Windows-Git-Repos\win-t\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41F18080-3E85-4AC1-AAFB-7C33E7F58BF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA9E1451-369B-4234-9AA0-3D2597CF6E6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D65865D6-BB34-410C-8183-31ED199784FF}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="336">
   <si>
     <t>Number</t>
   </si>
@@ -114,9 +114,6 @@
     <t>Excel</t>
   </si>
   <si>
-    <t>Aegis (WSL)</t>
-  </si>
-  <si>
     <t>aegis</t>
   </si>
   <si>
@@ -1051,6 +1048,24 @@
   </si>
   <si>
     <t>NTLite</t>
+  </si>
+  <si>
+    <t>Aegis</t>
+  </si>
+  <si>
+    <t>ae</t>
+  </si>
+  <si>
+    <t>Libreoffice</t>
+  </si>
+  <si>
+    <t>lo</t>
+  </si>
+  <si>
+    <t>Next Sunday Date</t>
+  </si>
+  <si>
+    <t>nsd</t>
   </si>
 </sst>
 </file>
@@ -1482,10 +1497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58A033C2-67FB-408D-B72B-8C45836FCF74}">
-  <dimension ref="B2:G166"/>
+  <dimension ref="B2:G168"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A72" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
-      <selection activeCell="C91" sqref="C91"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A69" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
+      <selection activeCell="H90" sqref="H90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21"/>
@@ -1521,7 +1536,7 @@
     </row>
     <row r="3" spans="2:7" ht="24.95" customHeight="1">
       <c r="B3" s="6" cm="1">
-        <f t="array" ref="B3:B162">_xlfn.SEQUENCE(COUNTA(C:C)-1)</f>
+        <f t="array" ref="B3:B164">_xlfn.SEQUENCE(COUNTA(C:C)-1)</f>
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -1557,10 +1572,10 @@
         <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>6</v>
@@ -1589,16 +1604,16 @@
         <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>14</v>
+        <v>330</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>15</v>
+        <v>331</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="G7" s="1"/>
     </row>
@@ -1607,30 +1622,28 @@
         <v>6</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>17</v>
-      </c>
+      <c r="G8" s="1"/>
     </row>
     <row r="9" spans="2:7" ht="24.95" customHeight="1">
       <c r="B9" s="6">
         <v>7</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>5</v>
@@ -1643,10 +1656,10 @@
         <v>8</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>5</v>
@@ -1659,10 +1672,10 @@
         <v>9</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>5</v>
@@ -1675,10 +1688,10 @@
         <v>10</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>5</v>
@@ -1691,10 +1704,10 @@
         <v>11</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>7</v>
@@ -1709,10 +1722,10 @@
         <v>12</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>7</v>
@@ -1727,10 +1740,10 @@
         <v>13</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>5</v>
@@ -1743,16 +1756,16 @@
         <v>14</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="E16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>17</v>
@@ -1763,19 +1776,19 @@
         <v>15</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="E17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G17" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="18" spans="2:7" ht="24.95" customHeight="1">
@@ -1783,10 +1796,10 @@
         <v>16</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>5</v>
@@ -1799,10 +1812,10 @@
         <v>17</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>41</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>5</v>
@@ -1815,16 +1828,16 @@
         <v>18</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G20" s="1"/>
     </row>
@@ -1833,16 +1846,16 @@
         <v>19</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G21" s="1"/>
     </row>
@@ -1851,10 +1864,10 @@
         <v>20</v>
       </c>
       <c r="C22" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>47</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>5</v>
@@ -1867,10 +1880,10 @@
         <v>21</v>
       </c>
       <c r="C23" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>49</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>6</v>
@@ -1883,10 +1896,10 @@
         <v>22</v>
       </c>
       <c r="C24" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>7</v>
@@ -1901,16 +1914,16 @@
         <v>23</v>
       </c>
       <c r="C25" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D25" s="1" t="s">
-        <v>53</v>
-      </c>
       <c r="E25" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G25" s="1"/>
     </row>
@@ -1919,10 +1932,10 @@
         <v>24</v>
       </c>
       <c r="C26" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>5</v>
@@ -1935,10 +1948,10 @@
         <v>25</v>
       </c>
       <c r="C27" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>319</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>320</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>6</v>
@@ -1951,10 +1964,10 @@
         <v>26</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>7</v>
@@ -1969,10 +1982,10 @@
         <v>27</v>
       </c>
       <c r="C29" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D29" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>5</v>
@@ -1985,10 +1998,10 @@
         <v>28</v>
       </c>
       <c r="C30" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D30" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>60</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>6</v>
@@ -2001,10 +2014,10 @@
         <v>29</v>
       </c>
       <c r="C31" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>321</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>322</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>5</v>
@@ -2017,10 +2030,10 @@
         <v>30</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>5</v>
@@ -2033,10 +2046,10 @@
         <v>31</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>5</v>
@@ -2051,10 +2064,10 @@
         <v>32</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>5</v>
@@ -2069,10 +2082,10 @@
         <v>33</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>5</v>
@@ -2087,10 +2100,10 @@
         <v>34</v>
       </c>
       <c r="C36" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D36" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>6</v>
@@ -2103,10 +2116,10 @@
         <v>35</v>
       </c>
       <c r="C37" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D37" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>72</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>5</v>
@@ -2119,16 +2132,16 @@
         <v>36</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G38" s="1"/>
     </row>
@@ -2137,10 +2150,10 @@
         <v>37</v>
       </c>
       <c r="C39" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D39" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>75</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>5</v>
@@ -2153,16 +2166,16 @@
         <v>38</v>
       </c>
       <c r="C40" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D40" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D40" s="1" t="s">
-        <v>78</v>
-      </c>
       <c r="E40" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G40" s="1"/>
     </row>
@@ -2171,10 +2184,10 @@
         <v>39</v>
       </c>
       <c r="C41" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D41" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>80</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>5</v>
@@ -2187,10 +2200,10 @@
         <v>40</v>
       </c>
       <c r="C42" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D42" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>82</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>7</v>
@@ -2205,16 +2218,16 @@
         <v>41</v>
       </c>
       <c r="C43" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D43" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D43" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="E43" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G43" s="1"/>
     </row>
@@ -2223,10 +2236,10 @@
         <v>42</v>
       </c>
       <c r="C44" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D44" s="1" t="s">
         <v>317</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>318</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>6</v>
@@ -2239,16 +2252,16 @@
         <v>43</v>
       </c>
       <c r="C45" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D45" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D45" s="1" t="s">
-        <v>86</v>
-      </c>
       <c r="E45" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G45" s="1"/>
     </row>
@@ -2257,10 +2270,10 @@
         <v>44</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>7</v>
@@ -2275,16 +2288,16 @@
         <v>45</v>
       </c>
       <c r="C47" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D47" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D47" s="1" t="s">
-        <v>90</v>
-      </c>
       <c r="E47" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G47" s="1"/>
     </row>
@@ -2293,10 +2306,10 @@
         <v>46</v>
       </c>
       <c r="C48" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D48" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>92</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>5</v>
@@ -2309,10 +2322,10 @@
         <v>47</v>
       </c>
       <c r="C49" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D49" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>94</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>5</v>
@@ -2325,10 +2338,10 @@
         <v>48</v>
       </c>
       <c r="C50" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D50" s="1" t="s">
         <v>95</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>96</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>7</v>
@@ -2343,10 +2356,10 @@
         <v>49</v>
       </c>
       <c r="C51" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D51" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>98</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>7</v>
@@ -2361,10 +2374,10 @@
         <v>50</v>
       </c>
       <c r="C52" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D52" s="1" t="s">
         <v>99</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>100</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>5</v>
@@ -2377,10 +2390,10 @@
         <v>51</v>
       </c>
       <c r="C53" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D53" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>102</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>5</v>
@@ -2393,10 +2406,10 @@
         <v>52</v>
       </c>
       <c r="C54" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D54" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>104</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>5</v>
@@ -2409,10 +2422,10 @@
         <v>53</v>
       </c>
       <c r="C55" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D55" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>106</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>5</v>
@@ -2425,10 +2438,10 @@
         <v>54</v>
       </c>
       <c r="C56" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D56" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>108</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>5</v>
@@ -2441,10 +2454,10 @@
         <v>55</v>
       </c>
       <c r="C57" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D57" s="1" t="s">
         <v>109</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>110</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>5</v>
@@ -2457,10 +2470,10 @@
         <v>56</v>
       </c>
       <c r="C58" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D58" s="1" t="s">
         <v>111</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>112</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>6</v>
@@ -2473,10 +2486,10 @@
         <v>57</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>5</v>
@@ -2489,10 +2502,10 @@
         <v>58</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>5</v>
@@ -2505,10 +2518,10 @@
         <v>59</v>
       </c>
       <c r="C61" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D61" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>119</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>7</v>
@@ -2523,10 +2536,10 @@
         <v>60</v>
       </c>
       <c r="C62" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D62" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>7</v>
@@ -2541,10 +2554,10 @@
         <v>61</v>
       </c>
       <c r="C63" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D63" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>123</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>5</v>
@@ -2557,16 +2570,16 @@
         <v>62</v>
       </c>
       <c r="C64" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D64" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="D64" s="1" t="s">
-        <v>125</v>
-      </c>
       <c r="E64" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G64" s="1"/>
     </row>
@@ -2575,10 +2588,10 @@
         <v>63</v>
       </c>
       <c r="C65" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D65" s="1" t="s">
         <v>126</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>127</v>
       </c>
       <c r="E65" s="1" t="s">
         <v>5</v>
@@ -2591,10 +2604,10 @@
         <v>64</v>
       </c>
       <c r="C66" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D66" s="1" t="s">
         <v>128</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>129</v>
       </c>
       <c r="E66" s="1" t="s">
         <v>5</v>
@@ -2607,10 +2620,10 @@
         <v>65</v>
       </c>
       <c r="C67" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D67" s="1" t="s">
         <v>130</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>131</v>
       </c>
       <c r="E67" s="1" t="s">
         <v>5</v>
@@ -2623,10 +2636,10 @@
         <v>66</v>
       </c>
       <c r="C68" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D68" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>133</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>5</v>
@@ -2639,10 +2652,10 @@
         <v>67</v>
       </c>
       <c r="C69" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D69" s="1" t="s">
         <v>134</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>135</v>
       </c>
       <c r="E69" s="1" t="s">
         <v>5</v>
@@ -2655,10 +2668,10 @@
         <v>68</v>
       </c>
       <c r="C70" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D70" s="1" t="s">
         <v>136</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>137</v>
       </c>
       <c r="E70" s="1" t="s">
         <v>5</v>
@@ -2671,10 +2684,10 @@
         <v>69</v>
       </c>
       <c r="C71" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D71" s="1" t="s">
         <v>138</v>
-      </c>
-      <c r="D71" s="1" t="s">
-        <v>139</v>
       </c>
       <c r="E71" s="1" t="s">
         <v>5</v>
@@ -2687,10 +2700,10 @@
         <v>70</v>
       </c>
       <c r="C72" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D72" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="D72" s="1" t="s">
-        <v>141</v>
       </c>
       <c r="E72" s="1" t="s">
         <v>5</v>
@@ -2703,10 +2716,10 @@
         <v>71</v>
       </c>
       <c r="C73" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D73" s="1" t="s">
         <v>142</v>
-      </c>
-      <c r="D73" s="1" t="s">
-        <v>143</v>
       </c>
       <c r="E73" s="1" t="s">
         <v>7</v>
@@ -2721,10 +2734,10 @@
         <v>72</v>
       </c>
       <c r="C74" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D74" s="1" t="s">
         <v>144</v>
-      </c>
-      <c r="D74" s="1" t="s">
-        <v>145</v>
       </c>
       <c r="E74" s="1" t="s">
         <v>5</v>
@@ -2737,10 +2750,10 @@
         <v>73</v>
       </c>
       <c r="C75" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D75" s="1" t="s">
         <v>146</v>
-      </c>
-      <c r="D75" s="1" t="s">
-        <v>147</v>
       </c>
       <c r="E75" s="1" t="s">
         <v>7</v>
@@ -2755,10 +2768,10 @@
         <v>74</v>
       </c>
       <c r="C76" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D76" s="1" t="s">
         <v>148</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>149</v>
       </c>
       <c r="E76" s="1" t="s">
         <v>5</v>
@@ -2771,17 +2784,15 @@
         <v>75</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>150</v>
+        <v>332</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>151</v>
+        <v>333</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F77" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F77" s="1"/>
       <c r="G77" s="1"/>
     </row>
     <row r="78" spans="2:7">
@@ -2789,15 +2800,17 @@
         <v>76</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F78" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="G78" s="1"/>
     </row>
     <row r="79" spans="2:7">
@@ -2805,10 +2818,10 @@
         <v>77</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>325</v>
+        <v>151</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>326</v>
+        <v>152</v>
       </c>
       <c r="E79" s="1" t="s">
         <v>5</v>
@@ -2821,10 +2834,10 @@
         <v>78</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>154</v>
+        <v>324</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>155</v>
+        <v>325</v>
       </c>
       <c r="E80" s="1" t="s">
         <v>5</v>
@@ -2837,10 +2850,10 @@
         <v>79</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E81" s="1" t="s">
         <v>5</v>
@@ -2853,10 +2866,10 @@
         <v>80</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E82" s="1" t="s">
         <v>5</v>
@@ -2869,10 +2882,10 @@
         <v>81</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="E83" s="1" t="s">
         <v>5</v>
@@ -2885,17 +2898,15 @@
         <v>82</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F84" s="1" t="s">
-        <v>34</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F84" s="1"/>
       <c r="G84" s="1"/>
     </row>
     <row r="85" spans="2:7">
@@ -2903,16 +2914,16 @@
         <v>83</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E85" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G85" s="1"/>
     </row>
@@ -2921,16 +2932,16 @@
         <v>84</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E86" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="G86" s="1"/>
     </row>
@@ -2939,15 +2950,17 @@
         <v>85</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F87" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F87" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="G87" s="1"/>
     </row>
     <row r="88" spans="2:7">
@@ -2955,13 +2968,13 @@
         <v>86</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F88" s="1"/>
       <c r="G88" s="1"/>
@@ -2971,13 +2984,13 @@
         <v>87</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F89" s="1"/>
       <c r="G89" s="1"/>
@@ -2987,10 +3000,10 @@
         <v>88</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E90" s="1" t="s">
         <v>5</v>
@@ -3003,15 +3016,17 @@
         <v>89</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>330</v>
+        <v>334</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>329</v>
+        <v>335</v>
       </c>
       <c r="E91" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F91" s="1"/>
+      <c r="F91" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="G91" s="1"/>
     </row>
     <row r="92" spans="2:7">
@@ -3019,10 +3034,10 @@
         <v>90</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>327</v>
+        <v>173</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>328</v>
+        <v>174</v>
       </c>
       <c r="E92" s="1" t="s">
         <v>5</v>
@@ -3035,10 +3050,10 @@
         <v>91</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>176</v>
+        <v>329</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>177</v>
+        <v>328</v>
       </c>
       <c r="E93" s="1" t="s">
         <v>5</v>
@@ -3051,10 +3066,10 @@
         <v>92</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>178</v>
+        <v>326</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>179</v>
+        <v>327</v>
       </c>
       <c r="E94" s="1" t="s">
         <v>5</v>
@@ -3067,10 +3082,10 @@
         <v>93</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="E95" s="1" t="s">
         <v>5</v>
@@ -3083,10 +3098,10 @@
         <v>94</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="E96" s="1" t="s">
         <v>5</v>
@@ -3099,10 +3114,10 @@
         <v>95</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="E97" s="1" t="s">
         <v>5</v>
@@ -3115,10 +3130,10 @@
         <v>96</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="E98" s="1" t="s">
         <v>5</v>
@@ -3131,10 +3146,10 @@
         <v>97</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="E99" s="1" t="s">
         <v>5</v>
@@ -3147,17 +3162,15 @@
         <v>98</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F100" s="1" t="s">
-        <v>34</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F100" s="1"/>
       <c r="G100" s="1"/>
     </row>
     <row r="101" spans="2:7">
@@ -3165,10 +3178,10 @@
         <v>99</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="E101" s="1" t="s">
         <v>5</v>
@@ -3181,15 +3194,17 @@
         <v>100</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F102" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F102" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="G102" s="1"/>
     </row>
     <row r="103" spans="2:7">
@@ -3197,10 +3212,10 @@
         <v>101</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="E103" s="1" t="s">
         <v>5</v>
@@ -3213,10 +3228,10 @@
         <v>102</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="E104" s="1" t="s">
         <v>5</v>
@@ -3229,10 +3244,10 @@
         <v>103</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="E105" s="1" t="s">
         <v>5</v>
@@ -3245,10 +3260,10 @@
         <v>104</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="E106" s="1" t="s">
         <v>5</v>
@@ -3261,10 +3276,10 @@
         <v>105</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="E107" s="1" t="s">
         <v>5</v>
@@ -3277,10 +3292,10 @@
         <v>106</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="E108" s="1" t="s">
         <v>5</v>
@@ -3293,17 +3308,15 @@
         <v>107</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F109" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F109" s="1"/>
       <c r="G109" s="1"/>
     </row>
     <row r="110" spans="2:7">
@@ -3311,10 +3324,10 @@
         <v>108</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="E110" s="1" t="s">
         <v>5</v>
@@ -3327,15 +3340,17 @@
         <v>109</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F111" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F111" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="G111" s="1"/>
     </row>
     <row r="112" spans="2:7">
@@ -3343,10 +3358,10 @@
         <v>110</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="E112" s="1" t="s">
         <v>5</v>
@@ -3359,10 +3374,10 @@
         <v>111</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E113" s="1" t="s">
         <v>5</v>
@@ -3375,13 +3390,13 @@
         <v>112</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F114" s="1"/>
       <c r="G114" s="1"/>
@@ -3391,10 +3406,10 @@
         <v>113</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="E115" s="1" t="s">
         <v>5</v>
@@ -3407,13 +3422,13 @@
         <v>114</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F116" s="1"/>
       <c r="G116" s="1"/>
@@ -3423,10 +3438,10 @@
         <v>115</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="E117" s="1" t="s">
         <v>5</v>
@@ -3439,17 +3454,15 @@
         <v>116</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F118" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F118" s="1"/>
       <c r="G118" s="1"/>
     </row>
     <row r="119" spans="2:7">
@@ -3457,10 +3470,10 @@
         <v>117</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="E119" s="1" t="s">
         <v>5</v>
@@ -3473,15 +3486,17 @@
         <v>118</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F120" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F120" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="G120" s="1"/>
     </row>
     <row r="121" spans="2:7">
@@ -3489,17 +3504,15 @@
         <v>119</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F121" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F121" s="1"/>
       <c r="G121" s="1"/>
     </row>
     <row r="122" spans="2:7">
@@ -3507,59 +3520,53 @@
         <v>120</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F122" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G122" s="1" t="s">
-        <v>37</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F122" s="1"/>
+      <c r="G122" s="1"/>
     </row>
     <row r="123" spans="2:7">
       <c r="B123" s="6">
         <v>121</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="E123" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F123" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G123" s="1" t="s">
-        <v>37</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="G123" s="1"/>
     </row>
     <row r="124" spans="2:7">
       <c r="B124" s="6">
         <v>122</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="E124" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F124" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G124" s="1" t="s">
-        <v>315</v>
+        <v>36</v>
       </c>
     </row>
     <row r="125" spans="2:7">
@@ -3567,49 +3574,57 @@
         <v>123</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="E125" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F125" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G125" s="1"/>
+        <v>33</v>
+      </c>
+      <c r="G125" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="126" spans="2:7">
       <c r="B126" s="6">
         <v>124</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F126" s="1"/>
-      <c r="G126" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F126" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G126" s="1" t="s">
+        <v>314</v>
+      </c>
     </row>
     <row r="127" spans="2:7">
       <c r="B127" s="6">
         <v>125</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F127" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F127" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="G127" s="1"/>
     </row>
     <row r="128" spans="2:7">
@@ -3617,17 +3632,15 @@
         <v>126</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="E128" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F128" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F128" s="1"/>
       <c r="G128" s="1"/>
     </row>
     <row r="129" spans="2:7">
@@ -3635,17 +3648,15 @@
         <v>127</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="E129" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F129" s="1" t="s">
-        <v>34</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F129" s="1"/>
       <c r="G129" s="1"/>
     </row>
     <row r="130" spans="2:7">
@@ -3653,15 +3664,17 @@
         <v>128</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="E130" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F130" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F130" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="G130" s="1"/>
     </row>
     <row r="131" spans="2:7">
@@ -3669,15 +3682,17 @@
         <v>129</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="E131" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F131" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F131" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="G131" s="1"/>
     </row>
     <row r="132" spans="2:7">
@@ -3685,10 +3700,10 @@
         <v>130</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="E132" s="1" t="s">
         <v>5</v>
@@ -3701,10 +3716,10 @@
         <v>131</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="E133" s="1" t="s">
         <v>5</v>
@@ -3717,10 +3732,10 @@
         <v>132</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="E134" s="1" t="s">
         <v>5</v>
@@ -3733,17 +3748,15 @@
         <v>133</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="E135" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F135" s="1" t="s">
-        <v>34</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F135" s="1"/>
       <c r="G135" s="1"/>
     </row>
     <row r="136" spans="2:7">
@@ -3751,13 +3764,13 @@
         <v>134</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="E136" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F136" s="1"/>
       <c r="G136" s="1"/>
@@ -3767,15 +3780,17 @@
         <v>135</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="E137" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F137" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F137" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="G137" s="1"/>
     </row>
     <row r="138" spans="2:7">
@@ -3783,13 +3798,13 @@
         <v>136</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="E138" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F138" s="1"/>
       <c r="G138" s="1"/>
@@ -3799,10 +3814,10 @@
         <v>137</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="E139" s="1" t="s">
         <v>5</v>
@@ -3815,10 +3830,10 @@
         <v>138</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="E140" s="1" t="s">
         <v>5</v>
@@ -3831,10 +3846,10 @@
         <v>139</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="E141" s="1" t="s">
         <v>5</v>
@@ -3847,10 +3862,10 @@
         <v>140</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="E142" s="1" t="s">
         <v>5</v>
@@ -3863,17 +3878,15 @@
         <v>141</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="E143" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F143" s="1" t="s">
-        <v>34</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F143" s="1"/>
       <c r="G143" s="1"/>
     </row>
     <row r="144" spans="2:7">
@@ -3881,10 +3894,10 @@
         <v>142</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="E144" s="1" t="s">
         <v>5</v>
@@ -3897,15 +3910,17 @@
         <v>143</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="E145" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F145" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F145" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="G145" s="1"/>
     </row>
     <row r="146" spans="2:7">
@@ -3913,17 +3928,15 @@
         <v>144</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="E146" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F146" s="1" t="s">
-        <v>34</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F146" s="1"/>
       <c r="G146" s="1"/>
     </row>
     <row r="147" spans="2:7">
@@ -3931,10 +3944,10 @@
         <v>145</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="E147" s="1" t="s">
         <v>5</v>
@@ -3947,15 +3960,17 @@
         <v>146</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="E148" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F148" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F148" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="G148" s="1"/>
     </row>
     <row r="149" spans="2:7">
@@ -3963,10 +3978,10 @@
         <v>147</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="E149" s="1" t="s">
         <v>5</v>
@@ -3979,10 +3994,10 @@
         <v>148</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="E150" s="1" t="s">
         <v>5</v>
@@ -3995,10 +4010,10 @@
         <v>149</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="E151" s="1" t="s">
         <v>5</v>
@@ -4011,10 +4026,10 @@
         <v>150</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>10</v>
+        <v>289</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="E152" s="1" t="s">
         <v>5</v>
@@ -4027,17 +4042,15 @@
         <v>151</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="E153" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F153" s="1" t="s">
-        <v>34</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F153" s="1"/>
       <c r="G153" s="1"/>
     </row>
     <row r="154" spans="2:7">
@@ -4045,10 +4058,10 @@
         <v>152</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>297</v>
+        <v>10</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="E154" s="1" t="s">
         <v>5</v>
@@ -4061,15 +4074,17 @@
         <v>153</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="D155" s="1" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="E155" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F155" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F155" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="G155" s="1"/>
     </row>
     <row r="156" spans="2:7">
@@ -4077,17 +4092,15 @@
         <v>154</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="E156" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F156" s="1" t="s">
-        <v>34</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F156" s="1"/>
       <c r="G156" s="1"/>
     </row>
     <row r="157" spans="2:7">
@@ -4095,17 +4108,15 @@
         <v>155</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="E157" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F157" s="1" t="s">
-        <v>34</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="F157" s="1"/>
       <c r="G157" s="1"/>
     </row>
     <row r="158" spans="2:7">
@@ -4113,16 +4124,16 @@
         <v>156</v>
       </c>
       <c r="C158" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="D158" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="D158" s="1" t="s">
-        <v>306</v>
-      </c>
       <c r="E158" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F158" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G158" s="1"/>
     </row>
@@ -4131,15 +4142,17 @@
         <v>157</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="E159" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F159" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F159" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="G159" s="1"/>
     </row>
     <row r="160" spans="2:7">
@@ -4147,16 +4160,16 @@
         <v>158</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>309</v>
+        <v>302</v>
       </c>
       <c r="D160" s="1" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="E160" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F160" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G160" s="1"/>
     </row>
@@ -4165,10 +4178,10 @@
         <v>159</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="D161" s="1" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="E161" s="1" t="s">
         <v>5</v>
@@ -4181,30 +4194,48 @@
         <v>160</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="D162" s="1" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="E162" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F162" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F162" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="G162" s="1"/>
     </row>
     <row r="163" spans="2:7">
-      <c r="B163" s="6"/>
-      <c r="C163" s="1"/>
-      <c r="D163" s="1"/>
-      <c r="E163" s="1"/>
+      <c r="B163" s="6">
+        <v>161</v>
+      </c>
+      <c r="C163" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="D163" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="E163" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F163" s="1"/>
       <c r="G163" s="1"/>
     </row>
     <row r="164" spans="2:7">
-      <c r="B164" s="6"/>
-      <c r="C164" s="1"/>
-      <c r="D164" s="1"/>
-      <c r="E164" s="1"/>
+      <c r="B164" s="6">
+        <v>162</v>
+      </c>
+      <c r="C164" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="D164" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="E164" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F164" s="1"/>
       <c r="G164" s="1"/>
     </row>
@@ -4224,12 +4255,28 @@
       <c r="F166" s="1"/>
       <c r="G166" s="1"/>
     </row>
+    <row r="167" spans="2:7">
+      <c r="B167" s="6"/>
+      <c r="C167" s="1"/>
+      <c r="D167" s="1"/>
+      <c r="E167" s="1"/>
+      <c r="F167" s="1"/>
+      <c r="G167" s="1"/>
+    </row>
+    <row r="168" spans="2:7">
+      <c r="B168" s="6"/>
+      <c r="C168" s="1"/>
+      <c r="D168" s="1"/>
+      <c r="E168" s="1"/>
+      <c r="F168" s="1"/>
+      <c r="G168" s="1"/>
+    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E162" xr:uid="{7E8CE32C-29D1-4006-9E0F-69B72A0F4378}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E164" xr:uid="{7E8CE32C-29D1-4006-9E0F-69B72A0F4378}">
       <formula1>"[Application],[Directory],[Script]"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F166" xr:uid="{A5D947FB-5606-4B36-88C5-81CC2B61C636}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F168" xr:uid="{A5D947FB-5606-4B36-88C5-81CC2B61C636}">
       <formula1>"[bat],[vbs]"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Repo Update: 2024-07-19 20:11:42
</commit_message>
<xml_diff>
--- a/Database/Run_shortcut_creator_aliases.xlsx
+++ b/Database/Run_shortcut_creator_aliases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\player-1\Documents\Windows-Git-Repos\win-t\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA9E1451-369B-4234-9AA0-3D2597CF6E6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C02D9174-C59B-4819-AC1C-E08D0C78E12B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D65865D6-BB34-410C-8183-31ED199784FF}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14625" windowHeight="15585" xr2:uid="{D65865D6-BB34-410C-8183-31ED199784FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Run Shortcut Creator Aliases" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="353">
   <si>
     <t>Number</t>
   </si>
@@ -93,9 +93,6 @@
     <t>Windows 11 Manager</t>
   </si>
   <si>
-    <t>11m</t>
-  </si>
-  <si>
     <t>Church Presentation (Admin)</t>
   </si>
   <si>
@@ -114,9 +111,6 @@
     <t>Excel</t>
   </si>
   <si>
-    <t>aegis</t>
-  </si>
-  <si>
     <t>Advanced Hymn Order</t>
   </si>
   <si>
@@ -129,18 +123,6 @@
     <t>aida</t>
   </si>
   <si>
-    <t xml:space="preserve">Advanced IP Scanner </t>
-  </si>
-  <si>
-    <t>ais</t>
-  </si>
-  <si>
-    <t>akcp</t>
-  </si>
-  <si>
-    <t>Admin - Kill Chuch Presentation</t>
-  </si>
-  <si>
     <t>Admin -Kill EasyWorship</t>
   </si>
   <si>
@@ -531,18 +513,6 @@
     <t>mix</t>
   </si>
   <si>
-    <t>MKVCleaver</t>
-  </si>
-  <si>
-    <t>mkvc</t>
-  </si>
-  <si>
-    <t>MKVToolNix</t>
-  </si>
-  <si>
-    <t>mkvt</t>
-  </si>
-  <si>
     <t>Microsoft Store</t>
   </si>
   <si>
@@ -615,9 +585,6 @@
     <t>pdf</t>
   </si>
   <si>
-    <t>Adobe Acrobat Dc</t>
-  </si>
-  <si>
     <t>pdfe</t>
   </si>
   <si>
@@ -813,12 +780,6 @@
     <t>subl</t>
   </si>
   <si>
-    <t>Subtitle Speech Synchronizer</t>
-  </si>
-  <si>
-    <t>subsync</t>
-  </si>
-  <si>
     <t>Mp3tag</t>
   </si>
   <si>
@@ -1029,9 +990,6 @@
     <t>aai</t>
   </si>
   <si>
-    <t>C:\MY-TOOLS\Windows Store\Alternative Windows Apps Installer\alt app installer</t>
-  </si>
-  <si>
     <t>Librewolf (Mails)</t>
   </si>
   <si>
@@ -1066,6 +1024,99 @@
   </si>
   <si>
     <t>nsd</t>
+  </si>
+  <si>
+    <t>C:\MY-TOOLS\Windows Store\alt app installer</t>
+  </si>
+  <si>
+    <t>aho</t>
+  </si>
+  <si>
+    <t>Libreoffice Draw</t>
+  </si>
+  <si>
+    <t>lod</t>
+  </si>
+  <si>
+    <t>Libreoffice Writer</t>
+  </si>
+  <si>
+    <t>low</t>
+  </si>
+  <si>
+    <t>LizardSystems Network Scanner</t>
+  </si>
+  <si>
+    <t>Windows Manager Directory</t>
+  </si>
+  <si>
+    <t>wmd</t>
+  </si>
+  <si>
+    <t>ns</t>
+  </si>
+  <si>
+    <t>Notepad ++</t>
+  </si>
+  <si>
+    <t>npp</t>
+  </si>
+  <si>
+    <t>cec</t>
+  </si>
+  <si>
+    <t>ChoEazyCopy</t>
+  </si>
+  <si>
+    <t>Folder Change View</t>
+  </si>
+  <si>
+    <t>fcv</t>
+  </si>
+  <si>
+    <t>R-drive Image</t>
+  </si>
+  <si>
+    <t>rdi</t>
+  </si>
+  <si>
+    <t>Foxit PDF Editor</t>
+  </si>
+  <si>
+    <t>Quick Startup</t>
+  </si>
+  <si>
+    <t>qs</t>
+  </si>
+  <si>
+    <t>Directory Opus</t>
+  </si>
+  <si>
+    <t>do</t>
+  </si>
+  <si>
+    <t>C:\Users\player-1</t>
+  </si>
+  <si>
+    <t>home</t>
+  </si>
+  <si>
+    <t>Adobe Acrobat DC</t>
+  </si>
+  <si>
+    <t>acro</t>
+  </si>
+  <si>
+    <t>Aliases_Automation</t>
+  </si>
+  <si>
+    <t>alia</t>
+  </si>
+  <si>
+    <t>ri</t>
+  </si>
+  <si>
+    <t>ReIcon</t>
   </si>
 </sst>
 </file>
@@ -1497,10 +1548,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58A033C2-67FB-408D-B72B-8C45836FCF74}">
-  <dimension ref="B2:G168"/>
+  <dimension ref="B2:G176"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A69" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
-      <selection activeCell="H90" sqref="H90"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B102" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
+      <selection activeCell="C121" sqref="C121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21"/>
@@ -1536,7 +1587,7 @@
     </row>
     <row r="3" spans="2:7" ht="24.95" customHeight="1">
       <c r="B3" s="6" cm="1">
-        <f t="array" ref="B3:B164">_xlfn.SEQUENCE(COUNTA(C:C)-1)</f>
+        <f t="array" ref="B3:B172">_xlfn.SEQUENCE(COUNTA(C:C)-1)</f>
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -1556,10 +1607,10 @@
         <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>10</v>
+        <v>322</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>11</v>
+        <v>309</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>6</v>
@@ -1572,13 +1623,13 @@
         <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>323</v>
+        <v>11</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>322</v>
+        <v>12</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
@@ -1588,10 +1639,10 @@
         <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>12</v>
+        <v>347</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>13</v>
+        <v>348</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>5</v>
@@ -1604,16 +1655,16 @@
         <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>330</v>
+        <v>316</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>331</v>
+        <v>317</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="G7" s="1"/>
     </row>
@@ -1622,16 +1673,16 @@
         <v>6</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="E8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="G8" s="1"/>
     </row>
@@ -1640,10 +1691,10 @@
         <v>7</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>18</v>
+        <v>323</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>5</v>
@@ -1656,10 +1707,10 @@
         <v>8</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>5</v>
@@ -1672,10 +1723,10 @@
         <v>9</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>315</v>
+        <v>302</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>5</v>
@@ -1688,15 +1739,17 @@
         <v>10</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F12" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="G12" s="1"/>
     </row>
     <row r="13" spans="2:7" ht="24.95" customHeight="1">
@@ -1704,17 +1757,15 @@
         <v>11</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F13" s="1"/>
       <c r="G13" s="1"/>
     </row>
     <row r="14" spans="2:7" ht="24.95" customHeight="1">
@@ -1722,31 +1773,33 @@
         <v>12</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F14" s="1" t="s">
+      <c r="G14" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G14" s="1"/>
     </row>
     <row r="15" spans="2:7" ht="24.95" customHeight="1">
       <c r="B15" s="6">
         <v>13</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>29</v>
+        <v>349</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>30</v>
+        <v>350</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
@@ -1756,19 +1809,19 @@
         <v>14</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="2:7" ht="24.95" customHeight="1">
@@ -1776,30 +1829,26 @@
         <v>15</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>36</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
     </row>
     <row r="18" spans="2:7" ht="24.95" customHeight="1">
       <c r="B18" s="6">
         <v>16</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>5</v>
@@ -1812,15 +1861,17 @@
         <v>17</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F19" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G19" s="1"/>
     </row>
     <row r="20" spans="2:7" ht="24.95" customHeight="1">
@@ -1828,16 +1879,16 @@
         <v>18</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="G20" s="1"/>
     </row>
@@ -1846,17 +1897,15 @@
         <v>19</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>33</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F21" s="1"/>
       <c r="G21" s="1"/>
     </row>
     <row r="22" spans="2:7" ht="24.95" customHeight="1">
@@ -1864,13 +1913,13 @@
         <v>20</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
@@ -1880,15 +1929,17 @@
         <v>21</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F23" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="G23" s="1"/>
     </row>
     <row r="24" spans="2:7" ht="24.95" customHeight="1">
@@ -1896,16 +1947,16 @@
         <v>22</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="G24" s="1"/>
     </row>
@@ -1914,17 +1965,15 @@
         <v>23</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>33</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F25" s="1"/>
       <c r="G25" s="1"/>
     </row>
     <row r="26" spans="2:7" ht="24.95" customHeight="1">
@@ -1932,13 +1981,13 @@
         <v>24</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>53</v>
+        <v>305</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>54</v>
+        <v>306</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
@@ -1948,13 +1997,13 @@
         <v>25</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>318</v>
+        <v>335</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>319</v>
+        <v>334</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
@@ -1964,16 +2013,16 @@
         <v>26</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G28" s="1"/>
     </row>
@@ -1982,10 +2031,10 @@
         <v>27</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>5</v>
@@ -1998,10 +2047,10 @@
         <v>28</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>6</v>
@@ -2014,10 +2063,10 @@
         <v>29</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>320</v>
+        <v>307</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>321</v>
+        <v>308</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>5</v>
@@ -2030,10 +2079,10 @@
         <v>30</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>5</v>
@@ -2046,16 +2095,16 @@
         <v>31</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G33" s="1"/>
     </row>
@@ -2064,16 +2113,16 @@
         <v>32</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G34" s="1"/>
     </row>
@@ -2082,16 +2131,16 @@
         <v>33</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G35" s="1"/>
     </row>
@@ -2100,10 +2149,10 @@
         <v>34</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>6</v>
@@ -2116,10 +2165,10 @@
         <v>35</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>5</v>
@@ -2132,16 +2181,16 @@
         <v>36</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="G38" s="1"/>
     </row>
@@ -2150,10 +2199,10 @@
         <v>37</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>5</v>
@@ -2166,16 +2215,16 @@
         <v>38</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="G40" s="1"/>
     </row>
@@ -2184,10 +2233,10 @@
         <v>39</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>5</v>
@@ -2200,16 +2249,16 @@
         <v>40</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G42" s="1"/>
     </row>
@@ -2218,17 +2267,15 @@
         <v>41</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>82</v>
+        <v>343</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>83</v>
+        <v>344</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>33</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F43" s="1"/>
       <c r="G43" s="1"/>
     </row>
     <row r="44" spans="2:7">
@@ -2236,15 +2283,17 @@
         <v>42</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>316</v>
+        <v>76</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>317</v>
+        <v>77</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F44" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G44" s="1"/>
     </row>
     <row r="45" spans="2:7">
@@ -2252,17 +2301,15 @@
         <v>43</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>84</v>
+        <v>303</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>85</v>
+        <v>304</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>33</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="F45" s="1"/>
       <c r="G45" s="1"/>
     </row>
     <row r="46" spans="2:7">
@@ -2270,16 +2317,16 @@
         <v>44</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="G46" s="1"/>
     </row>
@@ -2288,16 +2335,16 @@
         <v>45</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="G47" s="1"/>
     </row>
@@ -2306,15 +2353,17 @@
         <v>46</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F48" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G48" s="1"/>
     </row>
     <row r="49" spans="2:7">
@@ -2322,10 +2371,10 @@
         <v>47</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>5</v>
@@ -2338,17 +2387,15 @@
         <v>48</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F50" s="1"/>
       <c r="G50" s="1"/>
     </row>
     <row r="51" spans="2:7">
@@ -2356,16 +2403,16 @@
         <v>49</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G51" s="1"/>
     </row>
@@ -2374,15 +2421,17 @@
         <v>50</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F52" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="G52" s="1"/>
     </row>
     <row r="53" spans="2:7">
@@ -2390,10 +2439,10 @@
         <v>51</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>5</v>
@@ -2401,15 +2450,15 @@
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
     </row>
-    <row r="54" spans="2:7">
+    <row r="54" spans="2:7" ht="21.75" customHeight="1">
       <c r="B54" s="6">
         <v>52</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>5</v>
@@ -2422,10 +2471,10 @@
         <v>53</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>5</v>
@@ -2438,10 +2487,10 @@
         <v>54</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>106</v>
+        <v>336</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>107</v>
+        <v>337</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>5</v>
@@ -2454,10 +2503,10 @@
         <v>55</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>5</v>
@@ -2470,13 +2519,13 @@
         <v>56</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F58" s="1"/>
       <c r="G58" s="1"/>
@@ -2486,10 +2535,10 @@
         <v>57</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>5</v>
@@ -2502,13 +2551,13 @@
         <v>58</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F60" s="1"/>
       <c r="G60" s="1"/>
@@ -2518,17 +2567,15 @@
         <v>59</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F61" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F61" s="1"/>
       <c r="G61" s="1"/>
     </row>
     <row r="62" spans="2:7">
@@ -2536,17 +2583,15 @@
         <v>60</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F62" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F62" s="1"/>
       <c r="G62" s="1"/>
     </row>
     <row r="63" spans="2:7">
@@ -2554,15 +2599,17 @@
         <v>61</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F63" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="G63" s="1"/>
     </row>
     <row r="64" spans="2:7">
@@ -2570,16 +2617,16 @@
         <v>62</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="E64" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="G64" s="1"/>
     </row>
@@ -2588,13 +2635,13 @@
         <v>63</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>125</v>
+        <v>345</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>126</v>
+        <v>346</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F65" s="1"/>
       <c r="G65" s="1"/>
@@ -2604,10 +2651,10 @@
         <v>64</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="E66" s="1" t="s">
         <v>5</v>
@@ -2620,15 +2667,17 @@
         <v>65</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F67" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G67" s="1"/>
     </row>
     <row r="68" spans="2:7">
@@ -2636,10 +2685,10 @@
         <v>66</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>5</v>
@@ -2652,10 +2701,10 @@
         <v>67</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="E69" s="1" t="s">
         <v>5</v>
@@ -2668,10 +2717,10 @@
         <v>68</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="E70" s="1" t="s">
         <v>5</v>
@@ -2684,10 +2733,10 @@
         <v>69</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="E71" s="1" t="s">
         <v>5</v>
@@ -2700,10 +2749,10 @@
         <v>70</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="E72" s="1" t="s">
         <v>5</v>
@@ -2716,17 +2765,15 @@
         <v>71</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F73" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F73" s="1"/>
       <c r="G73" s="1"/>
     </row>
     <row r="74" spans="2:7">
@@ -2734,10 +2781,10 @@
         <v>72</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="E74" s="1" t="s">
         <v>5</v>
@@ -2750,17 +2797,15 @@
         <v>73</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F75" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F75" s="1"/>
       <c r="G75" s="1"/>
     </row>
     <row r="76" spans="2:7">
@@ -2768,15 +2813,17 @@
         <v>74</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F76" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="G76" s="1"/>
     </row>
     <row r="77" spans="2:7">
@@ -2784,10 +2831,10 @@
         <v>75</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>332</v>
+        <v>137</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>333</v>
+        <v>138</v>
       </c>
       <c r="E77" s="1" t="s">
         <v>5</v>
@@ -2800,16 +2847,16 @@
         <v>76</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="E78" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G78" s="1"/>
     </row>
@@ -2818,10 +2865,10 @@
         <v>77</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="E79" s="1" t="s">
         <v>5</v>
@@ -2834,10 +2881,10 @@
         <v>78</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
       <c r="E80" s="1" t="s">
         <v>5</v>
@@ -2850,10 +2897,10 @@
         <v>79</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>153</v>
+        <v>324</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>154</v>
+        <v>325</v>
       </c>
       <c r="E81" s="1" t="s">
         <v>5</v>
@@ -2866,15 +2913,17 @@
         <v>80</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F82" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="G82" s="1"/>
     </row>
     <row r="83" spans="2:7">
@@ -2882,10 +2931,10 @@
         <v>81</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>157</v>
+        <v>326</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>158</v>
+        <v>327</v>
       </c>
       <c r="E83" s="1" t="s">
         <v>5</v>
@@ -2898,10 +2947,10 @@
         <v>82</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="E84" s="1" t="s">
         <v>5</v>
@@ -2914,17 +2963,15 @@
         <v>83</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>161</v>
+        <v>310</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>162</v>
+        <v>311</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F85" s="1" t="s">
-        <v>33</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F85" s="1"/>
       <c r="G85" s="1"/>
     </row>
     <row r="86" spans="2:7">
@@ -2932,17 +2979,15 @@
         <v>84</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>163</v>
+        <v>147</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F86" s="1" t="s">
-        <v>33</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F86" s="1"/>
       <c r="G86" s="1"/>
     </row>
     <row r="87" spans="2:7">
@@ -2950,17 +2995,15 @@
         <v>85</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>165</v>
+        <v>149</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>166</v>
+        <v>150</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F87" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F87" s="1"/>
       <c r="G87" s="1"/>
     </row>
     <row r="88" spans="2:7">
@@ -2968,15 +3011,17 @@
         <v>86</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>167</v>
+        <v>151</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>168</v>
+        <v>152</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F88" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F88" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G88" s="1"/>
     </row>
     <row r="89" spans="2:7">
@@ -2984,15 +3029,17 @@
         <v>87</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>169</v>
+        <v>153</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>170</v>
+        <v>154</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F89" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F89" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G89" s="1"/>
     </row>
     <row r="90" spans="2:7">
@@ -3000,15 +3047,17 @@
         <v>88</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>171</v>
+        <v>155</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>172</v>
+        <v>156</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F90" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F90" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="G90" s="1"/>
     </row>
     <row r="91" spans="2:7">
@@ -3016,17 +3065,15 @@
         <v>89</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>334</v>
+        <v>157</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>335</v>
+        <v>158</v>
       </c>
       <c r="E91" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F91" s="1" t="s">
-        <v>33</v>
-      </c>
+      <c r="F91" s="1"/>
       <c r="G91" s="1"/>
     </row>
     <row r="92" spans="2:7">
@@ -3034,13 +3081,13 @@
         <v>90</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F92" s="1"/>
       <c r="G92" s="1"/>
@@ -3050,10 +3097,10 @@
         <v>91</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>329</v>
+        <v>161</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>328</v>
+        <v>162</v>
       </c>
       <c r="E93" s="1" t="s">
         <v>5</v>
@@ -3066,10 +3113,10 @@
         <v>92</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>326</v>
+        <v>163</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>327</v>
+        <v>164</v>
       </c>
       <c r="E94" s="1" t="s">
         <v>5</v>
@@ -3082,10 +3129,10 @@
         <v>93</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>175</v>
+        <v>332</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>176</v>
+        <v>333</v>
       </c>
       <c r="E95" s="1" t="s">
         <v>5</v>
@@ -3098,10 +3145,10 @@
         <v>94</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>177</v>
+        <v>328</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>178</v>
+        <v>331</v>
       </c>
       <c r="E96" s="1" t="s">
         <v>5</v>
@@ -3114,15 +3161,17 @@
         <v>95</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>179</v>
+        <v>320</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>180</v>
+        <v>321</v>
       </c>
       <c r="E97" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F97" s="1"/>
+      <c r="F97" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G97" s="1"/>
     </row>
     <row r="98" spans="2:7">
@@ -3130,10 +3179,10 @@
         <v>96</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>181</v>
+        <v>315</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>182</v>
+        <v>314</v>
       </c>
       <c r="E98" s="1" t="s">
         <v>5</v>
@@ -3146,10 +3195,10 @@
         <v>97</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>183</v>
+        <v>312</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>184</v>
+        <v>313</v>
       </c>
       <c r="E99" s="1" t="s">
         <v>5</v>
@@ -3162,10 +3211,10 @@
         <v>98</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>185</v>
+        <v>165</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>186</v>
+        <v>166</v>
       </c>
       <c r="E100" s="1" t="s">
         <v>5</v>
@@ -3178,10 +3227,10 @@
         <v>99</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>187</v>
+        <v>167</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>188</v>
+        <v>168</v>
       </c>
       <c r="E101" s="1" t="s">
         <v>5</v>
@@ -3194,17 +3243,15 @@
         <v>100</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>189</v>
+        <v>169</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>190</v>
+        <v>170</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F102" s="1" t="s">
-        <v>33</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F102" s="1"/>
       <c r="G102" s="1"/>
     </row>
     <row r="103" spans="2:7">
@@ -3212,10 +3259,10 @@
         <v>101</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>191</v>
+        <v>171</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>192</v>
+        <v>172</v>
       </c>
       <c r="E103" s="1" t="s">
         <v>5</v>
@@ -3228,10 +3275,10 @@
         <v>102</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>193</v>
+        <v>173</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>194</v>
+        <v>174</v>
       </c>
       <c r="E104" s="1" t="s">
         <v>5</v>
@@ -3244,10 +3291,10 @@
         <v>103</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>195</v>
+        <v>340</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>196</v>
+        <v>175</v>
       </c>
       <c r="E105" s="1" t="s">
         <v>5</v>
@@ -3260,10 +3307,10 @@
         <v>104</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>197</v>
+        <v>176</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>198</v>
+        <v>177</v>
       </c>
       <c r="E106" s="1" t="s">
         <v>5</v>
@@ -3276,15 +3323,17 @@
         <v>105</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>199</v>
+        <v>178</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>200</v>
+        <v>179</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F107" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F107" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G107" s="1"/>
     </row>
     <row r="108" spans="2:7">
@@ -3292,10 +3341,10 @@
         <v>106</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>201</v>
+        <v>180</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>202</v>
+        <v>181</v>
       </c>
       <c r="E108" s="1" t="s">
         <v>5</v>
@@ -3308,10 +3357,10 @@
         <v>107</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>203</v>
+        <v>182</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>204</v>
+        <v>183</v>
       </c>
       <c r="E109" s="1" t="s">
         <v>5</v>
@@ -3324,10 +3373,10 @@
         <v>108</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>205</v>
+        <v>184</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>206</v>
+        <v>185</v>
       </c>
       <c r="E110" s="1" t="s">
         <v>5</v>
@@ -3340,17 +3389,15 @@
         <v>109</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>207</v>
+        <v>186</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>208</v>
+        <v>187</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F111" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F111" s="1"/>
       <c r="G111" s="1"/>
     </row>
     <row r="112" spans="2:7">
@@ -3358,10 +3405,10 @@
         <v>110</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>209</v>
+        <v>188</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>210</v>
+        <v>189</v>
       </c>
       <c r="E112" s="1" t="s">
         <v>5</v>
@@ -3374,10 +3421,10 @@
         <v>111</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>211</v>
+        <v>190</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>212</v>
+        <v>191</v>
       </c>
       <c r="E113" s="1" t="s">
         <v>5</v>
@@ -3390,10 +3437,10 @@
         <v>112</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>213</v>
+        <v>192</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>214</v>
+        <v>193</v>
       </c>
       <c r="E114" s="1" t="s">
         <v>5</v>
@@ -3406,10 +3453,10 @@
         <v>113</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>215</v>
+        <v>341</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>216</v>
+        <v>342</v>
       </c>
       <c r="E115" s="1" t="s">
         <v>5</v>
@@ -3422,13 +3469,13 @@
         <v>114</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>217</v>
+        <v>194</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>218</v>
+        <v>195</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F116" s="1"/>
       <c r="G116" s="1"/>
@@ -3438,10 +3485,10 @@
         <v>115</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>219</v>
+        <v>338</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>220</v>
+        <v>339</v>
       </c>
       <c r="E117" s="1" t="s">
         <v>5</v>
@@ -3454,15 +3501,17 @@
         <v>116</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>221</v>
+        <v>196</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>222</v>
+        <v>197</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F118" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F118" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="G118" s="1"/>
     </row>
     <row r="119" spans="2:7">
@@ -3470,10 +3519,10 @@
         <v>117</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>223</v>
+        <v>198</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>224</v>
+        <v>199</v>
       </c>
       <c r="E119" s="1" t="s">
         <v>5</v>
@@ -3486,17 +3535,15 @@
         <v>118</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>225</v>
+        <v>200</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>226</v>
+        <v>201</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F120" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F120" s="1"/>
       <c r="G120" s="1"/>
     </row>
     <row r="121" spans="2:7">
@@ -3504,10 +3551,10 @@
         <v>119</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>227</v>
+        <v>352</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>228</v>
+        <v>351</v>
       </c>
       <c r="E121" s="1" t="s">
         <v>5</v>
@@ -3520,10 +3567,10 @@
         <v>120</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>229</v>
+        <v>202</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>230</v>
+        <v>203</v>
       </c>
       <c r="E122" s="1" t="s">
         <v>5</v>
@@ -3536,17 +3583,15 @@
         <v>121</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>231</v>
+        <v>204</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>232</v>
+        <v>205</v>
       </c>
       <c r="E123" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F123" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F123" s="1"/>
       <c r="G123" s="1"/>
     </row>
     <row r="124" spans="2:7">
@@ -3554,77 +3599,63 @@
         <v>122</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>233</v>
+        <v>206</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>235</v>
+        <v>207</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F124" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G124" s="1" t="s">
-        <v>36</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="F124" s="1"/>
+      <c r="G124" s="1"/>
     </row>
     <row r="125" spans="2:7">
       <c r="B125" s="6">
         <v>123</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>234</v>
+        <v>208</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>236</v>
+        <v>209</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F125" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G125" s="1" t="s">
-        <v>36</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F125" s="1"/>
+      <c r="G125" s="1"/>
     </row>
     <row r="126" spans="2:7">
       <c r="B126" s="6">
         <v>124</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>237</v>
+        <v>210</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>238</v>
+        <v>211</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F126" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G126" s="1" t="s">
-        <v>314</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F126" s="1"/>
+      <c r="G126" s="1"/>
     </row>
     <row r="127" spans="2:7">
       <c r="B127" s="6">
         <v>125</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>239</v>
+        <v>212</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>240</v>
+        <v>213</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F127" s="1" t="s">
-        <v>33</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F127" s="1"/>
       <c r="G127" s="1"/>
     </row>
     <row r="128" spans="2:7">
@@ -3632,15 +3663,17 @@
         <v>126</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>241</v>
+        <v>214</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>242</v>
+        <v>215</v>
       </c>
       <c r="E128" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F128" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F128" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="G128" s="1"/>
     </row>
     <row r="129" spans="2:7">
@@ -3648,10 +3681,10 @@
         <v>127</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>243</v>
+        <v>216</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>244</v>
+        <v>217</v>
       </c>
       <c r="E129" s="1" t="s">
         <v>5</v>
@@ -3664,17 +3697,15 @@
         <v>128</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>245</v>
+        <v>218</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>246</v>
+        <v>219</v>
       </c>
       <c r="E130" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F130" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F130" s="1"/>
       <c r="G130" s="1"/>
     </row>
     <row r="131" spans="2:7">
@@ -3682,16 +3713,16 @@
         <v>129</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>248</v>
+        <v>220</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>247</v>
+        <v>221</v>
       </c>
       <c r="E131" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F131" s="1" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="G131" s="1"/>
     </row>
@@ -3700,63 +3731,77 @@
         <v>130</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>249</v>
+        <v>222</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>250</v>
+        <v>224</v>
       </c>
       <c r="E132" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F132" s="1"/>
-      <c r="G132" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F132" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G132" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="133" spans="2:7">
       <c r="B133" s="6">
         <v>131</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>251</v>
+        <v>223</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>252</v>
+        <v>225</v>
       </c>
       <c r="E133" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F133" s="1"/>
-      <c r="G133" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F133" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G133" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="134" spans="2:7">
       <c r="B134" s="6">
         <v>132</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>253</v>
+        <v>226</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>254</v>
+        <v>227</v>
       </c>
       <c r="E134" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F134" s="1"/>
-      <c r="G134" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F134" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G134" s="1" t="s">
+        <v>301</v>
+      </c>
     </row>
     <row r="135" spans="2:7">
       <c r="B135" s="6">
         <v>133</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>255</v>
+        <v>228</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>256</v>
+        <v>229</v>
       </c>
       <c r="E135" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F135" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F135" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G135" s="1"/>
     </row>
     <row r="136" spans="2:7">
@@ -3764,10 +3809,10 @@
         <v>134</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>257</v>
+        <v>230</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>258</v>
+        <v>231</v>
       </c>
       <c r="E136" s="1" t="s">
         <v>5</v>
@@ -3780,17 +3825,15 @@
         <v>135</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>259</v>
+        <v>232</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>260</v>
+        <v>233</v>
       </c>
       <c r="E137" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F137" s="1" t="s">
-        <v>33</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F137" s="1"/>
       <c r="G137" s="1"/>
     </row>
     <row r="138" spans="2:7">
@@ -3798,15 +3841,17 @@
         <v>136</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>261</v>
+        <v>234</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>262</v>
+        <v>235</v>
       </c>
       <c r="E138" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F138" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F138" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="G138" s="1"/>
     </row>
     <row r="139" spans="2:7">
@@ -3814,15 +3859,17 @@
         <v>137</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>263</v>
+        <v>237</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>264</v>
+        <v>236</v>
       </c>
       <c r="E139" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F139" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F139" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G139" s="1"/>
     </row>
     <row r="140" spans="2:7">
@@ -3830,10 +3877,10 @@
         <v>138</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>265</v>
+        <v>238</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>266</v>
+        <v>239</v>
       </c>
       <c r="E140" s="1" t="s">
         <v>5</v>
@@ -3846,10 +3893,10 @@
         <v>139</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>267</v>
+        <v>240</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>268</v>
+        <v>241</v>
       </c>
       <c r="E141" s="1" t="s">
         <v>5</v>
@@ -3862,10 +3909,10 @@
         <v>140</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>269</v>
+        <v>242</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>270</v>
+        <v>243</v>
       </c>
       <c r="E142" s="1" t="s">
         <v>5</v>
@@ -3878,10 +3925,10 @@
         <v>141</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>271</v>
+        <v>244</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>272</v>
+        <v>245</v>
       </c>
       <c r="E143" s="1" t="s">
         <v>5</v>
@@ -3894,15 +3941,17 @@
         <v>142</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>273</v>
+        <v>246</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>274</v>
+        <v>247</v>
       </c>
       <c r="E144" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F144" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F144" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G144" s="1"/>
     </row>
     <row r="145" spans="2:7">
@@ -3910,17 +3959,15 @@
         <v>143</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>275</v>
+        <v>248</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="E145" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F145" s="1" t="s">
-        <v>33</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="F145" s="1"/>
       <c r="G145" s="1"/>
     </row>
     <row r="146" spans="2:7">
@@ -3928,10 +3975,10 @@
         <v>144</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>277</v>
+        <v>250</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>278</v>
+        <v>251</v>
       </c>
       <c r="E146" s="1" t="s">
         <v>5</v>
@@ -3944,10 +3991,10 @@
         <v>145</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>279</v>
+        <v>252</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>280</v>
+        <v>253</v>
       </c>
       <c r="E147" s="1" t="s">
         <v>5</v>
@@ -3960,17 +4007,15 @@
         <v>146</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>281</v>
+        <v>254</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>282</v>
+        <v>255</v>
       </c>
       <c r="E148" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F148" s="1" t="s">
-        <v>33</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F148" s="1"/>
       <c r="G148" s="1"/>
     </row>
     <row r="149" spans="2:7">
@@ -3978,10 +4023,10 @@
         <v>147</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>283</v>
+        <v>256</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>284</v>
+        <v>257</v>
       </c>
       <c r="E149" s="1" t="s">
         <v>5</v>
@@ -3994,10 +4039,10 @@
         <v>148</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>285</v>
+        <v>258</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>286</v>
+        <v>259</v>
       </c>
       <c r="E150" s="1" t="s">
         <v>5</v>
@@ -4010,10 +4055,10 @@
         <v>149</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>287</v>
+        <v>260</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>288</v>
+        <v>261</v>
       </c>
       <c r="E151" s="1" t="s">
         <v>5</v>
@@ -4026,15 +4071,17 @@
         <v>150</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>289</v>
+        <v>262</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>290</v>
+        <v>263</v>
       </c>
       <c r="E152" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F152" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F152" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G152" s="1"/>
     </row>
     <row r="153" spans="2:7">
@@ -4042,10 +4089,10 @@
         <v>151</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>291</v>
+        <v>264</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>292</v>
+        <v>265</v>
       </c>
       <c r="E153" s="1" t="s">
         <v>5</v>
@@ -4058,10 +4105,10 @@
         <v>152</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>10</v>
+        <v>266</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>293</v>
+        <v>267</v>
       </c>
       <c r="E154" s="1" t="s">
         <v>5</v>
@@ -4074,16 +4121,16 @@
         <v>153</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>294</v>
+        <v>268</v>
       </c>
       <c r="D155" s="1" t="s">
-        <v>295</v>
+        <v>269</v>
       </c>
       <c r="E155" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F155" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="G155" s="1"/>
     </row>
@@ -4092,10 +4139,10 @@
         <v>154</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>296</v>
+        <v>270</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>297</v>
+        <v>271</v>
       </c>
       <c r="E156" s="1" t="s">
         <v>5</v>
@@ -4108,13 +4155,13 @@
         <v>155</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>298</v>
+        <v>272</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>299</v>
+        <v>273</v>
       </c>
       <c r="E157" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F157" s="1"/>
       <c r="G157" s="1"/>
@@ -4124,17 +4171,15 @@
         <v>156</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>300</v>
+        <v>274</v>
       </c>
       <c r="D158" s="1" t="s">
-        <v>303</v>
+        <v>275</v>
       </c>
       <c r="E158" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F158" s="1" t="s">
-        <v>33</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F158" s="1"/>
       <c r="G158" s="1"/>
     </row>
     <row r="159" spans="2:7">
@@ -4142,17 +4187,15 @@
         <v>157</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>301</v>
+        <v>276</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>304</v>
+        <v>277</v>
       </c>
       <c r="E159" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F159" s="1" t="s">
-        <v>33</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F159" s="1"/>
       <c r="G159" s="1"/>
     </row>
     <row r="160" spans="2:7">
@@ -4160,17 +4203,15 @@
         <v>158</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>302</v>
+        <v>278</v>
       </c>
       <c r="D160" s="1" t="s">
-        <v>305</v>
+        <v>279</v>
       </c>
       <c r="E160" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F160" s="1" t="s">
-        <v>33</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F160" s="1"/>
       <c r="G160" s="1"/>
     </row>
     <row r="161" spans="2:7">
@@ -4178,10 +4219,10 @@
         <v>159</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>306</v>
+        <v>10</v>
       </c>
       <c r="D161" s="1" t="s">
-        <v>307</v>
+        <v>280</v>
       </c>
       <c r="E161" s="1" t="s">
         <v>5</v>
@@ -4194,17 +4235,15 @@
         <v>160</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>308</v>
+        <v>329</v>
       </c>
       <c r="D162" s="1" t="s">
-        <v>309</v>
+        <v>330</v>
       </c>
       <c r="E162" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F162" s="1" t="s">
-        <v>33</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="F162" s="1"/>
       <c r="G162" s="1"/>
     </row>
     <row r="163" spans="2:7">
@@ -4212,15 +4251,17 @@
         <v>161</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>310</v>
+        <v>281</v>
       </c>
       <c r="D163" s="1" t="s">
-        <v>311</v>
+        <v>282</v>
       </c>
       <c r="E163" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F163" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F163" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G163" s="1"/>
     </row>
     <row r="164" spans="2:7">
@@ -4228,10 +4269,10 @@
         <v>162</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>312</v>
+        <v>283</v>
       </c>
       <c r="D164" s="1" t="s">
-        <v>313</v>
+        <v>284</v>
       </c>
       <c r="E164" s="1" t="s">
         <v>5</v>
@@ -4240,43 +4281,179 @@
       <c r="G164" s="1"/>
     </row>
     <row r="165" spans="2:7">
-      <c r="B165" s="6"/>
-      <c r="C165" s="1"/>
-      <c r="D165" s="1"/>
-      <c r="E165" s="1"/>
+      <c r="B165" s="6">
+        <v>163</v>
+      </c>
+      <c r="C165" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="D165" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="E165" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="F165" s="1"/>
       <c r="G165" s="1"/>
     </row>
     <row r="166" spans="2:7">
-      <c r="B166" s="6"/>
-      <c r="C166" s="1"/>
-      <c r="D166" s="1"/>
-      <c r="E166" s="1"/>
-      <c r="F166" s="1"/>
+      <c r="B166" s="6">
+        <v>164</v>
+      </c>
+      <c r="C166" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="D166" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="E166" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F166" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G166" s="1"/>
     </row>
     <row r="167" spans="2:7">
-      <c r="B167" s="6"/>
-      <c r="C167" s="1"/>
-      <c r="D167" s="1"/>
-      <c r="E167" s="1"/>
-      <c r="F167" s="1"/>
+      <c r="B167" s="6">
+        <v>165</v>
+      </c>
+      <c r="C167" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="D167" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="E167" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F167" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G167" s="1"/>
     </row>
     <row r="168" spans="2:7">
-      <c r="B168" s="6"/>
-      <c r="C168" s="1"/>
-      <c r="D168" s="1"/>
-      <c r="E168" s="1"/>
-      <c r="F168" s="1"/>
+      <c r="B168" s="6">
+        <v>166</v>
+      </c>
+      <c r="C168" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="D168" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="E168" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F168" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G168" s="1"/>
+    </row>
+    <row r="169" spans="2:7">
+      <c r="B169" s="6">
+        <v>167</v>
+      </c>
+      <c r="C169" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="D169" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="E169" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F169" s="1"/>
+      <c r="G169" s="1"/>
+    </row>
+    <row r="170" spans="2:7">
+      <c r="B170" s="6">
+        <v>168</v>
+      </c>
+      <c r="C170" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="D170" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="E170" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F170" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G170" s="1"/>
+    </row>
+    <row r="171" spans="2:7">
+      <c r="B171" s="6">
+        <v>169</v>
+      </c>
+      <c r="C171" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="D171" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="E171" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F171" s="1"/>
+      <c r="G171" s="1"/>
+    </row>
+    <row r="172" spans="2:7">
+      <c r="B172" s="6">
+        <v>170</v>
+      </c>
+      <c r="C172" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="D172" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="E172" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F172" s="1"/>
+      <c r="G172" s="1"/>
+    </row>
+    <row r="173" spans="2:7">
+      <c r="B173" s="6"/>
+      <c r="C173" s="1"/>
+      <c r="D173" s="1"/>
+      <c r="E173" s="1"/>
+      <c r="F173" s="1"/>
+      <c r="G173" s="1"/>
+    </row>
+    <row r="174" spans="2:7">
+      <c r="B174" s="6"/>
+      <c r="C174" s="1"/>
+      <c r="D174" s="1"/>
+      <c r="E174" s="1"/>
+      <c r="F174" s="1"/>
+      <c r="G174" s="1"/>
+    </row>
+    <row r="175" spans="2:7">
+      <c r="B175" s="6"/>
+      <c r="C175" s="1"/>
+      <c r="D175" s="1"/>
+      <c r="E175" s="1"/>
+      <c r="F175" s="1"/>
+      <c r="G175" s="1"/>
+    </row>
+    <row r="176" spans="2:7">
+      <c r="B176" s="6"/>
+      <c r="C176" s="1"/>
+      <c r="D176" s="1"/>
+      <c r="E176" s="1"/>
+      <c r="F176" s="1"/>
+      <c r="G176" s="1"/>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E164" xr:uid="{7E8CE32C-29D1-4006-9E0F-69B72A0F4378}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E172" xr:uid="{7E8CE32C-29D1-4006-9E0F-69B72A0F4378}">
       <formula1>"[Application],[Directory],[Script]"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F168" xr:uid="{A5D947FB-5606-4B36-88C5-81CC2B61C636}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F176" xr:uid="{A5D947FB-5606-4B36-88C5-81CC2B61C636}">
       <formula1>"[bat],[vbs]"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Repo Update: 2024-07-29 15:51:08
</commit_message>
<xml_diff>
--- a/Database/Run_shortcut_creator_aliases.xlsx
+++ b/Database/Run_shortcut_creator_aliases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\player-1\Documents\Windows-Git-Repos\win-t\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C02D9174-C59B-4819-AC1C-E08D0C78E12B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AA3D8C1-8FEB-4BCD-9AC1-F157E790BE68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14625" windowHeight="15585" xr2:uid="{D65865D6-BB34-410C-8183-31ED199784FF}"/>
+    <workbookView xWindow="13215" yWindow="0" windowWidth="15705" windowHeight="15585" xr2:uid="{D65865D6-BB34-410C-8183-31ED199784FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Run Shortcut Creator Aliases" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="357">
   <si>
     <t>Number</t>
   </si>
@@ -1117,6 +1117,18 @@
   </si>
   <si>
     <t>ReIcon</t>
+  </si>
+  <si>
+    <t>kanti</t>
+  </si>
+  <si>
+    <t>Kill Antidote</t>
+  </si>
+  <si>
+    <t>anti</t>
+  </si>
+  <si>
+    <t>Antidote</t>
   </si>
 </sst>
 </file>
@@ -1548,10 +1560,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58A033C2-67FB-408D-B72B-8C45836FCF74}">
-  <dimension ref="B2:G176"/>
+  <dimension ref="B2:G178"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B102" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
-      <selection activeCell="C121" sqref="C121"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B164" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
+      <selection activeCell="D143" sqref="D143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21"/>
@@ -1587,7 +1599,7 @@
     </row>
     <row r="3" spans="2:7" ht="24.95" customHeight="1">
       <c r="B3" s="6" cm="1">
-        <f t="array" ref="B3:B172">_xlfn.SEQUENCE(COUNTA(C:C)-1)</f>
+        <f t="array" ref="B3:B174">_xlfn.SEQUENCE(COUNTA(C:C)-1)</f>
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -1829,10 +1841,10 @@
         <v>15</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>31</v>
+        <v>356</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>32</v>
+        <v>355</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>5</v>
@@ -1845,10 +1857,10 @@
         <v>16</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>5</v>
@@ -1861,17 +1873,15 @@
         <v>17</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>27</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F19" s="1"/>
       <c r="G19" s="1"/>
     </row>
     <row r="20" spans="2:7" ht="24.95" customHeight="1">
@@ -1879,10 +1889,10 @@
         <v>18</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>7</v>
@@ -1897,15 +1907,17 @@
         <v>19</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F21" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G21" s="1"/>
     </row>
     <row r="22" spans="2:7" ht="24.95" customHeight="1">
@@ -1913,13 +1925,13 @@
         <v>20</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
@@ -1929,17 +1941,15 @@
         <v>21</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="F23" s="1"/>
       <c r="G23" s="1"/>
     </row>
     <row r="24" spans="2:7" ht="24.95" customHeight="1">
@@ -1947,16 +1957,16 @@
         <v>22</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="G24" s="1"/>
     </row>
@@ -1965,15 +1975,17 @@
         <v>23</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F25" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G25" s="1"/>
     </row>
     <row r="26" spans="2:7" ht="24.95" customHeight="1">
@@ -1981,13 +1993,13 @@
         <v>24</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>305</v>
+        <v>47</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>306</v>
+        <v>48</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
@@ -1997,13 +2009,13 @@
         <v>25</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>335</v>
+        <v>305</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>334</v>
+        <v>306</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
@@ -2013,17 +2025,15 @@
         <v>26</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>110</v>
+        <v>335</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>49</v>
+        <v>334</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F28" s="1"/>
       <c r="G28" s="1"/>
     </row>
     <row r="29" spans="2:7" ht="24.95" customHeight="1">
@@ -2031,15 +2041,17 @@
         <v>27</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>50</v>
+        <v>110</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F29" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="G29" s="1"/>
     </row>
     <row r="30" spans="2:7" ht="24.95" customHeight="1">
@@ -2047,13 +2059,13 @@
         <v>28</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
@@ -2063,13 +2075,13 @@
         <v>29</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>307</v>
+        <v>52</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>308</v>
+        <v>53</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
@@ -2079,10 +2091,10 @@
         <v>30</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>55</v>
+        <v>307</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>54</v>
+        <v>308</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>5</v>
@@ -2095,17 +2107,15 @@
         <v>31</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F33" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="F33" s="1"/>
       <c r="G33" s="1"/>
     </row>
     <row r="34" spans="2:7" ht="24.95" customHeight="1">
@@ -2113,10 +2123,10 @@
         <v>32</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>5</v>
@@ -2131,10 +2141,10 @@
         <v>33</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>5</v>
@@ -2149,15 +2159,17 @@
         <v>34</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F36" s="1"/>
+        <v>5</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="G36" s="1"/>
     </row>
     <row r="37" spans="2:7" ht="24.95" customHeight="1">
@@ -2165,33 +2177,31 @@
         <v>35</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
     </row>
-    <row r="38" spans="2:7">
+    <row r="38" spans="2:7" ht="24.95" customHeight="1">
       <c r="B38" s="6">
         <v>36</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>27</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F38" s="1"/>
       <c r="G38" s="1"/>
     </row>
     <row r="39" spans="2:7">
@@ -2199,15 +2209,17 @@
         <v>37</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F39" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G39" s="1"/>
     </row>
     <row r="40" spans="2:7">
@@ -2215,17 +2227,15 @@
         <v>38</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>27</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F40" s="1"/>
       <c r="G40" s="1"/>
     </row>
     <row r="41" spans="2:7">
@@ -2233,15 +2243,17 @@
         <v>39</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F41" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G41" s="1"/>
     </row>
     <row r="42" spans="2:7">
@@ -2249,17 +2261,15 @@
         <v>40</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F42" s="1"/>
       <c r="G42" s="1"/>
     </row>
     <row r="43" spans="2:7">
@@ -2267,15 +2277,17 @@
         <v>41</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>343</v>
+        <v>74</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>344</v>
+        <v>75</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F43" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="G43" s="1"/>
     </row>
     <row r="44" spans="2:7">
@@ -2283,17 +2295,15 @@
         <v>42</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>76</v>
+        <v>343</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>77</v>
+        <v>344</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>27</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F44" s="1"/>
       <c r="G44" s="1"/>
     </row>
     <row r="45" spans="2:7">
@@ -2301,15 +2311,17 @@
         <v>43</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>303</v>
+        <v>76</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>304</v>
+        <v>77</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F45" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G45" s="1"/>
     </row>
     <row r="46" spans="2:7">
@@ -2317,17 +2329,15 @@
         <v>44</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>78</v>
+        <v>303</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>79</v>
+        <v>304</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>27</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="F46" s="1"/>
       <c r="G46" s="1"/>
     </row>
     <row r="47" spans="2:7">
@@ -2335,16 +2345,16 @@
         <v>45</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="G47" s="1"/>
     </row>
@@ -2353,16 +2363,16 @@
         <v>46</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="G48" s="1"/>
     </row>
@@ -2371,15 +2381,17 @@
         <v>47</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F49" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G49" s="1"/>
     </row>
     <row r="50" spans="2:7">
@@ -2387,10 +2399,10 @@
         <v>48</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>5</v>
@@ -2403,17 +2415,15 @@
         <v>49</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F51" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F51" s="1"/>
       <c r="G51" s="1"/>
     </row>
     <row r="52" spans="2:7">
@@ -2421,10 +2431,10 @@
         <v>50</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>7</v>
@@ -2439,26 +2449,28 @@
         <v>51</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F53" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="G53" s="1"/>
     </row>
-    <row r="54" spans="2:7" ht="21.75" customHeight="1">
+    <row r="54" spans="2:7">
       <c r="B54" s="6">
         <v>52</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>5</v>
@@ -2466,15 +2478,15 @@
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
     </row>
-    <row r="55" spans="2:7">
+    <row r="55" spans="2:7" ht="21.75" customHeight="1">
       <c r="B55" s="6">
         <v>53</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>5</v>
@@ -2487,10 +2499,10 @@
         <v>54</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>336</v>
+        <v>96</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>337</v>
+        <v>97</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>5</v>
@@ -2503,10 +2515,10 @@
         <v>55</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>98</v>
+        <v>336</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>99</v>
+        <v>337</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>5</v>
@@ -2519,10 +2531,10 @@
         <v>56</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>5</v>
@@ -2535,10 +2547,10 @@
         <v>57</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>5</v>
@@ -2551,13 +2563,13 @@
         <v>58</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F60" s="1"/>
       <c r="G60" s="1"/>
@@ -2567,13 +2579,13 @@
         <v>59</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F61" s="1"/>
       <c r="G61" s="1"/>
@@ -2583,10 +2595,10 @@
         <v>60</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>5</v>
@@ -2599,17 +2611,15 @@
         <v>61</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F63" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F63" s="1"/>
       <c r="G63" s="1"/>
     </row>
     <row r="64" spans="2:7">
@@ -2617,10 +2627,10 @@
         <v>62</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E64" s="1" t="s">
         <v>7</v>
@@ -2635,15 +2645,17 @@
         <v>63</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>345</v>
+        <v>113</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>346</v>
+        <v>114</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F65" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="G65" s="1"/>
     </row>
     <row r="66" spans="2:7">
@@ -2651,13 +2663,13 @@
         <v>64</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>115</v>
+        <v>345</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>116</v>
+        <v>346</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F66" s="1"/>
       <c r="G66" s="1"/>
@@ -2667,17 +2679,15 @@
         <v>65</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F67" s="1" t="s">
-        <v>27</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F67" s="1"/>
       <c r="G67" s="1"/>
     </row>
     <row r="68" spans="2:7">
@@ -2685,15 +2695,17 @@
         <v>66</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F68" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G68" s="1"/>
     </row>
     <row r="69" spans="2:7">
@@ -2701,10 +2713,10 @@
         <v>67</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E69" s="1" t="s">
         <v>5</v>
@@ -2717,10 +2729,10 @@
         <v>68</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E70" s="1" t="s">
         <v>5</v>
@@ -2733,10 +2745,10 @@
         <v>69</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E71" s="1" t="s">
         <v>5</v>
@@ -2749,10 +2761,10 @@
         <v>70</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E72" s="1" t="s">
         <v>5</v>
@@ -2765,10 +2777,10 @@
         <v>71</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E73" s="1" t="s">
         <v>5</v>
@@ -2781,10 +2793,10 @@
         <v>72</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E74" s="1" t="s">
         <v>5</v>
@@ -2797,10 +2809,10 @@
         <v>73</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E75" s="1" t="s">
         <v>5</v>
@@ -2813,16 +2825,16 @@
         <v>74</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>135</v>
+        <v>354</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>136</v>
+        <v>353</v>
       </c>
       <c r="E76" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="G76" s="1"/>
     </row>
@@ -2831,10 +2843,10 @@
         <v>75</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="E77" s="1" t="s">
         <v>5</v>
@@ -2847,10 +2859,10 @@
         <v>76</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E78" s="1" t="s">
         <v>7</v>
@@ -2865,10 +2877,10 @@
         <v>77</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="E79" s="1" t="s">
         <v>5</v>
@@ -2881,15 +2893,17 @@
         <v>78</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>318</v>
+        <v>139</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>319</v>
+        <v>140</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F80" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="G80" s="1"/>
     </row>
     <row r="81" spans="2:7">
@@ -2897,10 +2911,10 @@
         <v>79</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>324</v>
+        <v>141</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>325</v>
+        <v>142</v>
       </c>
       <c r="E81" s="1" t="s">
         <v>5</v>
@@ -2913,17 +2927,15 @@
         <v>80</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>143</v>
+        <v>318</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>144</v>
+        <v>319</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F82" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F82" s="1"/>
       <c r="G82" s="1"/>
     </row>
     <row r="83" spans="2:7">
@@ -2931,10 +2943,10 @@
         <v>81</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="E83" s="1" t="s">
         <v>5</v>
@@ -2947,15 +2959,17 @@
         <v>82</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F84" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="G84" s="1"/>
     </row>
     <row r="85" spans="2:7">
@@ -2963,10 +2977,10 @@
         <v>83</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>310</v>
+        <v>326</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>311</v>
+        <v>327</v>
       </c>
       <c r="E85" s="1" t="s">
         <v>5</v>
@@ -2979,10 +2993,10 @@
         <v>84</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E86" s="1" t="s">
         <v>5</v>
@@ -2995,10 +3009,10 @@
         <v>85</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>149</v>
+        <v>310</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>150</v>
+        <v>311</v>
       </c>
       <c r="E87" s="1" t="s">
         <v>5</v>
@@ -3011,17 +3025,15 @@
         <v>86</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F88" s="1" t="s">
-        <v>27</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F88" s="1"/>
       <c r="G88" s="1"/>
     </row>
     <row r="89" spans="2:7">
@@ -3029,17 +3041,15 @@
         <v>87</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F89" s="1" t="s">
-        <v>27</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F89" s="1"/>
       <c r="G89" s="1"/>
     </row>
     <row r="90" spans="2:7">
@@ -3047,16 +3057,16 @@
         <v>88</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E90" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="G90" s="1"/>
     </row>
@@ -3065,15 +3075,17 @@
         <v>89</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F91" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F91" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G91" s="1"/>
     </row>
     <row r="92" spans="2:7">
@@ -3081,15 +3093,17 @@
         <v>90</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F92" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F92" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="G92" s="1"/>
     </row>
     <row r="93" spans="2:7">
@@ -3097,10 +3111,10 @@
         <v>91</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="E93" s="1" t="s">
         <v>5</v>
@@ -3113,13 +3127,13 @@
         <v>92</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F94" s="1"/>
       <c r="G94" s="1"/>
@@ -3129,10 +3143,10 @@
         <v>93</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>332</v>
+        <v>161</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>333</v>
+        <v>162</v>
       </c>
       <c r="E95" s="1" t="s">
         <v>5</v>
@@ -3145,10 +3159,10 @@
         <v>94</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>328</v>
+        <v>163</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>331</v>
+        <v>164</v>
       </c>
       <c r="E96" s="1" t="s">
         <v>5</v>
@@ -3161,17 +3175,15 @@
         <v>95</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>320</v>
+        <v>332</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>321</v>
+        <v>333</v>
       </c>
       <c r="E97" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F97" s="1" t="s">
-        <v>27</v>
-      </c>
+      <c r="F97" s="1"/>
       <c r="G97" s="1"/>
     </row>
     <row r="98" spans="2:7">
@@ -3179,10 +3191,10 @@
         <v>96</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>315</v>
+        <v>328</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>314</v>
+        <v>331</v>
       </c>
       <c r="E98" s="1" t="s">
         <v>5</v>
@@ -3195,15 +3207,17 @@
         <v>97</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>312</v>
+        <v>320</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>313</v>
+        <v>321</v>
       </c>
       <c r="E99" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F99" s="1"/>
+      <c r="F99" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G99" s="1"/>
     </row>
     <row r="100" spans="2:7">
@@ -3211,10 +3225,10 @@
         <v>98</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>165</v>
+        <v>315</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>166</v>
+        <v>314</v>
       </c>
       <c r="E100" s="1" t="s">
         <v>5</v>
@@ -3227,10 +3241,10 @@
         <v>99</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>167</v>
+        <v>312</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>168</v>
+        <v>313</v>
       </c>
       <c r="E101" s="1" t="s">
         <v>5</v>
@@ -3243,10 +3257,10 @@
         <v>100</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="E102" s="1" t="s">
         <v>5</v>
@@ -3259,10 +3273,10 @@
         <v>101</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="E103" s="1" t="s">
         <v>5</v>
@@ -3275,10 +3289,10 @@
         <v>102</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="E104" s="1" t="s">
         <v>5</v>
@@ -3291,10 +3305,10 @@
         <v>103</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>340</v>
+        <v>171</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E105" s="1" t="s">
         <v>5</v>
@@ -3307,10 +3321,10 @@
         <v>104</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E106" s="1" t="s">
         <v>5</v>
@@ -3323,17 +3337,15 @@
         <v>105</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>178</v>
+        <v>340</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F107" s="1" t="s">
-        <v>27</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F107" s="1"/>
       <c r="G107" s="1"/>
     </row>
     <row r="108" spans="2:7">
@@ -3341,10 +3353,10 @@
         <v>106</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="E108" s="1" t="s">
         <v>5</v>
@@ -3357,15 +3369,17 @@
         <v>107</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F109" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F109" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G109" s="1"/>
     </row>
     <row r="110" spans="2:7">
@@ -3373,10 +3387,10 @@
         <v>108</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="E110" s="1" t="s">
         <v>5</v>
@@ -3389,10 +3403,10 @@
         <v>109</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="E111" s="1" t="s">
         <v>5</v>
@@ -3405,10 +3419,10 @@
         <v>110</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E112" s="1" t="s">
         <v>5</v>
@@ -3421,10 +3435,10 @@
         <v>111</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E113" s="1" t="s">
         <v>5</v>
@@ -3437,10 +3451,10 @@
         <v>112</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="E114" s="1" t="s">
         <v>5</v>
@@ -3453,10 +3467,10 @@
         <v>113</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>341</v>
+        <v>190</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>342</v>
+        <v>191</v>
       </c>
       <c r="E115" s="1" t="s">
         <v>5</v>
@@ -3469,10 +3483,10 @@
         <v>114</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E116" s="1" t="s">
         <v>5</v>
@@ -3485,10 +3499,10 @@
         <v>115</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="E117" s="1" t="s">
         <v>5</v>
@@ -3501,17 +3515,15 @@
         <v>116</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F118" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F118" s="1"/>
       <c r="G118" s="1"/>
     </row>
     <row r="119" spans="2:7">
@@ -3519,10 +3531,10 @@
         <v>117</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>198</v>
+        <v>338</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>199</v>
+        <v>339</v>
       </c>
       <c r="E119" s="1" t="s">
         <v>5</v>
@@ -3535,15 +3547,17 @@
         <v>118</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F120" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F120" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="G120" s="1"/>
     </row>
     <row r="121" spans="2:7">
@@ -3551,10 +3565,10 @@
         <v>119</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>352</v>
+        <v>198</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>351</v>
+        <v>199</v>
       </c>
       <c r="E121" s="1" t="s">
         <v>5</v>
@@ -3567,10 +3581,10 @@
         <v>120</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E122" s="1" t="s">
         <v>5</v>
@@ -3583,10 +3597,10 @@
         <v>121</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>204</v>
+        <v>352</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>205</v>
+        <v>351</v>
       </c>
       <c r="E123" s="1" t="s">
         <v>5</v>
@@ -3599,13 +3613,13 @@
         <v>122</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F124" s="1"/>
       <c r="G124" s="1"/>
@@ -3615,10 +3629,10 @@
         <v>123</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="E125" s="1" t="s">
         <v>5</v>
@@ -3631,13 +3645,13 @@
         <v>124</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F126" s="1"/>
       <c r="G126" s="1"/>
@@ -3647,10 +3661,10 @@
         <v>125</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="E127" s="1" t="s">
         <v>5</v>
@@ -3663,17 +3677,15 @@
         <v>126</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="E128" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F128" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F128" s="1"/>
       <c r="G128" s="1"/>
     </row>
     <row r="129" spans="2:7">
@@ -3681,10 +3693,10 @@
         <v>127</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="E129" s="1" t="s">
         <v>5</v>
@@ -3697,15 +3709,17 @@
         <v>128</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="E130" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F130" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F130" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="G130" s="1"/>
     </row>
     <row r="131" spans="2:7">
@@ -3713,17 +3727,15 @@
         <v>129</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="E131" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F131" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F131" s="1"/>
       <c r="G131" s="1"/>
     </row>
     <row r="132" spans="2:7">
@@ -3731,50 +3743,44 @@
         <v>130</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="E132" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F132" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G132" s="1" t="s">
-        <v>30</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F132" s="1"/>
+      <c r="G132" s="1"/>
     </row>
     <row r="133" spans="2:7">
       <c r="B133" s="6">
         <v>131</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="E133" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F133" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G133" s="1" t="s">
-        <v>30</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="G133" s="1"/>
     </row>
     <row r="134" spans="2:7">
       <c r="B134" s="6">
         <v>132</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="E134" s="1" t="s">
         <v>7</v>
@@ -3783,7 +3789,7 @@
         <v>27</v>
       </c>
       <c r="G134" s="1" t="s">
-        <v>301</v>
+        <v>30</v>
       </c>
     </row>
     <row r="135" spans="2:7">
@@ -3791,10 +3797,10 @@
         <v>133</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="E135" s="1" t="s">
         <v>7</v>
@@ -3802,38 +3808,46 @@
       <c r="F135" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G135" s="1"/>
+      <c r="G135" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="136" spans="2:7">
       <c r="B136" s="6">
         <v>134</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E136" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F136" s="1"/>
-      <c r="G136" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F136" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G136" s="1" t="s">
+        <v>301</v>
+      </c>
     </row>
     <row r="137" spans="2:7">
       <c r="B137" s="6">
         <v>135</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="E137" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F137" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F137" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G137" s="1"/>
     </row>
     <row r="138" spans="2:7">
@@ -3841,17 +3855,15 @@
         <v>136</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="E138" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F138" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F138" s="1"/>
       <c r="G138" s="1"/>
     </row>
     <row r="139" spans="2:7">
@@ -3859,17 +3871,15 @@
         <v>137</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="E139" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F139" s="1" t="s">
-        <v>27</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F139" s="1"/>
       <c r="G139" s="1"/>
     </row>
     <row r="140" spans="2:7">
@@ -3877,15 +3887,17 @@
         <v>138</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="E140" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F140" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F140" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="G140" s="1"/>
     </row>
     <row r="141" spans="2:7">
@@ -3893,15 +3905,17 @@
         <v>139</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="E141" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F141" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F141" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G141" s="1"/>
     </row>
     <row r="142" spans="2:7">
@@ -3909,10 +3923,10 @@
         <v>140</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="E142" s="1" t="s">
         <v>5</v>
@@ -3925,10 +3939,10 @@
         <v>141</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="E143" s="1" t="s">
         <v>5</v>
@@ -3941,17 +3955,15 @@
         <v>142</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="E144" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F144" s="1" t="s">
-        <v>27</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F144" s="1"/>
       <c r="G144" s="1"/>
     </row>
     <row r="145" spans="2:7">
@@ -3959,13 +3971,13 @@
         <v>143</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="E145" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F145" s="1"/>
       <c r="G145" s="1"/>
@@ -3975,15 +3987,17 @@
         <v>144</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="E146" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F146" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F146" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G146" s="1"/>
     </row>
     <row r="147" spans="2:7">
@@ -3991,13 +4005,13 @@
         <v>145</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="E147" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F147" s="1"/>
       <c r="G147" s="1"/>
@@ -4007,10 +4021,10 @@
         <v>146</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="E148" s="1" t="s">
         <v>5</v>
@@ -4023,10 +4037,10 @@
         <v>147</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="E149" s="1" t="s">
         <v>5</v>
@@ -4039,10 +4053,10 @@
         <v>148</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="E150" s="1" t="s">
         <v>5</v>
@@ -4055,10 +4069,10 @@
         <v>149</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="E151" s="1" t="s">
         <v>5</v>
@@ -4071,17 +4085,15 @@
         <v>150</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="E152" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F152" s="1" t="s">
-        <v>27</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F152" s="1"/>
       <c r="G152" s="1"/>
     </row>
     <row r="153" spans="2:7">
@@ -4089,10 +4101,10 @@
         <v>151</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="E153" s="1" t="s">
         <v>5</v>
@@ -4105,15 +4117,17 @@
         <v>152</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="E154" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F154" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F154" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G154" s="1"/>
     </row>
     <row r="155" spans="2:7">
@@ -4121,17 +4135,15 @@
         <v>153</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="D155" s="1" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="E155" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F155" s="1" t="s">
-        <v>27</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F155" s="1"/>
       <c r="G155" s="1"/>
     </row>
     <row r="156" spans="2:7">
@@ -4139,10 +4151,10 @@
         <v>154</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="E156" s="1" t="s">
         <v>5</v>
@@ -4155,15 +4167,17 @@
         <v>155</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="E157" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F157" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F157" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G157" s="1"/>
     </row>
     <row r="158" spans="2:7">
@@ -4171,10 +4185,10 @@
         <v>156</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="D158" s="1" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="E158" s="1" t="s">
         <v>5</v>
@@ -4187,10 +4201,10 @@
         <v>157</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="E159" s="1" t="s">
         <v>5</v>
@@ -4203,10 +4217,10 @@
         <v>158</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="D160" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="E160" s="1" t="s">
         <v>5</v>
@@ -4219,10 +4233,10 @@
         <v>159</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>10</v>
+        <v>276</v>
       </c>
       <c r="D161" s="1" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="E161" s="1" t="s">
         <v>5</v>
@@ -4235,13 +4249,13 @@
         <v>160</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>329</v>
+        <v>278</v>
       </c>
       <c r="D162" s="1" t="s">
-        <v>330</v>
+        <v>279</v>
       </c>
       <c r="E162" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F162" s="1"/>
       <c r="G162" s="1"/>
@@ -4251,17 +4265,15 @@
         <v>161</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>281</v>
+        <v>10</v>
       </c>
       <c r="D163" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E163" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F163" s="1" t="s">
-        <v>27</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F163" s="1"/>
       <c r="G163" s="1"/>
     </row>
     <row r="164" spans="2:7">
@@ -4269,13 +4281,13 @@
         <v>162</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>283</v>
+        <v>329</v>
       </c>
       <c r="D164" s="1" t="s">
-        <v>284</v>
+        <v>330</v>
       </c>
       <c r="E164" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F164" s="1"/>
       <c r="G164" s="1"/>
@@ -4285,15 +4297,17 @@
         <v>163</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="D165" s="1" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="E165" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F165" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F165" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G165" s="1"/>
     </row>
     <row r="166" spans="2:7">
@@ -4301,17 +4315,15 @@
         <v>164</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="D166" s="1" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="E166" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F166" s="1" t="s">
-        <v>27</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F166" s="1"/>
       <c r="G166" s="1"/>
     </row>
     <row r="167" spans="2:7">
@@ -4319,17 +4331,15 @@
         <v>165</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="D167" s="1" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="E167" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F167" s="1" t="s">
-        <v>27</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="F167" s="1"/>
       <c r="G167" s="1"/>
     </row>
     <row r="168" spans="2:7">
@@ -4337,10 +4347,10 @@
         <v>166</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D168" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="E168" s="1" t="s">
         <v>7</v>
@@ -4355,15 +4365,17 @@
         <v>167</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="D169" s="1" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="E169" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F169" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F169" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G169" s="1"/>
     </row>
     <row r="170" spans="2:7">
@@ -4371,10 +4383,10 @@
         <v>168</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="D170" s="1" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="E170" s="1" t="s">
         <v>7</v>
@@ -4389,10 +4401,10 @@
         <v>169</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="D171" s="1" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="E171" s="1" t="s">
         <v>5</v>
@@ -4405,30 +4417,48 @@
         <v>170</v>
       </c>
       <c r="C172" s="1" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="D172" s="1" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="E172" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F172" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F172" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G172" s="1"/>
     </row>
     <row r="173" spans="2:7">
-      <c r="B173" s="6"/>
-      <c r="C173" s="1"/>
-      <c r="D173" s="1"/>
-      <c r="E173" s="1"/>
+      <c r="B173" s="6">
+        <v>171</v>
+      </c>
+      <c r="C173" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="D173" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="E173" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F173" s="1"/>
       <c r="G173" s="1"/>
     </row>
     <row r="174" spans="2:7">
-      <c r="B174" s="6"/>
-      <c r="C174" s="1"/>
-      <c r="D174" s="1"/>
-      <c r="E174" s="1"/>
+      <c r="B174" s="6">
+        <v>172</v>
+      </c>
+      <c r="C174" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="D174" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="E174" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F174" s="1"/>
       <c r="G174" s="1"/>
     </row>
@@ -4448,12 +4478,28 @@
       <c r="F176" s="1"/>
       <c r="G176" s="1"/>
     </row>
+    <row r="177" spans="2:7">
+      <c r="B177" s="6"/>
+      <c r="C177" s="1"/>
+      <c r="D177" s="1"/>
+      <c r="E177" s="1"/>
+      <c r="F177" s="1"/>
+      <c r="G177" s="1"/>
+    </row>
+    <row r="178" spans="2:7">
+      <c r="B178" s="6"/>
+      <c r="C178" s="1"/>
+      <c r="D178" s="1"/>
+      <c r="E178" s="1"/>
+      <c r="F178" s="1"/>
+      <c r="G178" s="1"/>
+    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E172" xr:uid="{7E8CE32C-29D1-4006-9E0F-69B72A0F4378}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E174" xr:uid="{7E8CE32C-29D1-4006-9E0F-69B72A0F4378}">
       <formula1>"[Application],[Directory],[Script]"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F176" xr:uid="{A5D947FB-5606-4B36-88C5-81CC2B61C636}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F178" xr:uid="{A5D947FB-5606-4B36-88C5-81CC2B61C636}">
       <formula1>"[bat],[vbs]"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Repo Update: 2024-08-11 11:02:04
</commit_message>
<xml_diff>
--- a/Database/Run_shortcut_creator_aliases.xlsx
+++ b/Database/Run_shortcut_creator_aliases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\player-1\Documents\Windows-Git-Repos\win-t\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AA3D8C1-8FEB-4BCD-9AC1-F157E790BE68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6768F076-7955-47DC-BD87-6BDBA39326BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13215" yWindow="0" windowWidth="15705" windowHeight="15585" xr2:uid="{D65865D6-BB34-410C-8183-31ED199784FF}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14625" windowHeight="15585" xr2:uid="{D65865D6-BB34-410C-8183-31ED199784FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Run Shortcut Creator Aliases" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="359">
   <si>
     <t>Number</t>
   </si>
@@ -1129,6 +1129,12 @@
   </si>
   <si>
     <t>Antidote</t>
+  </si>
+  <si>
+    <t>ug</t>
+  </si>
+  <si>
+    <t>UnigetUI</t>
   </si>
 </sst>
 </file>
@@ -1560,10 +1566,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58A033C2-67FB-408D-B72B-8C45836FCF74}">
-  <dimension ref="B2:G178"/>
+  <dimension ref="B2:G179"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B164" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
-      <selection activeCell="D143" sqref="D143"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B133" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
+      <selection activeCell="C157" sqref="C157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21"/>
@@ -1599,7 +1605,7 @@
     </row>
     <row r="3" spans="2:7" ht="24.95" customHeight="1">
       <c r="B3" s="6" cm="1">
-        <f t="array" ref="B3:B174">_xlfn.SEQUENCE(COUNTA(C:C)-1)</f>
+        <f t="array" ref="B3:B175">_xlfn.SEQUENCE(COUNTA(C:C)-1)</f>
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -4085,10 +4091,10 @@
         <v>150</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>258</v>
+        <v>358</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>259</v>
+        <v>357</v>
       </c>
       <c r="E152" s="1" t="s">
         <v>5</v>
@@ -4101,10 +4107,10 @@
         <v>151</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="E153" s="1" t="s">
         <v>5</v>
@@ -4117,17 +4123,15 @@
         <v>152</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="E154" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F154" s="1" t="s">
-        <v>27</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F154" s="1"/>
       <c r="G154" s="1"/>
     </row>
     <row r="155" spans="2:7">
@@ -4135,15 +4139,17 @@
         <v>153</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D155" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="E155" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F155" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F155" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G155" s="1"/>
     </row>
     <row r="156" spans="2:7">
@@ -4151,10 +4157,10 @@
         <v>154</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="E156" s="1" t="s">
         <v>5</v>
@@ -4167,17 +4173,15 @@
         <v>155</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E157" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F157" s="1" t="s">
-        <v>27</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F157" s="1"/>
       <c r="G157" s="1"/>
     </row>
     <row r="158" spans="2:7">
@@ -4185,15 +4189,17 @@
         <v>156</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D158" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="E158" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F158" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F158" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G158" s="1"/>
     </row>
     <row r="159" spans="2:7">
@@ -4201,10 +4207,10 @@
         <v>157</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E159" s="1" t="s">
         <v>5</v>
@@ -4217,10 +4223,10 @@
         <v>158</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D160" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="E160" s="1" t="s">
         <v>5</v>
@@ -4233,10 +4239,10 @@
         <v>159</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D161" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E161" s="1" t="s">
         <v>5</v>
@@ -4249,10 +4255,10 @@
         <v>160</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D162" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="E162" s="1" t="s">
         <v>5</v>
@@ -4265,10 +4271,10 @@
         <v>161</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>10</v>
+        <v>278</v>
       </c>
       <c r="D163" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E163" s="1" t="s">
         <v>5</v>
@@ -4281,13 +4287,13 @@
         <v>162</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>329</v>
+        <v>10</v>
       </c>
       <c r="D164" s="1" t="s">
-        <v>330</v>
+        <v>280</v>
       </c>
       <c r="E164" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F164" s="1"/>
       <c r="G164" s="1"/>
@@ -4297,17 +4303,15 @@
         <v>163</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>281</v>
+        <v>329</v>
       </c>
       <c r="D165" s="1" t="s">
-        <v>282</v>
+        <v>330</v>
       </c>
       <c r="E165" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F165" s="1" t="s">
-        <v>27</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="F165" s="1"/>
       <c r="G165" s="1"/>
     </row>
     <row r="166" spans="2:7">
@@ -4315,15 +4319,17 @@
         <v>164</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D166" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="E166" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F166" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F166" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G166" s="1"/>
     </row>
     <row r="167" spans="2:7">
@@ -4331,13 +4337,13 @@
         <v>165</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D167" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E167" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F167" s="1"/>
       <c r="G167" s="1"/>
@@ -4347,17 +4353,15 @@
         <v>166</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D168" s="1" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="E168" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F168" s="1" t="s">
-        <v>27</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="F168" s="1"/>
       <c r="G168" s="1"/>
     </row>
     <row r="169" spans="2:7">
@@ -4365,10 +4369,10 @@
         <v>167</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D169" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E169" s="1" t="s">
         <v>7</v>
@@ -4383,10 +4387,10 @@
         <v>168</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D170" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E170" s="1" t="s">
         <v>7</v>
@@ -4401,15 +4405,17 @@
         <v>169</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="D171" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="E171" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F171" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F171" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G171" s="1"/>
     </row>
     <row r="172" spans="2:7">
@@ -4417,17 +4423,15 @@
         <v>170</v>
       </c>
       <c r="C172" s="1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="D172" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="E172" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F172" s="1" t="s">
-        <v>27</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F172" s="1"/>
       <c r="G172" s="1"/>
     </row>
     <row r="173" spans="2:7">
@@ -4435,15 +4439,17 @@
         <v>171</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D173" s="1" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="E173" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F173" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F173" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G173" s="1"/>
     </row>
     <row r="174" spans="2:7">
@@ -4451,10 +4457,10 @@
         <v>172</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D174" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="E174" s="1" t="s">
         <v>5</v>
@@ -4463,10 +4469,18 @@
       <c r="G174" s="1"/>
     </row>
     <row r="175" spans="2:7">
-      <c r="B175" s="6"/>
-      <c r="C175" s="1"/>
-      <c r="D175" s="1"/>
-      <c r="E175" s="1"/>
+      <c r="B175" s="6">
+        <v>173</v>
+      </c>
+      <c r="C175" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="D175" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="E175" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F175" s="1"/>
       <c r="G175" s="1"/>
     </row>
@@ -4494,12 +4508,20 @@
       <c r="F178" s="1"/>
       <c r="G178" s="1"/>
     </row>
+    <row r="179" spans="2:7">
+      <c r="B179" s="6"/>
+      <c r="C179" s="1"/>
+      <c r="D179" s="1"/>
+      <c r="E179" s="1"/>
+      <c r="F179" s="1"/>
+      <c r="G179" s="1"/>
+    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E174" xr:uid="{7E8CE32C-29D1-4006-9E0F-69B72A0F4378}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E175" xr:uid="{7E8CE32C-29D1-4006-9E0F-69B72A0F4378}">
       <formula1>"[Application],[Directory],[Script]"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F178" xr:uid="{A5D947FB-5606-4B36-88C5-81CC2B61C636}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F179" xr:uid="{A5D947FB-5606-4B36-88C5-81CC2B61C636}">
       <formula1>"[bat],[vbs]"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
update Run Shurtuct Creator Configs
</commit_message>
<xml_diff>
--- a/Database/Run_shortcut_creator_aliases.xlsx
+++ b/Database/Run_shortcut_creator_aliases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\player-1\Documents\Windows-Git-Repos\win-t\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6768F076-7955-47DC-BD87-6BDBA39326BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7867E72-AA4E-4961-AFB8-1673C5DE736F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14295" yWindow="0" windowWidth="14625" windowHeight="15585" xr2:uid="{D65865D6-BB34-410C-8183-31ED199784FF}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="359">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="365">
   <si>
     <t>Number</t>
   </si>
@@ -1135,6 +1135,24 @@
   </si>
   <si>
     <t>UnigetUI</t>
+  </si>
+  <si>
+    <t>Hymns</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>Kill Hymns</t>
+  </si>
+  <si>
+    <t>kh</t>
+  </si>
+  <si>
+    <t>Sunday Data</t>
+  </si>
+  <si>
+    <t>sd</t>
   </si>
 </sst>
 </file>
@@ -1566,10 +1584,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58A033C2-67FB-408D-B72B-8C45836FCF74}">
-  <dimension ref="B2:G179"/>
+  <dimension ref="B2:G182"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B133" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
-      <selection activeCell="C157" sqref="C157"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A160" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
+      <selection activeCell="C134" sqref="C134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21"/>
@@ -1605,7 +1623,7 @@
     </row>
     <row r="3" spans="2:7" ht="24.95" customHeight="1">
       <c r="B3" s="6" cm="1">
-        <f t="array" ref="B3:B175">_xlfn.SEQUENCE(COUNTA(C:C)-1)</f>
+        <f t="array" ref="B3:B178">_xlfn.SEQUENCE(COUNTA(C:C)-1)</f>
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -2633,17 +2651,15 @@
         <v>62</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>111</v>
+        <v>359</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>112</v>
+        <v>360</v>
       </c>
       <c r="E64" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F64" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="F64" s="1"/>
       <c r="G64" s="1"/>
     </row>
     <row r="65" spans="2:7">
@@ -2651,10 +2667,10 @@
         <v>63</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E65" s="1" t="s">
         <v>7</v>
@@ -2669,15 +2685,17 @@
         <v>64</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>345</v>
+        <v>113</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>346</v>
+        <v>114</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F66" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="G66" s="1"/>
     </row>
     <row r="67" spans="2:7">
@@ -2685,13 +2703,13 @@
         <v>65</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>115</v>
+        <v>345</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>116</v>
+        <v>346</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F67" s="1"/>
       <c r="G67" s="1"/>
@@ -2701,17 +2719,15 @@
         <v>66</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F68" s="1" t="s">
-        <v>27</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F68" s="1"/>
       <c r="G68" s="1"/>
     </row>
     <row r="69" spans="2:7">
@@ -2719,15 +2735,17 @@
         <v>67</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F69" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G69" s="1"/>
     </row>
     <row r="70" spans="2:7">
@@ -2735,10 +2753,10 @@
         <v>68</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E70" s="1" t="s">
         <v>5</v>
@@ -2751,10 +2769,10 @@
         <v>69</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E71" s="1" t="s">
         <v>5</v>
@@ -2767,10 +2785,10 @@
         <v>70</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E72" s="1" t="s">
         <v>5</v>
@@ -2783,10 +2801,10 @@
         <v>71</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E73" s="1" t="s">
         <v>5</v>
@@ -2799,10 +2817,10 @@
         <v>72</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E74" s="1" t="s">
         <v>5</v>
@@ -2815,10 +2833,10 @@
         <v>73</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E75" s="1" t="s">
         <v>5</v>
@@ -2831,17 +2849,15 @@
         <v>74</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>354</v>
+        <v>131</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>353</v>
+        <v>132</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F76" s="1" t="s">
-        <v>27</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F76" s="1"/>
       <c r="G76" s="1"/>
     </row>
     <row r="77" spans="2:7">
@@ -2849,15 +2865,17 @@
         <v>75</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>133</v>
+        <v>354</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>134</v>
+        <v>353</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F77" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G77" s="1"/>
     </row>
     <row r="78" spans="2:7">
@@ -2865,17 +2883,15 @@
         <v>76</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F78" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F78" s="1"/>
       <c r="G78" s="1"/>
     </row>
     <row r="79" spans="2:7">
@@ -2883,15 +2899,17 @@
         <v>77</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F79" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="G79" s="1"/>
     </row>
     <row r="80" spans="2:7">
@@ -2899,17 +2917,15 @@
         <v>78</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F80" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F80" s="1"/>
       <c r="G80" s="1"/>
     </row>
     <row r="81" spans="2:7">
@@ -2917,15 +2933,17 @@
         <v>79</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F81" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="G81" s="1"/>
     </row>
     <row r="82" spans="2:7">
@@ -2933,13 +2951,13 @@
         <v>80</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>318</v>
+        <v>361</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>319</v>
+        <v>362</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F82" s="1"/>
       <c r="G82" s="1"/>
@@ -2949,10 +2967,10 @@
         <v>81</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>324</v>
+        <v>141</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>325</v>
+        <v>142</v>
       </c>
       <c r="E83" s="1" t="s">
         <v>5</v>
@@ -2965,17 +2983,15 @@
         <v>82</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>143</v>
+        <v>318</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>144</v>
+        <v>319</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F84" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F84" s="1"/>
       <c r="G84" s="1"/>
     </row>
     <row r="85" spans="2:7">
@@ -2983,10 +2999,10 @@
         <v>83</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="E85" s="1" t="s">
         <v>5</v>
@@ -2999,15 +3015,17 @@
         <v>84</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F86" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F86" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="G86" s="1"/>
     </row>
     <row r="87" spans="2:7">
@@ -3015,10 +3033,10 @@
         <v>85</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>310</v>
+        <v>326</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>311</v>
+        <v>327</v>
       </c>
       <c r="E87" s="1" t="s">
         <v>5</v>
@@ -3031,10 +3049,10 @@
         <v>86</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E88" s="1" t="s">
         <v>5</v>
@@ -3047,10 +3065,10 @@
         <v>87</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>149</v>
+        <v>310</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>150</v>
+        <v>311</v>
       </c>
       <c r="E89" s="1" t="s">
         <v>5</v>
@@ -3063,17 +3081,15 @@
         <v>88</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F90" s="1" t="s">
-        <v>27</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F90" s="1"/>
       <c r="G90" s="1"/>
     </row>
     <row r="91" spans="2:7">
@@ -3081,17 +3097,15 @@
         <v>89</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F91" s="1" t="s">
-        <v>27</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F91" s="1"/>
       <c r="G91" s="1"/>
     </row>
     <row r="92" spans="2:7">
@@ -3099,16 +3113,16 @@
         <v>90</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E92" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="G92" s="1"/>
     </row>
@@ -3117,15 +3131,17 @@
         <v>91</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F93" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F93" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G93" s="1"/>
     </row>
     <row r="94" spans="2:7">
@@ -3133,15 +3149,17 @@
         <v>92</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F94" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F94" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="G94" s="1"/>
     </row>
     <row r="95" spans="2:7">
@@ -3149,10 +3167,10 @@
         <v>93</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="E95" s="1" t="s">
         <v>5</v>
@@ -3165,13 +3183,13 @@
         <v>94</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F96" s="1"/>
       <c r="G96" s="1"/>
@@ -3181,10 +3199,10 @@
         <v>95</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>332</v>
+        <v>161</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>333</v>
+        <v>162</v>
       </c>
       <c r="E97" s="1" t="s">
         <v>5</v>
@@ -3197,10 +3215,10 @@
         <v>96</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>328</v>
+        <v>163</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>331</v>
+        <v>164</v>
       </c>
       <c r="E98" s="1" t="s">
         <v>5</v>
@@ -3213,17 +3231,15 @@
         <v>97</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>320</v>
+        <v>332</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>321</v>
+        <v>333</v>
       </c>
       <c r="E99" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F99" s="1" t="s">
-        <v>27</v>
-      </c>
+      <c r="F99" s="1"/>
       <c r="G99" s="1"/>
     </row>
     <row r="100" spans="2:7">
@@ -3231,10 +3247,10 @@
         <v>98</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>315</v>
+        <v>328</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>314</v>
+        <v>331</v>
       </c>
       <c r="E100" s="1" t="s">
         <v>5</v>
@@ -3247,15 +3263,17 @@
         <v>99</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>312</v>
+        <v>320</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>313</v>
+        <v>321</v>
       </c>
       <c r="E101" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F101" s="1"/>
+      <c r="F101" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G101" s="1"/>
     </row>
     <row r="102" spans="2:7">
@@ -3263,10 +3281,10 @@
         <v>100</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>165</v>
+        <v>315</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>166</v>
+        <v>314</v>
       </c>
       <c r="E102" s="1" t="s">
         <v>5</v>
@@ -3279,10 +3297,10 @@
         <v>101</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>167</v>
+        <v>312</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>168</v>
+        <v>313</v>
       </c>
       <c r="E103" s="1" t="s">
         <v>5</v>
@@ -3295,10 +3313,10 @@
         <v>102</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="E104" s="1" t="s">
         <v>5</v>
@@ -3311,10 +3329,10 @@
         <v>103</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="E105" s="1" t="s">
         <v>5</v>
@@ -3327,10 +3345,10 @@
         <v>104</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="E106" s="1" t="s">
         <v>5</v>
@@ -3343,10 +3361,10 @@
         <v>105</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>340</v>
+        <v>171</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E107" s="1" t="s">
         <v>5</v>
@@ -3359,10 +3377,10 @@
         <v>106</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E108" s="1" t="s">
         <v>5</v>
@@ -3375,17 +3393,15 @@
         <v>107</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>178</v>
+        <v>340</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F109" s="1" t="s">
-        <v>27</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F109" s="1"/>
       <c r="G109" s="1"/>
     </row>
     <row r="110" spans="2:7">
@@ -3393,10 +3409,10 @@
         <v>108</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="E110" s="1" t="s">
         <v>5</v>
@@ -3409,15 +3425,17 @@
         <v>109</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F111" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F111" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G111" s="1"/>
     </row>
     <row r="112" spans="2:7">
@@ -3425,10 +3443,10 @@
         <v>110</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="E112" s="1" t="s">
         <v>5</v>
@@ -3441,10 +3459,10 @@
         <v>111</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="E113" s="1" t="s">
         <v>5</v>
@@ -3457,10 +3475,10 @@
         <v>112</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E114" s="1" t="s">
         <v>5</v>
@@ -3473,10 +3491,10 @@
         <v>113</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E115" s="1" t="s">
         <v>5</v>
@@ -3489,10 +3507,10 @@
         <v>114</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="E116" s="1" t="s">
         <v>5</v>
@@ -3505,10 +3523,10 @@
         <v>115</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>341</v>
+        <v>190</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>342</v>
+        <v>191</v>
       </c>
       <c r="E117" s="1" t="s">
         <v>5</v>
@@ -3521,10 +3539,10 @@
         <v>116</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E118" s="1" t="s">
         <v>5</v>
@@ -3537,10 +3555,10 @@
         <v>117</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="E119" s="1" t="s">
         <v>5</v>
@@ -3553,17 +3571,15 @@
         <v>118</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F120" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F120" s="1"/>
       <c r="G120" s="1"/>
     </row>
     <row r="121" spans="2:7">
@@ -3571,10 +3587,10 @@
         <v>119</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>198</v>
+        <v>338</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>199</v>
+        <v>339</v>
       </c>
       <c r="E121" s="1" t="s">
         <v>5</v>
@@ -3587,15 +3603,17 @@
         <v>120</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F122" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F122" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="G122" s="1"/>
     </row>
     <row r="123" spans="2:7">
@@ -3603,10 +3621,10 @@
         <v>121</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>352</v>
+        <v>198</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>351</v>
+        <v>199</v>
       </c>
       <c r="E123" s="1" t="s">
         <v>5</v>
@@ -3619,10 +3637,10 @@
         <v>122</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E124" s="1" t="s">
         <v>5</v>
@@ -3635,10 +3653,10 @@
         <v>123</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>204</v>
+        <v>352</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>205</v>
+        <v>351</v>
       </c>
       <c r="E125" s="1" t="s">
         <v>5</v>
@@ -3651,13 +3669,13 @@
         <v>124</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F126" s="1"/>
       <c r="G126" s="1"/>
@@ -3667,10 +3685,10 @@
         <v>125</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="E127" s="1" t="s">
         <v>5</v>
@@ -3683,13 +3701,13 @@
         <v>126</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E128" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F128" s="1"/>
       <c r="G128" s="1"/>
@@ -3699,13 +3717,13 @@
         <v>127</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>212</v>
+        <v>363</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>213</v>
+        <v>364</v>
       </c>
       <c r="E129" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F129" s="1"/>
       <c r="G129" s="1"/>
@@ -3715,17 +3733,15 @@
         <v>128</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="E130" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F130" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F130" s="1"/>
       <c r="G130" s="1"/>
     </row>
     <row r="131" spans="2:7">
@@ -3733,10 +3749,10 @@
         <v>129</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="E131" s="1" t="s">
         <v>5</v>
@@ -3749,10 +3765,10 @@
         <v>130</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="E132" s="1" t="s">
         <v>5</v>
@@ -3765,10 +3781,10 @@
         <v>131</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="E133" s="1" t="s">
         <v>7</v>
@@ -3783,70 +3799,60 @@
         <v>132</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="E134" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F134" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G134" s="1" t="s">
-        <v>30</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F134" s="1"/>
+      <c r="G134" s="1"/>
     </row>
     <row r="135" spans="2:7">
       <c r="B135" s="6">
         <v>133</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="E135" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F135" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G135" s="1" t="s">
-        <v>30</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F135" s="1"/>
+      <c r="G135" s="1"/>
     </row>
     <row r="136" spans="2:7">
       <c r="B136" s="6">
         <v>134</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="E136" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F136" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G136" s="1" t="s">
-        <v>301</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="G136" s="1"/>
     </row>
     <row r="137" spans="2:7">
       <c r="B137" s="6">
         <v>135</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="E137" s="1" t="s">
         <v>7</v>
@@ -3854,55 +3860,65 @@
       <c r="F137" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G137" s="1"/>
+      <c r="G137" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="138" spans="2:7">
       <c r="B138" s="6">
         <v>136</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="E138" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F138" s="1"/>
-      <c r="G138" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F138" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G138" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="139" spans="2:7">
       <c r="B139" s="6">
         <v>137</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="E139" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F139" s="1"/>
-      <c r="G139" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F139" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G139" s="1" t="s">
+        <v>301</v>
+      </c>
     </row>
     <row r="140" spans="2:7">
       <c r="B140" s="6">
         <v>138</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="E140" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F140" s="1" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="G140" s="1"/>
     </row>
@@ -3911,17 +3927,15 @@
         <v>139</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="E141" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F141" s="1" t="s">
-        <v>27</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F141" s="1"/>
       <c r="G141" s="1"/>
     </row>
     <row r="142" spans="2:7">
@@ -3929,10 +3943,10 @@
         <v>140</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="E142" s="1" t="s">
         <v>5</v>
@@ -3945,15 +3959,17 @@
         <v>141</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="E143" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F143" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F143" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="G143" s="1"/>
     </row>
     <row r="144" spans="2:7">
@@ -3961,15 +3977,17 @@
         <v>142</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="E144" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F144" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F144" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G144" s="1"/>
     </row>
     <row r="145" spans="2:7">
@@ -3977,10 +3995,10 @@
         <v>143</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="E145" s="1" t="s">
         <v>5</v>
@@ -3993,17 +4011,15 @@
         <v>144</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="E146" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F146" s="1" t="s">
-        <v>27</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F146" s="1"/>
       <c r="G146" s="1"/>
     </row>
     <row r="147" spans="2:7">
@@ -4011,13 +4027,13 @@
         <v>145</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="E147" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F147" s="1"/>
       <c r="G147" s="1"/>
@@ -4027,10 +4043,10 @@
         <v>146</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="E148" s="1" t="s">
         <v>5</v>
@@ -4043,15 +4059,17 @@
         <v>147</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="E149" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F149" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F149" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G149" s="1"/>
     </row>
     <row r="150" spans="2:7">
@@ -4059,13 +4077,13 @@
         <v>148</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="E150" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F150" s="1"/>
       <c r="G150" s="1"/>
@@ -4075,10 +4093,10 @@
         <v>149</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="E151" s="1" t="s">
         <v>5</v>
@@ -4091,10 +4109,10 @@
         <v>150</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>358</v>
+        <v>252</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>357</v>
+        <v>253</v>
       </c>
       <c r="E152" s="1" t="s">
         <v>5</v>
@@ -4107,10 +4125,10 @@
         <v>151</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="E153" s="1" t="s">
         <v>5</v>
@@ -4123,10 +4141,10 @@
         <v>152</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="E154" s="1" t="s">
         <v>5</v>
@@ -4139,17 +4157,15 @@
         <v>153</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>262</v>
+        <v>358</v>
       </c>
       <c r="D155" s="1" t="s">
-        <v>263</v>
+        <v>357</v>
       </c>
       <c r="E155" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F155" s="1" t="s">
-        <v>27</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F155" s="1"/>
       <c r="G155" s="1"/>
     </row>
     <row r="156" spans="2:7">
@@ -4157,10 +4173,10 @@
         <v>154</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="E156" s="1" t="s">
         <v>5</v>
@@ -4173,10 +4189,10 @@
         <v>155</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="E157" s="1" t="s">
         <v>5</v>
@@ -4189,10 +4205,10 @@
         <v>156</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="D158" s="1" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="E158" s="1" t="s">
         <v>7</v>
@@ -4207,10 +4223,10 @@
         <v>157</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="E159" s="1" t="s">
         <v>5</v>
@@ -4223,10 +4239,10 @@
         <v>158</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="D160" s="1" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="E160" s="1" t="s">
         <v>5</v>
@@ -4239,15 +4255,17 @@
         <v>159</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="D161" s="1" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="E161" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F161" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F161" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G161" s="1"/>
     </row>
     <row r="162" spans="2:7">
@@ -4255,10 +4273,10 @@
         <v>160</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="D162" s="1" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="E162" s="1" t="s">
         <v>5</v>
@@ -4271,10 +4289,10 @@
         <v>161</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="D163" s="1" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="E163" s="1" t="s">
         <v>5</v>
@@ -4287,10 +4305,10 @@
         <v>162</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>10</v>
+        <v>274</v>
       </c>
       <c r="D164" s="1" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="E164" s="1" t="s">
         <v>5</v>
@@ -4303,13 +4321,13 @@
         <v>163</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>329</v>
+        <v>276</v>
       </c>
       <c r="D165" s="1" t="s">
-        <v>330</v>
+        <v>277</v>
       </c>
       <c r="E165" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F165" s="1"/>
       <c r="G165" s="1"/>
@@ -4319,17 +4337,15 @@
         <v>164</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="D166" s="1" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="E166" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F166" s="1" t="s">
-        <v>27</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F166" s="1"/>
       <c r="G166" s="1"/>
     </row>
     <row r="167" spans="2:7">
@@ -4337,10 +4353,10 @@
         <v>165</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>283</v>
+        <v>10</v>
       </c>
       <c r="D167" s="1" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="E167" s="1" t="s">
         <v>5</v>
@@ -4353,10 +4369,10 @@
         <v>166</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>285</v>
+        <v>329</v>
       </c>
       <c r="D168" s="1" t="s">
-        <v>286</v>
+        <v>330</v>
       </c>
       <c r="E168" s="1" t="s">
         <v>6</v>
@@ -4369,10 +4385,10 @@
         <v>167</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="D169" s="1" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="E169" s="1" t="s">
         <v>7</v>
@@ -4387,17 +4403,15 @@
         <v>168</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="D170" s="1" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="E170" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F170" s="1" t="s">
-        <v>27</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F170" s="1"/>
       <c r="G170" s="1"/>
     </row>
     <row r="171" spans="2:7">
@@ -4405,17 +4419,15 @@
         <v>169</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="D171" s="1" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="E171" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F171" s="1" t="s">
-        <v>27</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="F171" s="1"/>
       <c r="G171" s="1"/>
     </row>
     <row r="172" spans="2:7">
@@ -4423,15 +4435,17 @@
         <v>170</v>
       </c>
       <c r="C172" s="1" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="D172" s="1" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="E172" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F172" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F172" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G172" s="1"/>
     </row>
     <row r="173" spans="2:7">
@@ -4439,10 +4453,10 @@
         <v>171</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="D173" s="1" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="E173" s="1" t="s">
         <v>7</v>
@@ -4457,15 +4471,17 @@
         <v>172</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="D174" s="1" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="E174" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F174" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F174" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G174" s="1"/>
     </row>
     <row r="175" spans="2:7">
@@ -4473,10 +4489,10 @@
         <v>173</v>
       </c>
       <c r="C175" s="1" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="D175" s="1" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="E175" s="1" t="s">
         <v>5</v>
@@ -4485,26 +4501,52 @@
       <c r="G175" s="1"/>
     </row>
     <row r="176" spans="2:7">
-      <c r="B176" s="6"/>
-      <c r="C176" s="1"/>
-      <c r="D176" s="1"/>
-      <c r="E176" s="1"/>
-      <c r="F176" s="1"/>
+      <c r="B176" s="6">
+        <v>174</v>
+      </c>
+      <c r="C176" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="D176" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="E176" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F176" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G176" s="1"/>
     </row>
     <row r="177" spans="2:7">
-      <c r="B177" s="6"/>
-      <c r="C177" s="1"/>
-      <c r="D177" s="1"/>
-      <c r="E177" s="1"/>
+      <c r="B177" s="6">
+        <v>175</v>
+      </c>
+      <c r="C177" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="D177" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="E177" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F177" s="1"/>
       <c r="G177" s="1"/>
     </row>
     <row r="178" spans="2:7">
-      <c r="B178" s="6"/>
-      <c r="C178" s="1"/>
-      <c r="D178" s="1"/>
-      <c r="E178" s="1"/>
+      <c r="B178" s="6">
+        <v>176</v>
+      </c>
+      <c r="C178" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="D178" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="E178" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F178" s="1"/>
       <c r="G178" s="1"/>
     </row>
@@ -4516,12 +4558,36 @@
       <c r="F179" s="1"/>
       <c r="G179" s="1"/>
     </row>
+    <row r="180" spans="2:7">
+      <c r="B180" s="6"/>
+      <c r="C180" s="1"/>
+      <c r="D180" s="1"/>
+      <c r="E180" s="1"/>
+      <c r="F180" s="1"/>
+      <c r="G180" s="1"/>
+    </row>
+    <row r="181" spans="2:7">
+      <c r="B181" s="6"/>
+      <c r="C181" s="1"/>
+      <c r="D181" s="1"/>
+      <c r="E181" s="1"/>
+      <c r="F181" s="1"/>
+      <c r="G181" s="1"/>
+    </row>
+    <row r="182" spans="2:7">
+      <c r="B182" s="6"/>
+      <c r="C182" s="1"/>
+      <c r="D182" s="1"/>
+      <c r="E182" s="1"/>
+      <c r="F182" s="1"/>
+      <c r="G182" s="1"/>
+    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E175" xr:uid="{7E8CE32C-29D1-4006-9E0F-69B72A0F4378}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E178" xr:uid="{7E8CE32C-29D1-4006-9E0F-69B72A0F4378}">
       <formula1>"[Application],[Directory],[Script]"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F179" xr:uid="{A5D947FB-5606-4B36-88C5-81CC2B61C636}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F182" xr:uid="{A5D947FB-5606-4B36-88C5-81CC2B61C636}">
       <formula1>"[bat],[vbs]"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
update Run shortuct Creator configs 1.0
</commit_message>
<xml_diff>
--- a/Database/Run_shortcut_creator_aliases.xlsx
+++ b/Database/Run_shortcut_creator_aliases.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\player-1\Documents\Windows-Git-Repos\win-t\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE3B2CEE-BF32-4D78-91D2-E5628DFE5CF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C782DC5-151F-4AB5-B303-A221680641FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14295" yWindow="0" windowWidth="14625" windowHeight="15585" xr2:uid="{D65865D6-BB34-410C-8183-31ED199784FF}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="371">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="376">
   <si>
     <t>Number</t>
   </si>
@@ -1171,6 +1171,21 @@
   </si>
   <si>
     <t>Advanced Renamer</t>
+  </si>
+  <si>
+    <t>Office Tab Center</t>
+  </si>
+  <si>
+    <t>otc</t>
+  </si>
+  <si>
+    <t>Microsoft Visio</t>
+  </si>
+  <si>
+    <t>vis</t>
+  </si>
+  <si>
+    <t>Regcool</t>
   </si>
 </sst>
 </file>
@@ -1602,10 +1617,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58A033C2-67FB-408D-B72B-8C45836FCF74}">
-  <dimension ref="B2:G185"/>
+  <dimension ref="B2:G188"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B151" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B107" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
+      <selection activeCell="C129" sqref="C129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21"/>
@@ -1641,7 +1656,7 @@
     </row>
     <row r="3" spans="2:7" ht="24.95" customHeight="1">
       <c r="B3" s="6" cm="1">
-        <f t="array" ref="B3:B181">_xlfn.SEQUENCE(COUNTA(C:C)-1)</f>
+        <f t="array" ref="B3:B184">_xlfn.SEQUENCE(COUNTA(C:C)-1)</f>
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -3381,10 +3396,10 @@
         <v>105</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>164</v>
+        <v>371</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>165</v>
+        <v>372</v>
       </c>
       <c r="E107" s="1" t="s">
         <v>5</v>
@@ -3397,10 +3412,10 @@
         <v>106</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E108" s="1" t="s">
         <v>5</v>
@@ -3413,10 +3428,10 @@
         <v>107</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E109" s="1" t="s">
         <v>5</v>
@@ -3429,10 +3444,10 @@
         <v>108</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E110" s="1" t="s">
         <v>5</v>
@@ -3445,10 +3460,10 @@
         <v>109</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E111" s="1" t="s">
         <v>5</v>
@@ -3461,10 +3476,10 @@
         <v>110</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>339</v>
+        <v>172</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E112" s="1" t="s">
         <v>5</v>
@@ -3477,10 +3492,10 @@
         <v>111</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>175</v>
+        <v>339</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E113" s="1" t="s">
         <v>5</v>
@@ -3493,17 +3508,15 @@
         <v>112</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F114" s="1" t="s">
-        <v>27</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F114" s="1"/>
       <c r="G114" s="1"/>
     </row>
     <row r="115" spans="2:7">
@@ -3511,15 +3524,17 @@
         <v>113</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F115" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F115" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G115" s="1"/>
     </row>
     <row r="116" spans="2:7">
@@ -3527,10 +3542,10 @@
         <v>114</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E116" s="1" t="s">
         <v>5</v>
@@ -3543,10 +3558,10 @@
         <v>115</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E117" s="1" t="s">
         <v>5</v>
@@ -3559,10 +3574,10 @@
         <v>116</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E118" s="1" t="s">
         <v>5</v>
@@ -3575,10 +3590,10 @@
         <v>117</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E119" s="1" t="s">
         <v>5</v>
@@ -3591,10 +3606,10 @@
         <v>118</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E120" s="1" t="s">
         <v>5</v>
@@ -3607,10 +3622,10 @@
         <v>119</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E121" s="1" t="s">
         <v>5</v>
@@ -3623,10 +3638,10 @@
         <v>120</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>340</v>
+        <v>191</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>341</v>
+        <v>192</v>
       </c>
       <c r="E122" s="1" t="s">
         <v>5</v>
@@ -3639,10 +3654,10 @@
         <v>121</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>193</v>
+        <v>340</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>194</v>
+        <v>341</v>
       </c>
       <c r="E123" s="1" t="s">
         <v>5</v>
@@ -3655,10 +3670,10 @@
         <v>122</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>337</v>
+        <v>375</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>338</v>
+        <v>194</v>
       </c>
       <c r="E124" s="1" t="s">
         <v>5</v>
@@ -3671,17 +3686,15 @@
         <v>123</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F125" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F125" s="1"/>
       <c r="G125" s="1"/>
     </row>
     <row r="126" spans="2:7">
@@ -3689,10 +3702,10 @@
         <v>124</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>197</v>
+        <v>337</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>198</v>
+        <v>338</v>
       </c>
       <c r="E126" s="1" t="s">
         <v>5</v>
@@ -3705,15 +3718,17 @@
         <v>125</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F127" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F127" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="G127" s="1"/>
     </row>
     <row r="128" spans="2:7">
@@ -3721,10 +3736,10 @@
         <v>126</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>351</v>
+        <v>197</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>350</v>
+        <v>198</v>
       </c>
       <c r="E128" s="1" t="s">
         <v>5</v>
@@ -3737,10 +3752,10 @@
         <v>127</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E129" s="1" t="s">
         <v>5</v>
@@ -3753,10 +3768,10 @@
         <v>128</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>203</v>
+        <v>351</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>204</v>
+        <v>350</v>
       </c>
       <c r="E130" s="1" t="s">
         <v>5</v>
@@ -3769,13 +3784,13 @@
         <v>129</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="E131" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F131" s="1"/>
       <c r="G131" s="1"/>
@@ -3785,17 +3800,15 @@
         <v>130</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>362</v>
+        <v>203</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>363</v>
+        <v>204</v>
       </c>
       <c r="E132" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F132" s="1" t="s">
-        <v>27</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F132" s="1"/>
       <c r="G132" s="1"/>
     </row>
     <row r="133" spans="2:7">
@@ -3803,13 +3816,13 @@
         <v>131</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E133" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F133" s="1"/>
       <c r="G133" s="1"/>
@@ -3819,15 +3832,17 @@
         <v>132</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>209</v>
+        <v>362</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>210</v>
+        <v>363</v>
       </c>
       <c r="E134" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F134" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F134" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G134" s="1"/>
     </row>
     <row r="135" spans="2:7">
@@ -3835,10 +3850,10 @@
         <v>133</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="E135" s="1" t="s">
         <v>5</v>
@@ -3851,17 +3866,15 @@
         <v>134</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="E136" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F136" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F136" s="1"/>
       <c r="G136" s="1"/>
     </row>
     <row r="137" spans="2:7">
@@ -3869,10 +3882,10 @@
         <v>135</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="E137" s="1" t="s">
         <v>5</v>
@@ -3885,15 +3898,17 @@
         <v>136</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="E138" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F138" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F138" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="G138" s="1"/>
     </row>
     <row r="139" spans="2:7">
@@ -3901,17 +3916,15 @@
         <v>137</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E139" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F139" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F139" s="1"/>
       <c r="G139" s="1"/>
     </row>
     <row r="140" spans="2:7">
@@ -3919,50 +3932,44 @@
         <v>138</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="E140" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F140" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G140" s="1" t="s">
-        <v>30</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F140" s="1"/>
+      <c r="G140" s="1"/>
     </row>
     <row r="141" spans="2:7">
       <c r="B141" s="6">
         <v>139</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="E141" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F141" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G141" s="1" t="s">
-        <v>30</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="G141" s="1"/>
     </row>
     <row r="142" spans="2:7">
       <c r="B142" s="6">
         <v>140</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="E142" s="1" t="s">
         <v>7</v>
@@ -3971,7 +3978,7 @@
         <v>27</v>
       </c>
       <c r="G142" s="1" t="s">
-        <v>300</v>
+        <v>30</v>
       </c>
     </row>
     <row r="143" spans="2:7">
@@ -3979,10 +3986,10 @@
         <v>141</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="E143" s="1" t="s">
         <v>7</v>
@@ -3990,38 +3997,46 @@
       <c r="F143" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G143" s="1"/>
+      <c r="G143" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="144" spans="2:7">
       <c r="B144" s="6">
         <v>142</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="E144" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F144" s="1"/>
-      <c r="G144" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F144" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G144" s="1" t="s">
+        <v>300</v>
+      </c>
     </row>
     <row r="145" spans="2:7">
       <c r="B145" s="6">
         <v>143</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E145" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F145" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F145" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G145" s="1"/>
     </row>
     <row r="146" spans="2:7">
@@ -4029,17 +4044,15 @@
         <v>144</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="E146" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F146" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F146" s="1"/>
       <c r="G146" s="1"/>
     </row>
     <row r="147" spans="2:7">
@@ -4047,17 +4060,15 @@
         <v>145</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="E147" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F147" s="1" t="s">
-        <v>27</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F147" s="1"/>
       <c r="G147" s="1"/>
     </row>
     <row r="148" spans="2:7">
@@ -4065,15 +4076,17 @@
         <v>146</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="E148" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F148" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F148" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="G148" s="1"/>
     </row>
     <row r="149" spans="2:7">
@@ -4081,15 +4094,17 @@
         <v>147</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="E149" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F149" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F149" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G149" s="1"/>
     </row>
     <row r="150" spans="2:7">
@@ -4097,10 +4112,10 @@
         <v>148</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="E150" s="1" t="s">
         <v>5</v>
@@ -4113,10 +4128,10 @@
         <v>149</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="E151" s="1" t="s">
         <v>5</v>
@@ -4129,17 +4144,15 @@
         <v>150</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="E152" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F152" s="1" t="s">
-        <v>27</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F152" s="1"/>
       <c r="G152" s="1"/>
     </row>
     <row r="153" spans="2:7">
@@ -4147,13 +4160,13 @@
         <v>151</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="E153" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F153" s="1"/>
       <c r="G153" s="1"/>
@@ -4163,15 +4176,17 @@
         <v>152</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="E154" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F154" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F154" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G154" s="1"/>
     </row>
     <row r="155" spans="2:7">
@@ -4179,13 +4194,13 @@
         <v>153</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="D155" s="1" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="E155" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F155" s="1"/>
       <c r="G155" s="1"/>
@@ -4195,10 +4210,10 @@
         <v>154</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="E156" s="1" t="s">
         <v>5</v>
@@ -4211,10 +4226,10 @@
         <v>155</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="E157" s="1" t="s">
         <v>5</v>
@@ -4227,10 +4242,10 @@
         <v>156</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>357</v>
+        <v>253</v>
       </c>
       <c r="D158" s="1" t="s">
-        <v>356</v>
+        <v>254</v>
       </c>
       <c r="E158" s="1" t="s">
         <v>5</v>
@@ -4243,10 +4258,10 @@
         <v>157</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E159" s="1" t="s">
         <v>5</v>
@@ -4259,10 +4274,10 @@
         <v>158</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>259</v>
+        <v>357</v>
       </c>
       <c r="D160" s="1" t="s">
-        <v>260</v>
+        <v>356</v>
       </c>
       <c r="E160" s="1" t="s">
         <v>5</v>
@@ -4275,17 +4290,15 @@
         <v>159</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="D161" s="1" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="E161" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F161" s="1" t="s">
-        <v>27</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F161" s="1"/>
       <c r="G161" s="1"/>
     </row>
     <row r="162" spans="2:7">
@@ -4293,10 +4306,10 @@
         <v>160</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="D162" s="1" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="E162" s="1" t="s">
         <v>5</v>
@@ -4309,15 +4322,17 @@
         <v>161</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="D163" s="1" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="E163" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F163" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F163" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G163" s="1"/>
     </row>
     <row r="164" spans="2:7">
@@ -4325,17 +4340,15 @@
         <v>162</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>267</v>
+        <v>373</v>
       </c>
       <c r="D164" s="1" t="s">
-        <v>268</v>
+        <v>374</v>
       </c>
       <c r="E164" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F164" s="1" t="s">
-        <v>27</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F164" s="1"/>
       <c r="G164" s="1"/>
     </row>
     <row r="165" spans="2:7">
@@ -4343,10 +4356,10 @@
         <v>163</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="D165" s="1" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="E165" s="1" t="s">
         <v>5</v>
@@ -4359,10 +4372,10 @@
         <v>164</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D166" s="1" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="E166" s="1" t="s">
         <v>5</v>
@@ -4375,15 +4388,17 @@
         <v>165</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="D167" s="1" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="E167" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F167" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F167" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G167" s="1"/>
     </row>
     <row r="168" spans="2:7">
@@ -4391,10 +4406,10 @@
         <v>166</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="D168" s="1" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="E168" s="1" t="s">
         <v>5</v>
@@ -4407,10 +4422,10 @@
         <v>167</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="D169" s="1" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="E169" s="1" t="s">
         <v>5</v>
@@ -4423,10 +4438,10 @@
         <v>168</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>10</v>
+        <v>273</v>
       </c>
       <c r="D170" s="1" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="E170" s="1" t="s">
         <v>5</v>
@@ -4439,13 +4454,13 @@
         <v>169</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>328</v>
+        <v>275</v>
       </c>
       <c r="D171" s="1" t="s">
-        <v>329</v>
+        <v>276</v>
       </c>
       <c r="E171" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F171" s="1"/>
       <c r="G171" s="1"/>
@@ -4455,17 +4470,15 @@
         <v>170</v>
       </c>
       <c r="C172" s="1" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="D172" s="1" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="E172" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F172" s="1" t="s">
-        <v>27</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F172" s="1"/>
       <c r="G172" s="1"/>
     </row>
     <row r="173" spans="2:7">
@@ -4473,10 +4486,10 @@
         <v>171</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>282</v>
+        <v>10</v>
       </c>
       <c r="D173" s="1" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="E173" s="1" t="s">
         <v>5</v>
@@ -4489,10 +4502,10 @@
         <v>172</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>284</v>
+        <v>328</v>
       </c>
       <c r="D174" s="1" t="s">
-        <v>285</v>
+        <v>329</v>
       </c>
       <c r="E174" s="1" t="s">
         <v>6</v>
@@ -4505,10 +4518,10 @@
         <v>173</v>
       </c>
       <c r="C175" s="1" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="D175" s="1" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="E175" s="1" t="s">
         <v>7</v>
@@ -4523,17 +4536,15 @@
         <v>174</v>
       </c>
       <c r="C176" s="1" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="D176" s="1" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="E176" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F176" s="1" t="s">
-        <v>27</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F176" s="1"/>
       <c r="G176" s="1"/>
     </row>
     <row r="177" spans="2:7">
@@ -4541,17 +4552,15 @@
         <v>175</v>
       </c>
       <c r="C177" s="1" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="D177" s="1" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="E177" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F177" s="1" t="s">
-        <v>27</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="F177" s="1"/>
       <c r="G177" s="1"/>
     </row>
     <row r="178" spans="2:7">
@@ -4559,15 +4568,17 @@
         <v>176</v>
       </c>
       <c r="C178" s="1" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="D178" s="1" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="E178" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F178" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F178" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G178" s="1"/>
     </row>
     <row r="179" spans="2:7">
@@ -4575,10 +4586,10 @@
         <v>177</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="D179" s="1" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="E179" s="1" t="s">
         <v>7</v>
@@ -4593,15 +4604,17 @@
         <v>178</v>
       </c>
       <c r="C180" s="1" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="D180" s="1" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="E180" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F180" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F180" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G180" s="1"/>
     </row>
     <row r="181" spans="2:7">
@@ -4609,10 +4622,10 @@
         <v>179</v>
       </c>
       <c r="C181" s="1" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="D181" s="1" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="E181" s="1" t="s">
         <v>5</v>
@@ -4621,26 +4634,52 @@
       <c r="G181" s="1"/>
     </row>
     <row r="182" spans="2:7">
-      <c r="B182" s="6"/>
-      <c r="C182" s="1"/>
-      <c r="D182" s="1"/>
-      <c r="E182" s="1"/>
-      <c r="F182" s="1"/>
+      <c r="B182" s="6">
+        <v>180</v>
+      </c>
+      <c r="C182" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="D182" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="E182" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F182" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G182" s="1"/>
     </row>
     <row r="183" spans="2:7">
-      <c r="B183" s="6"/>
-      <c r="C183" s="1"/>
-      <c r="D183" s="1"/>
-      <c r="E183" s="1"/>
+      <c r="B183" s="6">
+        <v>181</v>
+      </c>
+      <c r="C183" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="D183" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="E183" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F183" s="1"/>
       <c r="G183" s="1"/>
     </row>
     <row r="184" spans="2:7">
-      <c r="B184" s="6"/>
-      <c r="C184" s="1"/>
-      <c r="D184" s="1"/>
-      <c r="E184" s="1"/>
+      <c r="B184" s="6">
+        <v>182</v>
+      </c>
+      <c r="C184" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="D184" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="E184" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F184" s="1"/>
       <c r="G184" s="1"/>
     </row>
@@ -4652,12 +4691,36 @@
       <c r="F185" s="1"/>
       <c r="G185" s="1"/>
     </row>
+    <row r="186" spans="2:7">
+      <c r="B186" s="6"/>
+      <c r="C186" s="1"/>
+      <c r="D186" s="1"/>
+      <c r="E186" s="1"/>
+      <c r="F186" s="1"/>
+      <c r="G186" s="1"/>
+    </row>
+    <row r="187" spans="2:7">
+      <c r="B187" s="6"/>
+      <c r="C187" s="1"/>
+      <c r="D187" s="1"/>
+      <c r="E187" s="1"/>
+      <c r="F187" s="1"/>
+      <c r="G187" s="1"/>
+    </row>
+    <row r="188" spans="2:7">
+      <c r="B188" s="6"/>
+      <c r="C188" s="1"/>
+      <c r="D188" s="1"/>
+      <c r="E188" s="1"/>
+      <c r="F188" s="1"/>
+      <c r="G188" s="1"/>
+    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E181" xr:uid="{7E8CE32C-29D1-4006-9E0F-69B72A0F4378}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E184" xr:uid="{7E8CE32C-29D1-4006-9E0F-69B72A0F4378}">
       <formula1>"[Application],[Directory],[Script]"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F185" xr:uid="{A5D947FB-5606-4B36-88C5-81CC2B61C636}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F188" xr:uid="{A5D947FB-5606-4B36-88C5-81CC2B61C636}">
       <formula1>"[bat],[vbs]"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Update New changes 2025-01-18-05.23.42
</commit_message>
<xml_diff>
--- a/Database/Run_shortcut_creator_aliases.xlsx
+++ b/Database/Run_shortcut_creator_aliases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\player-1\Documents\Windows-Git-Repos\win-t\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{708019BB-71A0-4A60-B4C9-739EE5DE859A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{087ABB4F-017C-4785-9947-20A0C65C1912}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14295" yWindow="0" windowWidth="14625" windowHeight="15585" xr2:uid="{D65865D6-BB34-410C-8183-31ED199784FF}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="394">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="441">
   <si>
     <t>Number</t>
   </si>
@@ -1240,6 +1240,147 @@
   </si>
   <si>
     <t>Before Mass</t>
+  </si>
+  <si>
+    <t>Markdown</t>
+  </si>
+  <si>
+    <t>All Hymn Order</t>
+  </si>
+  <si>
+    <t>allho</t>
+  </si>
+  <si>
+    <t>hls</t>
+  </si>
+  <si>
+    <t>Hymn List Selection (Choir's EasyWorship Schedule Select Tool)</t>
+  </si>
+  <si>
+    <t>cp-win10</t>
+  </si>
+  <si>
+    <t>cp-win11</t>
+  </si>
+  <si>
+    <t>cp-win1124h2</t>
+  </si>
+  <si>
+    <t>Church Presentation Main Script Extract For Windows 10</t>
+  </si>
+  <si>
+    <t>Church Presentation Main Script Extract For Windows 11</t>
+  </si>
+  <si>
+    <t>Church Presentation Main Script Extract For Windows 11 24H2</t>
+  </si>
+  <si>
+    <t>New Hymns (Easyworhip New Schedule)</t>
+  </si>
+  <si>
+    <t>nh</t>
+  </si>
+  <si>
+    <t>sync</t>
+  </si>
+  <si>
+    <t>Synchredible</t>
+  </si>
+  <si>
+    <t>Altus - Web Whatsapp Clone</t>
+  </si>
+  <si>
+    <t>aw</t>
+  </si>
+  <si>
+    <t>cd</t>
+  </si>
+  <si>
+    <t>Corel Draw 22</t>
+  </si>
+  <si>
+    <t>cfm</t>
+  </si>
+  <si>
+    <t>Corel Font Manager</t>
+  </si>
+  <si>
+    <t>cam</t>
+  </si>
+  <si>
+    <t>Camtasia 2022</t>
+  </si>
+  <si>
+    <t>Camtasia 2022 Recorder</t>
+  </si>
+  <si>
+    <t>camd</t>
+  </si>
+  <si>
+    <t>wp</t>
+  </si>
+  <si>
+    <t>WindowTop</t>
+  </si>
+  <si>
+    <t>fm</t>
+  </si>
+  <si>
+    <t>High-Logic MainType</t>
+  </si>
+  <si>
+    <t>fl</t>
+  </si>
+  <si>
+    <t>FileLocater Pro</t>
+  </si>
+  <si>
+    <t>icoc</t>
+  </si>
+  <si>
+    <t>IcoFX</t>
+  </si>
+  <si>
+    <t>cc</t>
+  </si>
+  <si>
+    <t>ColorCatcher 3.4</t>
+  </si>
+  <si>
+    <t>Start Ansi Typing (Sinhala)</t>
+  </si>
+  <si>
+    <t>at</t>
+  </si>
+  <si>
+    <t>kat</t>
+  </si>
+  <si>
+    <t>Kill Ansi Typing (Sinhala)</t>
+  </si>
+  <si>
+    <t>mp</t>
+  </si>
+  <si>
+    <t>Microsoft Photos</t>
+  </si>
+  <si>
+    <t>wake</t>
+  </si>
+  <si>
+    <t>Wakey</t>
+  </si>
+  <si>
+    <t>bat</t>
+  </si>
+  <si>
+    <t>Bat To Exe Converter</t>
+  </si>
+  <si>
+    <t>pexe</t>
+  </si>
+  <si>
+    <t>win-ps2exe</t>
   </si>
 </sst>
 </file>
@@ -1671,16 +1812,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58A033C2-67FB-408D-B72B-8C45836FCF74}">
-  <dimension ref="B2:G196"/>
+  <dimension ref="B2:G219"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A174" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A120" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
+      <selection activeCell="E138" sqref="E138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="13.5703125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="93.42578125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="98.28515625" style="4" customWidth="1"/>
     <col min="4" max="4" width="19.42578125" style="4" customWidth="1"/>
     <col min="5" max="5" width="25.7109375" style="5" customWidth="1"/>
     <col min="6" max="6" width="28.28515625" style="5" customWidth="1"/>
@@ -1710,7 +1851,7 @@
     </row>
     <row r="3" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="6" cm="1">
-        <f t="array" ref="B3:B192">_xlfn.SEQUENCE(COUNTA(C:C)-1)</f>
+        <f t="array" ref="B3:B215">_xlfn.SEQUENCE(COUNTA(C:C)-1)</f>
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -1820,10 +1961,14 @@
         <v>319</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>394</v>
+      </c>
     </row>
     <row r="10" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="6">
@@ -1907,9 +2052,7 @@
       <c r="F14" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G14" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="G14" s="1"/>
     </row>
     <row r="15" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="6">
@@ -1932,19 +2075,19 @@
         <v>14</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>28</v>
+        <v>395</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>29</v>
+        <v>396</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
@@ -1952,26 +2095,30 @@
         <v>15</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>351</v>
+        <v>28</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>350</v>
+        <v>29</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="18" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="6">
         <v>16</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>366</v>
+        <v>351</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>365</v>
+        <v>350</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>5</v>
@@ -1984,10 +2131,10 @@
         <v>17</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>31</v>
+        <v>366</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>32</v>
+        <v>365</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>5</v>
@@ -2000,10 +2147,10 @@
         <v>18</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>33</v>
+        <v>429</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>34</v>
+        <v>430</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>5</v>
@@ -2016,17 +2163,15 @@
         <v>19</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>27</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F21" s="1"/>
       <c r="G21" s="1"/>
     </row>
     <row r="22" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
@@ -2034,17 +2179,15 @@
         <v>20</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>27</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F22" s="1"/>
       <c r="G22" s="1"/>
     </row>
     <row r="23" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
@@ -2052,10 +2195,10 @@
         <v>21</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>39</v>
+        <v>409</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>40</v>
+        <v>410</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>5</v>
@@ -2068,15 +2211,17 @@
         <v>22</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F24" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G24" s="1"/>
     </row>
     <row r="25" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
@@ -2084,16 +2229,16 @@
         <v>23</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="G25" s="1"/>
     </row>
@@ -2102,17 +2247,15 @@
         <v>24</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>27</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F26" s="1"/>
       <c r="G26" s="1"/>
     </row>
     <row r="27" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
@@ -2120,17 +2263,15 @@
         <v>25</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>393</v>
+        <v>41</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>392</v>
+        <v>42</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="F27" s="1"/>
       <c r="G27" s="1"/>
     </row>
     <row r="28" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
@@ -2138,13 +2279,13 @@
         <v>26</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>301</v>
+        <v>438</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>302</v>
+        <v>437</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
@@ -2154,15 +2295,17 @@
         <v>27</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>331</v>
+        <v>43</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>330</v>
+        <v>44</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F29" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="G29" s="1"/>
     </row>
     <row r="30" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
@@ -2170,16 +2313,16 @@
         <v>28</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>106</v>
+        <v>45</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="G30" s="1"/>
     </row>
@@ -2188,15 +2331,17 @@
         <v>29</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>376</v>
+        <v>393</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>48</v>
+        <v>392</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F31" s="1"/>
+      <c r="F31" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="G31" s="1"/>
     </row>
     <row r="32" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
@@ -2204,13 +2349,13 @@
         <v>30</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>49</v>
+        <v>416</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>50</v>
+        <v>415</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
@@ -2220,10 +2365,10 @@
         <v>31</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>303</v>
+        <v>417</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>304</v>
+        <v>418</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>5</v>
@@ -2236,13 +2381,13 @@
         <v>32</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>52</v>
+        <v>301</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>51</v>
+        <v>302</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
@@ -2252,17 +2397,15 @@
         <v>33</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>54</v>
+        <v>428</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>53</v>
+        <v>427</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F35" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="F35" s="1"/>
       <c r="G35" s="1"/>
     </row>
     <row r="36" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
@@ -2270,17 +2413,15 @@
         <v>34</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>55</v>
+        <v>412</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>58</v>
+        <v>411</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F36" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="F36" s="1"/>
       <c r="G36" s="1"/>
     </row>
     <row r="37" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
@@ -2288,17 +2429,15 @@
         <v>35</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>56</v>
+        <v>331</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>57</v>
+        <v>330</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F37" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="F37" s="1"/>
       <c r="G37" s="1"/>
     </row>
     <row r="38" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
@@ -2306,13 +2445,13 @@
         <v>36</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>59</v>
+        <v>414</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>60</v>
+        <v>413</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
@@ -2322,78 +2461,76 @@
         <v>37</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>61</v>
+        <v>106</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F39" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="G39" s="1"/>
     </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B40" s="6">
         <v>38</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>65</v>
+        <v>376</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>27</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F40" s="1"/>
       <c r="G40" s="1"/>
     </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B41" s="6">
         <v>39</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>360</v>
+        <v>49</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
     </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B42" s="6">
         <v>40</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>66</v>
+        <v>303</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>67</v>
+        <v>304</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>27</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F42" s="1"/>
       <c r="G42" s="1"/>
     </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B43" s="6">
         <v>41</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>5</v>
@@ -2401,67 +2538,69 @@
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
     </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B44" s="6">
         <v>42</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F44" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G44" s="1"/>
     </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B45" s="6">
         <v>43</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>338</v>
+        <v>55</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>339</v>
+        <v>58</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F45" s="1"/>
+      <c r="F45" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="G45" s="1"/>
     </row>
-    <row r="46" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B46" s="6">
         <v>44</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="G46" s="1"/>
     </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B47" s="6">
         <v>45</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>299</v>
+        <v>59</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>300</v>
+        <v>60</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>6</v>
@@ -2469,69 +2608,63 @@
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
     </row>
-    <row r="48" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B48" s="6">
         <v>46</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>74</v>
+        <v>402</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>75</v>
+        <v>399</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>27</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F48" s="1"/>
       <c r="G48" s="1"/>
     </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B49" s="6">
         <v>47</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>77</v>
+        <v>403</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>76</v>
+        <v>400</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F49" s="1"/>
       <c r="G49" s="1"/>
     </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B50" s="6">
         <v>48</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>78</v>
+        <v>404</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>79</v>
+        <v>401</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>27</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F50" s="1"/>
       <c r="G50" s="1"/>
     </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B51" s="6">
         <v>49</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>364</v>
+        <v>61</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>363</v>
+        <v>62</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>5</v>
@@ -2544,10 +2677,10 @@
         <v>50</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>7</v>
@@ -2562,17 +2695,15 @@
         <v>51</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>388</v>
+        <v>360</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>389</v>
+        <v>64</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F53" s="1"/>
       <c r="G53" s="1"/>
     </row>
     <row r="54" spans="2:7" x14ac:dyDescent="0.35">
@@ -2580,15 +2711,17 @@
         <v>52</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F54" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G54" s="1"/>
     </row>
     <row r="55" spans="2:7" x14ac:dyDescent="0.35">
@@ -2596,17 +2729,15 @@
         <v>53</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F55" s="1"/>
       <c r="G55" s="1"/>
     </row>
     <row r="56" spans="2:7" x14ac:dyDescent="0.35">
@@ -2614,10 +2745,10 @@
         <v>54</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>7</v>
@@ -2632,10 +2763,10 @@
         <v>55</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>88</v>
+        <v>338</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>89</v>
+        <v>339</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>5</v>
@@ -2643,20 +2774,22 @@
       <c r="F57" s="1"/>
       <c r="G57" s="1"/>
     </row>
-    <row r="58" spans="2:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B58" s="6">
         <v>56</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F58" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G58" s="1"/>
     </row>
     <row r="59" spans="2:7" x14ac:dyDescent="0.35">
@@ -2664,13 +2797,13 @@
         <v>57</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>92</v>
+        <v>299</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>93</v>
+        <v>300</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
@@ -2680,15 +2813,17 @@
         <v>58</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>332</v>
+        <v>74</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>333</v>
+        <v>75</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F60" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G60" s="1"/>
     </row>
     <row r="61" spans="2:7" x14ac:dyDescent="0.35">
@@ -2696,15 +2831,17 @@
         <v>59</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>94</v>
+        <v>77</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F61" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="G61" s="1"/>
     </row>
     <row r="62" spans="2:7" x14ac:dyDescent="0.35">
@@ -2712,15 +2849,17 @@
         <v>60</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>96</v>
+        <v>78</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F62" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G62" s="1"/>
     </row>
     <row r="63" spans="2:7" x14ac:dyDescent="0.35">
@@ -2728,10 +2867,10 @@
         <v>61</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>98</v>
+        <v>364</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>99</v>
+        <v>363</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>5</v>
@@ -2744,15 +2883,17 @@
         <v>62</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F64" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G64" s="1"/>
     </row>
     <row r="65" spans="2:7" x14ac:dyDescent="0.35">
@@ -2760,15 +2901,17 @@
         <v>63</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>102</v>
+        <v>388</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>104</v>
+        <v>389</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F65" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="G65" s="1"/>
     </row>
     <row r="66" spans="2:7" x14ac:dyDescent="0.35">
@@ -2776,10 +2919,10 @@
         <v>64</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>103</v>
+        <v>82</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>105</v>
+        <v>83</v>
       </c>
       <c r="E66" s="1" t="s">
         <v>5</v>
@@ -2792,15 +2935,17 @@
         <v>65</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>354</v>
+        <v>84</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>355</v>
+        <v>85</v>
       </c>
       <c r="E67" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F67" s="1"/>
+      <c r="F67" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="G67" s="1"/>
     </row>
     <row r="68" spans="2:7" x14ac:dyDescent="0.35">
@@ -2808,10 +2953,10 @@
         <v>66</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>107</v>
+        <v>86</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>7</v>
@@ -2826,31 +2971,29 @@
         <v>67</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>109</v>
+        <v>88</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>110</v>
+        <v>89</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F69" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F69" s="1"/>
       <c r="G69" s="1"/>
     </row>
-    <row r="70" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="70" spans="2:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B70" s="6">
         <v>68</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>340</v>
+        <v>90</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>341</v>
+        <v>91</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F70" s="1"/>
       <c r="G70" s="1"/>
@@ -2860,10 +3003,10 @@
         <v>69</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>112</v>
+        <v>93</v>
       </c>
       <c r="E71" s="1" t="s">
         <v>5</v>
@@ -2876,17 +3019,15 @@
         <v>70</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>113</v>
+        <v>332</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>114</v>
+        <v>333</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F72" s="1" t="s">
-        <v>27</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F72" s="1"/>
       <c r="G72" s="1"/>
     </row>
     <row r="73" spans="2:7" x14ac:dyDescent="0.35">
@@ -2894,10 +3035,10 @@
         <v>71</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>115</v>
+        <v>424</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>116</v>
+        <v>423</v>
       </c>
       <c r="E73" s="1" t="s">
         <v>5</v>
@@ -2910,10 +3051,10 @@
         <v>72</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>390</v>
+        <v>422</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>391</v>
+        <v>421</v>
       </c>
       <c r="E74" s="1" t="s">
         <v>5</v>
@@ -2926,10 +3067,10 @@
         <v>73</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>118</v>
+        <v>95</v>
       </c>
       <c r="E75" s="1" t="s">
         <v>5</v>
@@ -2942,10 +3083,10 @@
         <v>74</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>119</v>
+        <v>96</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>120</v>
+        <v>97</v>
       </c>
       <c r="E76" s="1" t="s">
         <v>5</v>
@@ -2958,10 +3099,10 @@
         <v>75</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>121</v>
+        <v>98</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>122</v>
+        <v>99</v>
       </c>
       <c r="E77" s="1" t="s">
         <v>5</v>
@@ -2974,13 +3115,13 @@
         <v>76</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>123</v>
+        <v>100</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>124</v>
+        <v>101</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F78" s="1"/>
       <c r="G78" s="1"/>
@@ -2990,10 +3131,10 @@
         <v>77</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>125</v>
+        <v>102</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>126</v>
+        <v>104</v>
       </c>
       <c r="E79" s="1" t="s">
         <v>5</v>
@@ -3006,10 +3147,10 @@
         <v>78</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>127</v>
+        <v>103</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>128</v>
+        <v>105</v>
       </c>
       <c r="E80" s="1" t="s">
         <v>5</v>
@@ -3022,13 +3163,13 @@
         <v>79</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>372</v>
+        <v>354</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>373</v>
+        <v>355</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F81" s="1"/>
       <c r="G81" s="1"/>
@@ -3038,16 +3179,16 @@
         <v>80</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>349</v>
+        <v>107</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>348</v>
+        <v>108</v>
       </c>
       <c r="E82" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="G82" s="1"/>
     </row>
@@ -3056,15 +3197,17 @@
         <v>81</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>129</v>
+        <v>398</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>130</v>
+        <v>397</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F83" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="G83" s="1"/>
     </row>
     <row r="84" spans="2:7" x14ac:dyDescent="0.35">
@@ -3072,10 +3215,10 @@
         <v>82</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>131</v>
+        <v>109</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>132</v>
+        <v>110</v>
       </c>
       <c r="E84" s="1" t="s">
         <v>7</v>
@@ -3090,13 +3233,13 @@
         <v>83</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>133</v>
+        <v>340</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>134</v>
+        <v>341</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F85" s="1"/>
       <c r="G85" s="1"/>
@@ -3106,17 +3249,15 @@
         <v>84</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>135</v>
+        <v>111</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>136</v>
+        <v>112</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F86" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F86" s="1"/>
       <c r="G86" s="1"/>
     </row>
     <row r="87" spans="2:7" x14ac:dyDescent="0.35">
@@ -3124,15 +3265,17 @@
         <v>85</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>356</v>
+        <v>113</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>357</v>
+        <v>114</v>
       </c>
       <c r="E87" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F87" s="1"/>
+      <c r="F87" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G87" s="1"/>
     </row>
     <row r="88" spans="2:7" x14ac:dyDescent="0.35">
@@ -3140,10 +3283,10 @@
         <v>86</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>138</v>
+        <v>116</v>
       </c>
       <c r="E88" s="1" t="s">
         <v>5</v>
@@ -3156,17 +3299,15 @@
         <v>87</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>361</v>
+        <v>426</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>362</v>
+        <v>425</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F89" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F89" s="1"/>
       <c r="G89" s="1"/>
     </row>
     <row r="90" spans="2:7" x14ac:dyDescent="0.35">
@@ -3174,10 +3315,10 @@
         <v>88</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>314</v>
+        <v>390</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>315</v>
+        <v>391</v>
       </c>
       <c r="E90" s="1" t="s">
         <v>5</v>
@@ -3190,10 +3331,10 @@
         <v>89</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>320</v>
+        <v>117</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>321</v>
+        <v>118</v>
       </c>
       <c r="E91" s="1" t="s">
         <v>5</v>
@@ -3206,17 +3347,15 @@
         <v>90</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>139</v>
+        <v>119</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F92" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F92" s="1"/>
       <c r="G92" s="1"/>
     </row>
     <row r="93" spans="2:7" x14ac:dyDescent="0.35">
@@ -3224,10 +3363,10 @@
         <v>91</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>322</v>
+        <v>121</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>323</v>
+        <v>122</v>
       </c>
       <c r="E93" s="1" t="s">
         <v>5</v>
@@ -3240,10 +3379,10 @@
         <v>92</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>141</v>
+        <v>123</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>142</v>
+        <v>124</v>
       </c>
       <c r="E94" s="1" t="s">
         <v>5</v>
@@ -3256,10 +3395,10 @@
         <v>93</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>306</v>
+        <v>125</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>307</v>
+        <v>126</v>
       </c>
       <c r="E95" s="1" t="s">
         <v>5</v>
@@ -3272,10 +3411,10 @@
         <v>94</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>144</v>
+        <v>128</v>
       </c>
       <c r="E96" s="1" t="s">
         <v>5</v>
@@ -3288,10 +3427,10 @@
         <v>95</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>145</v>
+        <v>372</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>146</v>
+        <v>373</v>
       </c>
       <c r="E97" s="1" t="s">
         <v>5</v>
@@ -3304,10 +3443,10 @@
         <v>96</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>147</v>
+        <v>349</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>148</v>
+        <v>348</v>
       </c>
       <c r="E98" s="1" t="s">
         <v>7</v>
@@ -3322,17 +3461,15 @@
         <v>97</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>149</v>
+        <v>129</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>150</v>
+        <v>130</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F99" s="1" t="s">
-        <v>27</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F99" s="1"/>
       <c r="G99" s="1"/>
     </row>
     <row r="100" spans="2:7" x14ac:dyDescent="0.35">
@@ -3340,17 +3477,15 @@
         <v>98</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>151</v>
+        <v>432</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>152</v>
+        <v>431</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F100" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F100" s="1"/>
       <c r="G100" s="1"/>
     </row>
     <row r="101" spans="2:7" x14ac:dyDescent="0.35">
@@ -3358,15 +3493,17 @@
         <v>99</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>153</v>
+        <v>131</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>154</v>
+        <v>132</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F101" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F101" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="G101" s="1"/>
     </row>
     <row r="102" spans="2:7" x14ac:dyDescent="0.35">
@@ -3374,13 +3511,13 @@
         <v>100</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>155</v>
+        <v>133</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>156</v>
+        <v>134</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F102" s="1"/>
       <c r="G102" s="1"/>
@@ -3390,15 +3527,17 @@
         <v>101</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>157</v>
+        <v>135</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>158</v>
+        <v>136</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F103" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F103" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="G103" s="1"/>
     </row>
     <row r="104" spans="2:7" x14ac:dyDescent="0.35">
@@ -3406,13 +3545,13 @@
         <v>102</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>159</v>
+        <v>356</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>160</v>
+        <v>357</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F104" s="1"/>
       <c r="G104" s="1"/>
@@ -3422,10 +3561,10 @@
         <v>103</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>328</v>
+        <v>137</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>329</v>
+        <v>138</v>
       </c>
       <c r="E105" s="1" t="s">
         <v>5</v>
@@ -3438,15 +3577,17 @@
         <v>104</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>324</v>
+        <v>361</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>327</v>
+        <v>362</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F106" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F106" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="G106" s="1"/>
     </row>
     <row r="107" spans="2:7" x14ac:dyDescent="0.35">
@@ -3454,17 +3595,15 @@
         <v>105</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="E107" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F107" s="1" t="s">
-        <v>27</v>
-      </c>
+      <c r="F107" s="1"/>
       <c r="G107" s="1"/>
     </row>
     <row r="108" spans="2:7" x14ac:dyDescent="0.35">
@@ -3472,33 +3611,33 @@
         <v>106</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>379</v>
+        <v>320</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>378</v>
+        <v>321</v>
       </c>
       <c r="E108" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F108" s="1"/>
-      <c r="G108" s="1" t="s">
-        <v>380</v>
-      </c>
+      <c r="G108" s="1"/>
     </row>
     <row r="109" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B109" s="6">
         <v>107</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>311</v>
+        <v>139</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>310</v>
+        <v>140</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F109" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F109" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="G109" s="1"/>
     </row>
     <row r="110" spans="2:7" x14ac:dyDescent="0.35">
@@ -3506,10 +3645,10 @@
         <v>108</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>308</v>
+        <v>322</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>309</v>
+        <v>323</v>
       </c>
       <c r="E110" s="1" t="s">
         <v>5</v>
@@ -3522,10 +3661,10 @@
         <v>109</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>367</v>
+        <v>141</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>368</v>
+        <v>142</v>
       </c>
       <c r="E111" s="1" t="s">
         <v>5</v>
@@ -3538,10 +3677,10 @@
         <v>110</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>161</v>
+        <v>306</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>162</v>
+        <v>307</v>
       </c>
       <c r="E112" s="1" t="s">
         <v>5</v>
@@ -3554,10 +3693,10 @@
         <v>111</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>163</v>
+        <v>143</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>164</v>
+        <v>144</v>
       </c>
       <c r="E113" s="1" t="s">
         <v>5</v>
@@ -3570,10 +3709,10 @@
         <v>112</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>165</v>
+        <v>145</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>166</v>
+        <v>146</v>
       </c>
       <c r="E114" s="1" t="s">
         <v>5</v>
@@ -3586,15 +3725,17 @@
         <v>113</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>167</v>
+        <v>434</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>168</v>
+        <v>433</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F115" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F115" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G115" s="1"/>
     </row>
     <row r="116" spans="2:7" x14ac:dyDescent="0.35">
@@ -3602,15 +3743,17 @@
         <v>114</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>169</v>
+        <v>147</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>170</v>
+        <v>148</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F116" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F116" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G116" s="1"/>
     </row>
     <row r="117" spans="2:7" x14ac:dyDescent="0.35">
@@ -3618,15 +3761,17 @@
         <v>115</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>336</v>
+        <v>149</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>171</v>
+        <v>150</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F117" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F117" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G117" s="1"/>
     </row>
     <row r="118" spans="2:7" x14ac:dyDescent="0.35">
@@ -3634,15 +3779,17 @@
         <v>116</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>172</v>
+        <v>151</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>173</v>
+        <v>152</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F118" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F118" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="G118" s="1"/>
     </row>
     <row r="119" spans="2:7" x14ac:dyDescent="0.35">
@@ -3650,17 +3797,15 @@
         <v>117</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>174</v>
+        <v>153</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>175</v>
+        <v>154</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F119" s="1" t="s">
-        <v>27</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F119" s="1"/>
       <c r="G119" s="1"/>
     </row>
     <row r="120" spans="2:7" x14ac:dyDescent="0.35">
@@ -3668,13 +3813,13 @@
         <v>118</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>176</v>
+        <v>155</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>177</v>
+        <v>156</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F120" s="1"/>
       <c r="G120" s="1"/>
@@ -3684,10 +3829,10 @@
         <v>119</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>178</v>
+        <v>157</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>179</v>
+        <v>158</v>
       </c>
       <c r="E121" s="1" t="s">
         <v>5</v>
@@ -3700,15 +3845,17 @@
         <v>120</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>180</v>
+        <v>405</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>181</v>
+        <v>406</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F122" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F122" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="G122" s="1"/>
     </row>
     <row r="123" spans="2:7" x14ac:dyDescent="0.35">
@@ -3716,10 +3863,10 @@
         <v>121</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>182</v>
+        <v>159</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>183</v>
+        <v>160</v>
       </c>
       <c r="E123" s="1" t="s">
         <v>5</v>
@@ -3732,10 +3879,10 @@
         <v>122</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>184</v>
+        <v>328</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>185</v>
+        <v>329</v>
       </c>
       <c r="E124" s="1" t="s">
         <v>5</v>
@@ -3748,10 +3895,10 @@
         <v>123</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>186</v>
+        <v>324</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>187</v>
+        <v>327</v>
       </c>
       <c r="E125" s="1" t="s">
         <v>5</v>
@@ -3764,15 +3911,17 @@
         <v>124</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>188</v>
+        <v>316</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>189</v>
+        <v>317</v>
       </c>
       <c r="E126" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F126" s="1"/>
+      <c r="F126" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G126" s="1"/>
     </row>
     <row r="127" spans="2:7" x14ac:dyDescent="0.35">
@@ -3780,26 +3929,28 @@
         <v>125</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>337</v>
+        <v>378</v>
       </c>
       <c r="E127" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F127" s="1"/>
-      <c r="G127" s="1"/>
+      <c r="G127" s="1" t="s">
+        <v>380</v>
+      </c>
     </row>
     <row r="128" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B128" s="6">
         <v>126</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>371</v>
+        <v>311</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>191</v>
+        <v>310</v>
       </c>
       <c r="E128" s="1" t="s">
         <v>5</v>
@@ -3812,10 +3963,10 @@
         <v>127</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>190</v>
+        <v>308</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>191</v>
+        <v>309</v>
       </c>
       <c r="E129" s="1" t="s">
         <v>5</v>
@@ -3828,10 +3979,10 @@
         <v>128</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>334</v>
+        <v>367</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>335</v>
+        <v>368</v>
       </c>
       <c r="E130" s="1" t="s">
         <v>5</v>
@@ -3844,17 +3995,15 @@
         <v>129</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>374</v>
+        <v>161</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>375</v>
+        <v>162</v>
       </c>
       <c r="E131" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F131" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F131" s="1"/>
       <c r="G131" s="1"/>
     </row>
     <row r="132" spans="2:7" x14ac:dyDescent="0.35">
@@ -3862,17 +4011,15 @@
         <v>130</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>192</v>
+        <v>163</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>193</v>
+        <v>164</v>
       </c>
       <c r="E132" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F132" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F132" s="1"/>
       <c r="G132" s="1"/>
     </row>
     <row r="133" spans="2:7" x14ac:dyDescent="0.35">
@@ -3880,10 +4027,10 @@
         <v>131</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>194</v>
+        <v>165</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>195</v>
+        <v>166</v>
       </c>
       <c r="E133" s="1" t="s">
         <v>5</v>
@@ -3896,10 +4043,10 @@
         <v>132</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>196</v>
+        <v>167</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>197</v>
+        <v>168</v>
       </c>
       <c r="E134" s="1" t="s">
         <v>5</v>
@@ -3912,10 +4059,10 @@
         <v>133</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>347</v>
+        <v>169</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>346</v>
+        <v>170</v>
       </c>
       <c r="E135" s="1" t="s">
         <v>5</v>
@@ -3928,10 +4075,10 @@
         <v>134</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>198</v>
+        <v>336</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>199</v>
+        <v>171</v>
       </c>
       <c r="E136" s="1" t="s">
         <v>5</v>
@@ -3944,10 +4091,10 @@
         <v>135</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>200</v>
+        <v>172</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>201</v>
+        <v>173</v>
       </c>
       <c r="E137" s="1" t="s">
         <v>5</v>
@@ -3960,13 +4107,13 @@
         <v>136</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>202</v>
+        <v>440</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>203</v>
+        <v>439</v>
       </c>
       <c r="E138" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F138" s="1"/>
       <c r="G138" s="1"/>
@@ -3976,10 +4123,10 @@
         <v>137</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>358</v>
+        <v>174</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>359</v>
+        <v>175</v>
       </c>
       <c r="E139" s="1" t="s">
         <v>7</v>
@@ -3994,10 +4141,10 @@
         <v>138</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>204</v>
+        <v>176</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>205</v>
+        <v>177</v>
       </c>
       <c r="E140" s="1" t="s">
         <v>5</v>
@@ -4010,10 +4157,10 @@
         <v>139</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>206</v>
+        <v>178</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>207</v>
+        <v>179</v>
       </c>
       <c r="E141" s="1" t="s">
         <v>5</v>
@@ -4026,10 +4173,10 @@
         <v>140</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>208</v>
+        <v>180</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>209</v>
+        <v>181</v>
       </c>
       <c r="E142" s="1" t="s">
         <v>5</v>
@@ -4042,17 +4189,15 @@
         <v>141</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>210</v>
+        <v>182</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>211</v>
+        <v>183</v>
       </c>
       <c r="E143" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F143" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F143" s="1"/>
       <c r="G143" s="1"/>
     </row>
     <row r="144" spans="2:7" x14ac:dyDescent="0.35">
@@ -4060,10 +4205,10 @@
         <v>142</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>212</v>
+        <v>184</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>213</v>
+        <v>185</v>
       </c>
       <c r="E144" s="1" t="s">
         <v>5</v>
@@ -4076,10 +4221,10 @@
         <v>143</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>214</v>
+        <v>186</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>215</v>
+        <v>187</v>
       </c>
       <c r="E145" s="1" t="s">
         <v>5</v>
@@ -4092,17 +4237,15 @@
         <v>144</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>216</v>
+        <v>188</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>217</v>
+        <v>189</v>
       </c>
       <c r="E146" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F146" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F146" s="1"/>
       <c r="G146" s="1"/>
     </row>
     <row r="147" spans="2:7" x14ac:dyDescent="0.35">
@@ -4110,77 +4253,63 @@
         <v>145</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>218</v>
+        <v>377</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>220</v>
+        <v>337</v>
       </c>
       <c r="E147" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F147" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G147" s="1" t="s">
-        <v>30</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F147" s="1"/>
+      <c r="G147" s="1"/>
     </row>
     <row r="148" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B148" s="6">
         <v>146</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>219</v>
+        <v>371</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>221</v>
+        <v>191</v>
       </c>
       <c r="E148" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F148" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G148" s="1" t="s">
-        <v>30</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F148" s="1"/>
+      <c r="G148" s="1"/>
     </row>
     <row r="149" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B149" s="6">
         <v>147</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>222</v>
+        <v>190</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>223</v>
+        <v>191</v>
       </c>
       <c r="E149" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F149" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G149" s="1" t="s">
-        <v>297</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F149" s="1"/>
+      <c r="G149" s="1"/>
     </row>
     <row r="150" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B150" s="6">
         <v>148</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>224</v>
+        <v>334</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>225</v>
+        <v>335</v>
       </c>
       <c r="E150" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F150" s="1" t="s">
-        <v>27</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F150" s="1"/>
       <c r="G150" s="1"/>
     </row>
     <row r="151" spans="2:7" x14ac:dyDescent="0.35">
@@ -4188,15 +4317,17 @@
         <v>149</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>226</v>
+        <v>374</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>227</v>
+        <v>375</v>
       </c>
       <c r="E151" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F151" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F151" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="G151" s="1"/>
     </row>
     <row r="152" spans="2:7" x14ac:dyDescent="0.35">
@@ -4204,15 +4335,17 @@
         <v>150</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>228</v>
+        <v>192</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>229</v>
+        <v>193</v>
       </c>
       <c r="E152" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F152" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F152" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="G152" s="1"/>
     </row>
     <row r="153" spans="2:7" x14ac:dyDescent="0.35">
@@ -4220,17 +4353,15 @@
         <v>151</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>230</v>
+        <v>194</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>231</v>
+        <v>195</v>
       </c>
       <c r="E153" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F153" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F153" s="1"/>
       <c r="G153" s="1"/>
     </row>
     <row r="154" spans="2:7" x14ac:dyDescent="0.35">
@@ -4238,17 +4369,15 @@
         <v>152</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>233</v>
+        <v>196</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>232</v>
+        <v>197</v>
       </c>
       <c r="E154" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F154" s="1" t="s">
-        <v>27</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F154" s="1"/>
       <c r="G154" s="1"/>
     </row>
     <row r="155" spans="2:7" x14ac:dyDescent="0.35">
@@ -4256,10 +4385,10 @@
         <v>153</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>234</v>
+        <v>347</v>
       </c>
       <c r="D155" s="1" t="s">
-        <v>235</v>
+        <v>346</v>
       </c>
       <c r="E155" s="1" t="s">
         <v>5</v>
@@ -4272,10 +4401,10 @@
         <v>154</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>236</v>
+        <v>198</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>237</v>
+        <v>199</v>
       </c>
       <c r="E156" s="1" t="s">
         <v>5</v>
@@ -4288,10 +4417,10 @@
         <v>155</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>238</v>
+        <v>200</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>239</v>
+        <v>201</v>
       </c>
       <c r="E157" s="1" t="s">
         <v>5</v>
@@ -4304,13 +4433,13 @@
         <v>156</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>240</v>
+        <v>202</v>
       </c>
       <c r="D158" s="1" t="s">
-        <v>241</v>
+        <v>203</v>
       </c>
       <c r="E158" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F158" s="1"/>
       <c r="G158" s="1"/>
@@ -4320,10 +4449,10 @@
         <v>157</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>242</v>
+        <v>358</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>243</v>
+        <v>359</v>
       </c>
       <c r="E159" s="1" t="s">
         <v>7</v>
@@ -4338,13 +4467,13 @@
         <v>158</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>244</v>
+        <v>204</v>
       </c>
       <c r="D160" s="1" t="s">
-        <v>245</v>
+        <v>205</v>
       </c>
       <c r="E160" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F160" s="1"/>
       <c r="G160" s="1"/>
@@ -4354,10 +4483,10 @@
         <v>159</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>381</v>
+        <v>206</v>
       </c>
       <c r="D161" s="1" t="s">
-        <v>382</v>
+        <v>207</v>
       </c>
       <c r="E161" s="1" t="s">
         <v>5</v>
@@ -4370,10 +4499,10 @@
         <v>160</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>246</v>
+        <v>208</v>
       </c>
       <c r="D162" s="1" t="s">
-        <v>247</v>
+        <v>209</v>
       </c>
       <c r="E162" s="1" t="s">
         <v>5</v>
@@ -4386,15 +4515,17 @@
         <v>161</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>248</v>
+        <v>210</v>
       </c>
       <c r="D163" s="1" t="s">
-        <v>249</v>
+        <v>211</v>
       </c>
       <c r="E163" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F163" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F163" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="G163" s="1"/>
     </row>
     <row r="164" spans="2:7" x14ac:dyDescent="0.35">
@@ -4402,10 +4533,10 @@
         <v>162</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>250</v>
+        <v>212</v>
       </c>
       <c r="D164" s="1" t="s">
-        <v>251</v>
+        <v>213</v>
       </c>
       <c r="E164" s="1" t="s">
         <v>5</v>
@@ -4418,10 +4549,10 @@
         <v>163</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>252</v>
+        <v>214</v>
       </c>
       <c r="D165" s="1" t="s">
-        <v>253</v>
+        <v>215</v>
       </c>
       <c r="E165" s="1" t="s">
         <v>5</v>
@@ -4434,15 +4565,17 @@
         <v>164</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>353</v>
+        <v>216</v>
       </c>
       <c r="D166" s="1" t="s">
-        <v>352</v>
+        <v>217</v>
       </c>
       <c r="E166" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F166" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F166" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="G166" s="1"/>
     </row>
     <row r="167" spans="2:7" x14ac:dyDescent="0.35">
@@ -4450,51 +4583,59 @@
         <v>165</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>254</v>
+        <v>218</v>
       </c>
       <c r="D167" s="1" t="s">
-        <v>255</v>
+        <v>220</v>
       </c>
       <c r="E167" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F167" s="1"/>
-      <c r="G167" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F167" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G167" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="168" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B168" s="6">
         <v>166</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>383</v>
+        <v>219</v>
       </c>
       <c r="D168" s="1" t="s">
-        <v>384</v>
+        <v>221</v>
       </c>
       <c r="E168" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F168" s="1"/>
-      <c r="G168" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F168" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G168" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="169" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B169" s="6">
         <v>167</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>385</v>
+        <v>222</v>
       </c>
       <c r="D169" s="1" t="s">
-        <v>386</v>
+        <v>223</v>
       </c>
       <c r="E169" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F169" s="1" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="G169" s="1" t="s">
-        <v>387</v>
+        <v>297</v>
       </c>
     </row>
     <row r="170" spans="2:7" x14ac:dyDescent="0.35">
@@ -4502,15 +4643,17 @@
         <v>168</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>256</v>
+        <v>224</v>
       </c>
       <c r="D170" s="1" t="s">
-        <v>257</v>
+        <v>225</v>
       </c>
       <c r="E170" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F170" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F170" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G170" s="1"/>
     </row>
     <row r="171" spans="2:7" x14ac:dyDescent="0.35">
@@ -4518,17 +4661,15 @@
         <v>169</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>258</v>
+        <v>226</v>
       </c>
       <c r="D171" s="1" t="s">
-        <v>259</v>
+        <v>227</v>
       </c>
       <c r="E171" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F171" s="1" t="s">
-        <v>27</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F171" s="1"/>
       <c r="G171" s="1"/>
     </row>
     <row r="172" spans="2:7" x14ac:dyDescent="0.35">
@@ -4536,10 +4677,10 @@
         <v>170</v>
       </c>
       <c r="C172" s="1" t="s">
-        <v>369</v>
+        <v>228</v>
       </c>
       <c r="D172" s="1" t="s">
-        <v>370</v>
+        <v>229</v>
       </c>
       <c r="E172" s="1" t="s">
         <v>5</v>
@@ -4552,15 +4693,17 @@
         <v>171</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>260</v>
+        <v>230</v>
       </c>
       <c r="D173" s="1" t="s">
-        <v>261</v>
+        <v>231</v>
       </c>
       <c r="E173" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F173" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F173" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="G173" s="1"/>
     </row>
     <row r="174" spans="2:7" x14ac:dyDescent="0.35">
@@ -4568,15 +4711,17 @@
         <v>172</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>262</v>
+        <v>233</v>
       </c>
       <c r="D174" s="1" t="s">
-        <v>263</v>
+        <v>232</v>
       </c>
       <c r="E174" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F174" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F174" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G174" s="1"/>
     </row>
     <row r="175" spans="2:7" x14ac:dyDescent="0.35">
@@ -4584,17 +4729,15 @@
         <v>173</v>
       </c>
       <c r="C175" s="1" t="s">
-        <v>264</v>
+        <v>234</v>
       </c>
       <c r="D175" s="1" t="s">
-        <v>265</v>
+        <v>235</v>
       </c>
       <c r="E175" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F175" s="1" t="s">
-        <v>27</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F175" s="1"/>
       <c r="G175" s="1"/>
     </row>
     <row r="176" spans="2:7" x14ac:dyDescent="0.35">
@@ -4602,10 +4745,10 @@
         <v>174</v>
       </c>
       <c r="C176" s="1" t="s">
-        <v>266</v>
+        <v>408</v>
       </c>
       <c r="D176" s="1" t="s">
-        <v>267</v>
+        <v>407</v>
       </c>
       <c r="E176" s="1" t="s">
         <v>5</v>
@@ -4618,10 +4761,10 @@
         <v>175</v>
       </c>
       <c r="C177" s="1" t="s">
-        <v>268</v>
+        <v>236</v>
       </c>
       <c r="D177" s="1" t="s">
-        <v>269</v>
+        <v>237</v>
       </c>
       <c r="E177" s="1" t="s">
         <v>5</v>
@@ -4634,10 +4777,10 @@
         <v>176</v>
       </c>
       <c r="C178" s="1" t="s">
-        <v>270</v>
+        <v>238</v>
       </c>
       <c r="D178" s="1" t="s">
-        <v>271</v>
+        <v>239</v>
       </c>
       <c r="E178" s="1" t="s">
         <v>5</v>
@@ -4650,10 +4793,10 @@
         <v>177</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>272</v>
+        <v>240</v>
       </c>
       <c r="D179" s="1" t="s">
-        <v>273</v>
+        <v>241</v>
       </c>
       <c r="E179" s="1" t="s">
         <v>5</v>
@@ -4666,15 +4809,17 @@
         <v>178</v>
       </c>
       <c r="C180" s="1" t="s">
-        <v>274</v>
+        <v>242</v>
       </c>
       <c r="D180" s="1" t="s">
-        <v>275</v>
+        <v>243</v>
       </c>
       <c r="E180" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F180" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F180" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G180" s="1"/>
     </row>
     <row r="181" spans="2:7" x14ac:dyDescent="0.35">
@@ -4682,13 +4827,13 @@
         <v>179</v>
       </c>
       <c r="C181" s="1" t="s">
-        <v>10</v>
+        <v>244</v>
       </c>
       <c r="D181" s="1" t="s">
-        <v>276</v>
+        <v>245</v>
       </c>
       <c r="E181" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F181" s="1"/>
       <c r="G181" s="1"/>
@@ -4698,13 +4843,13 @@
         <v>180</v>
       </c>
       <c r="C182" s="1" t="s">
-        <v>325</v>
+        <v>381</v>
       </c>
       <c r="D182" s="1" t="s">
-        <v>326</v>
+        <v>382</v>
       </c>
       <c r="E182" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F182" s="1"/>
       <c r="G182" s="1"/>
@@ -4714,17 +4859,15 @@
         <v>181</v>
       </c>
       <c r="C183" s="1" t="s">
-        <v>277</v>
+        <v>246</v>
       </c>
       <c r="D183" s="1" t="s">
-        <v>278</v>
+        <v>247</v>
       </c>
       <c r="E183" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F183" s="1" t="s">
-        <v>27</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F183" s="1"/>
       <c r="G183" s="1"/>
     </row>
     <row r="184" spans="2:7" x14ac:dyDescent="0.35">
@@ -4732,10 +4875,10 @@
         <v>182</v>
       </c>
       <c r="C184" s="1" t="s">
-        <v>279</v>
+        <v>248</v>
       </c>
       <c r="D184" s="1" t="s">
-        <v>280</v>
+        <v>249</v>
       </c>
       <c r="E184" s="1" t="s">
         <v>5</v>
@@ -4748,13 +4891,13 @@
         <v>183</v>
       </c>
       <c r="C185" s="1" t="s">
-        <v>281</v>
+        <v>250</v>
       </c>
       <c r="D185" s="1" t="s">
-        <v>282</v>
+        <v>251</v>
       </c>
       <c r="E185" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F185" s="1"/>
       <c r="G185" s="1"/>
@@ -4764,17 +4907,15 @@
         <v>184</v>
       </c>
       <c r="C186" s="1" t="s">
-        <v>283</v>
+        <v>252</v>
       </c>
       <c r="D186" s="1" t="s">
-        <v>286</v>
+        <v>253</v>
       </c>
       <c r="E186" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F186" s="1" t="s">
-        <v>27</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F186" s="1"/>
       <c r="G186" s="1"/>
     </row>
     <row r="187" spans="2:7" x14ac:dyDescent="0.35">
@@ -4782,17 +4923,15 @@
         <v>185</v>
       </c>
       <c r="C187" s="1" t="s">
-        <v>284</v>
+        <v>353</v>
       </c>
       <c r="D187" s="1" t="s">
-        <v>287</v>
+        <v>352</v>
       </c>
       <c r="E187" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F187" s="1" t="s">
-        <v>27</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F187" s="1"/>
       <c r="G187" s="1"/>
     </row>
     <row r="188" spans="2:7" x14ac:dyDescent="0.35">
@@ -4800,17 +4939,15 @@
         <v>186</v>
       </c>
       <c r="C188" s="1" t="s">
-        <v>285</v>
+        <v>254</v>
       </c>
       <c r="D188" s="1" t="s">
-        <v>288</v>
+        <v>255</v>
       </c>
       <c r="E188" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F188" s="1" t="s">
-        <v>27</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F188" s="1"/>
       <c r="G188" s="1"/>
     </row>
     <row r="189" spans="2:7" x14ac:dyDescent="0.35">
@@ -4818,10 +4955,10 @@
         <v>187</v>
       </c>
       <c r="C189" s="1" t="s">
-        <v>289</v>
+        <v>383</v>
       </c>
       <c r="D189" s="1" t="s">
-        <v>290</v>
+        <v>384</v>
       </c>
       <c r="E189" s="1" t="s">
         <v>5</v>
@@ -4834,28 +4971,30 @@
         <v>188</v>
       </c>
       <c r="C190" s="1" t="s">
-        <v>291</v>
+        <v>385</v>
       </c>
       <c r="D190" s="1" t="s">
-        <v>292</v>
+        <v>386</v>
       </c>
       <c r="E190" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F190" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G190" s="1"/>
+        <v>15</v>
+      </c>
+      <c r="G190" s="1" t="s">
+        <v>387</v>
+      </c>
     </row>
     <row r="191" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B191" s="6">
         <v>189</v>
       </c>
       <c r="C191" s="1" t="s">
-        <v>293</v>
+        <v>256</v>
       </c>
       <c r="D191" s="1" t="s">
-        <v>294</v>
+        <v>257</v>
       </c>
       <c r="E191" s="1" t="s">
         <v>5</v>
@@ -4868,55 +5007,439 @@
         <v>190</v>
       </c>
       <c r="C192" s="1" t="s">
-        <v>295</v>
+        <v>258</v>
       </c>
       <c r="D192" s="1" t="s">
-        <v>296</v>
+        <v>259</v>
       </c>
       <c r="E192" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F192" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F192" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G192" s="1"/>
     </row>
     <row r="193" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B193" s="6"/>
-      <c r="C193" s="1"/>
-      <c r="D193" s="1"/>
-      <c r="E193" s="1"/>
+      <c r="B193" s="6">
+        <v>191</v>
+      </c>
+      <c r="C193" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="D193" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="E193" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F193" s="1"/>
       <c r="G193" s="1"/>
     </row>
     <row r="194" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B194" s="6"/>
-      <c r="C194" s="1"/>
-      <c r="D194" s="1"/>
-      <c r="E194" s="1"/>
+      <c r="B194" s="6">
+        <v>192</v>
+      </c>
+      <c r="C194" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="D194" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="E194" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F194" s="1"/>
       <c r="G194" s="1"/>
     </row>
     <row r="195" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B195" s="6"/>
-      <c r="C195" s="1"/>
-      <c r="D195" s="1"/>
-      <c r="E195" s="1"/>
+      <c r="B195" s="6">
+        <v>193</v>
+      </c>
+      <c r="C195" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="D195" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="E195" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F195" s="1"/>
       <c r="G195" s="1"/>
     </row>
     <row r="196" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B196" s="6"/>
-      <c r="C196" s="1"/>
-      <c r="D196" s="1"/>
-      <c r="E196" s="1"/>
-      <c r="F196" s="1"/>
+      <c r="B196" s="6">
+        <v>194</v>
+      </c>
+      <c r="C196" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="D196" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="E196" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F196" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G196" s="1"/>
+    </row>
+    <row r="197" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B197" s="6">
+        <v>195</v>
+      </c>
+      <c r="C197" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="D197" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="E197" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F197" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G197" s="1"/>
+    </row>
+    <row r="198" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B198" s="6">
+        <v>196</v>
+      </c>
+      <c r="C198" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="D198" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="E198" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F198" s="1"/>
+      <c r="G198" s="1"/>
+    </row>
+    <row r="199" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B199" s="6">
+        <v>197</v>
+      </c>
+      <c r="C199" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="D199" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="E199" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F199" s="1"/>
+      <c r="G199" s="1"/>
+    </row>
+    <row r="200" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B200" s="6">
+        <v>198</v>
+      </c>
+      <c r="C200" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="D200" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="E200" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F200" s="1"/>
+      <c r="G200" s="1"/>
+    </row>
+    <row r="201" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B201" s="6">
+        <v>199</v>
+      </c>
+      <c r="C201" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="D201" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="E201" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F201" s="1"/>
+      <c r="G201" s="1"/>
+    </row>
+    <row r="202" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B202" s="6">
+        <v>200</v>
+      </c>
+      <c r="C202" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="D202" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="E202" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F202" s="1"/>
+      <c r="G202" s="1"/>
+    </row>
+    <row r="203" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B203" s="6">
+        <v>201</v>
+      </c>
+      <c r="C203" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D203" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="E203" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F203" s="1"/>
+      <c r="G203" s="1"/>
+    </row>
+    <row r="204" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B204" s="6">
+        <v>202</v>
+      </c>
+      <c r="C204" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="D204" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="E204" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F204" s="1"/>
+      <c r="G204" s="1"/>
+    </row>
+    <row r="205" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B205" s="6">
+        <v>203</v>
+      </c>
+      <c r="C205" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="D205" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="E205" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F205" s="1"/>
+      <c r="G205" s="1"/>
+    </row>
+    <row r="206" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B206" s="6">
+        <v>204</v>
+      </c>
+      <c r="C206" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="D206" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="E206" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F206" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G206" s="1"/>
+    </row>
+    <row r="207" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B207" s="6">
+        <v>205</v>
+      </c>
+      <c r="C207" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="D207" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="E207" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F207" s="1"/>
+      <c r="G207" s="1"/>
+    </row>
+    <row r="208" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B208" s="6">
+        <v>206</v>
+      </c>
+      <c r="C208" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="D208" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="E208" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F208" s="1"/>
+      <c r="G208" s="1"/>
+    </row>
+    <row r="209" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B209" s="6">
+        <v>207</v>
+      </c>
+      <c r="C209" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="D209" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="E209" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F209" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G209" s="1"/>
+    </row>
+    <row r="210" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B210" s="6">
+        <v>208</v>
+      </c>
+      <c r="C210" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="D210" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="E210" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F210" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G210" s="1"/>
+    </row>
+    <row r="211" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B211" s="6">
+        <v>209</v>
+      </c>
+      <c r="C211" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="D211" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="E211" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F211" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G211" s="1"/>
+    </row>
+    <row r="212" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B212" s="6">
+        <v>210</v>
+      </c>
+      <c r="C212" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="D212" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="E212" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F212" s="1"/>
+      <c r="G212" s="1"/>
+    </row>
+    <row r="213" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B213" s="6">
+        <v>211</v>
+      </c>
+      <c r="C213" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="D213" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="E213" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F213" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G213" s="1"/>
+    </row>
+    <row r="214" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B214" s="6">
+        <v>212</v>
+      </c>
+      <c r="C214" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="D214" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="E214" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F214" s="1"/>
+      <c r="G214" s="1"/>
+    </row>
+    <row r="215" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B215" s="6">
+        <v>213</v>
+      </c>
+      <c r="C215" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="D215" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="E215" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F215" s="1"/>
+      <c r="G215" s="1"/>
+    </row>
+    <row r="216" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B216" s="6"/>
+      <c r="C216" s="1"/>
+      <c r="D216" s="1"/>
+      <c r="E216" s="1"/>
+      <c r="F216" s="1"/>
+      <c r="G216" s="1"/>
+    </row>
+    <row r="217" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B217" s="6"/>
+      <c r="C217" s="1"/>
+      <c r="D217" s="1"/>
+      <c r="E217" s="1"/>
+      <c r="F217" s="1"/>
+      <c r="G217" s="1"/>
+    </row>
+    <row r="218" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B218" s="6"/>
+      <c r="C218" s="1"/>
+      <c r="D218" s="1"/>
+      <c r="E218" s="1"/>
+      <c r="F218" s="1"/>
+      <c r="G218" s="1"/>
+    </row>
+    <row r="219" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B219" s="6"/>
+      <c r="C219" s="1"/>
+      <c r="D219" s="1"/>
+      <c r="E219" s="1"/>
+      <c r="F219" s="1"/>
+      <c r="G219" s="1"/>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E192" xr:uid="{7E8CE32C-29D1-4006-9E0F-69B72A0F4378}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E215" xr:uid="{7E8CE32C-29D1-4006-9E0F-69B72A0F4378}">
       <formula1>"[Application],[Directory],[Script]"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F196" xr:uid="{A5D947FB-5606-4B36-88C5-81CC2B61C636}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F219" xr:uid="{A5D947FB-5606-4B36-88C5-81CC2B61C636}">
       <formula1>"[bat],[vbs]"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Update before New Windows 2025-02-14-18.05.31
</commit_message>
<xml_diff>
--- a/Database/Run_shortcut_creator_aliases.xlsx
+++ b/Database/Run_shortcut_creator_aliases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\player-1\Documents\Windows-Git-Repos\win-t\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{087ABB4F-017C-4785-9947-20A0C65C1912}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49E14D03-F0FC-4C3E-9A17-028B83C6E0A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14625" windowHeight="15585" xr2:uid="{D65865D6-BB34-410C-8183-31ED199784FF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D65865D6-BB34-410C-8183-31ED199784FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Run Shortcut Creator Aliases" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="441">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="445">
   <si>
     <t>Number</t>
   </si>
@@ -318,9 +318,6 @@
     <t>eh</t>
   </si>
   <si>
-    <t xml:space="preserve">Espanso </t>
-  </si>
-  <si>
     <t>ep</t>
   </si>
   <si>
@@ -1381,6 +1378,21 @@
   </si>
   <si>
     <t>win-ps2exe</t>
+  </si>
+  <si>
+    <t>ss</t>
+  </si>
+  <si>
+    <t>Start Screen (Start-Desktop-PowerPoint-File-Quickly.exe)</t>
+  </si>
+  <si>
+    <t>ee</t>
+  </si>
+  <si>
+    <t>Easyworship Ewsx (Start-Desktop-EasyWorship-File-Quickly.exe)</t>
+  </si>
+  <si>
+    <t>Espanso Start</t>
   </si>
 </sst>
 </file>
@@ -1812,10 +1824,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58A033C2-67FB-408D-B72B-8C45836FCF74}">
-  <dimension ref="B2:G219"/>
+  <dimension ref="B2:G221"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A120" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
-      <selection activeCell="E138" sqref="E138"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B200" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
+      <selection activeCell="N181" sqref="N181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -1851,7 +1863,7 @@
     </row>
     <row r="3" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="6" cm="1">
-        <f t="array" ref="B3:B215">_xlfn.SEQUENCE(COUNTA(C:C)-1)</f>
+        <f t="array" ref="B3:B217">_xlfn.SEQUENCE(COUNTA(C:C)-1)</f>
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -1871,10 +1883,10 @@
         <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>6</v>
@@ -1903,10 +1915,10 @@
         <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>342</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>343</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>5</v>
@@ -1919,10 +1931,10 @@
         <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>312</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>313</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>7</v>
@@ -1958,7 +1970,7 @@
         <v>17</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>7</v>
@@ -1967,7 +1979,7 @@
         <v>15</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="10" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
@@ -1991,7 +2003,7 @@
         <v>9</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>20</v>
@@ -2059,10 +2071,10 @@
         <v>13</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>344</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>345</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>7</v>
@@ -2075,10 +2087,10 @@
         <v>14</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>395</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>396</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>7</v>
@@ -2115,10 +2127,10 @@
         <v>16</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>5</v>
@@ -2131,10 +2143,10 @@
         <v>17</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>5</v>
@@ -2147,10 +2159,10 @@
         <v>18</v>
       </c>
       <c r="C20" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>429</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>430</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>5</v>
@@ -2195,10 +2207,10 @@
         <v>21</v>
       </c>
       <c r="C23" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>409</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>410</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>5</v>
@@ -2279,10 +2291,10 @@
         <v>26</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>5</v>
@@ -2331,10 +2343,10 @@
         <v>29</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>5</v>
@@ -2349,10 +2361,10 @@
         <v>30</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>5</v>
@@ -2365,10 +2377,10 @@
         <v>31</v>
       </c>
       <c r="C33" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="D33" s="1" t="s">
         <v>417</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>418</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>5</v>
@@ -2381,10 +2393,10 @@
         <v>32</v>
       </c>
       <c r="C34" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="D34" s="1" t="s">
         <v>301</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>302</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>6</v>
@@ -2397,10 +2409,10 @@
         <v>33</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>5</v>
@@ -2413,10 +2425,10 @@
         <v>34</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>5</v>
@@ -2429,10 +2441,10 @@
         <v>35</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>5</v>
@@ -2445,10 +2457,10 @@
         <v>36</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>5</v>
@@ -2461,7 +2473,7 @@
         <v>37</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>47</v>
@@ -2479,7 +2491,7 @@
         <v>38</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>48</v>
@@ -2511,10 +2523,10 @@
         <v>40</v>
       </c>
       <c r="C42" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="D42" s="1" t="s">
         <v>303</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>304</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>5</v>
@@ -2613,10 +2625,10 @@
         <v>46</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>5</v>
@@ -2629,10 +2641,10 @@
         <v>47</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>5</v>
@@ -2645,10 +2657,10 @@
         <v>48</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>5</v>
@@ -2695,7 +2707,7 @@
         <v>51</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>64</v>
@@ -2763,10 +2775,10 @@
         <v>55</v>
       </c>
       <c r="C57" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="D57" s="1" t="s">
         <v>338</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>339</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>5</v>
@@ -2797,10 +2809,10 @@
         <v>57</v>
       </c>
       <c r="C59" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="D59" s="1" t="s">
         <v>299</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>300</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>6</v>
@@ -2867,10 +2879,10 @@
         <v>61</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>5</v>
@@ -2901,10 +2913,10 @@
         <v>63</v>
       </c>
       <c r="C65" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="D65" s="1" t="s">
         <v>388</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>389</v>
       </c>
       <c r="E65" s="1" t="s">
         <v>7</v>
@@ -2935,17 +2947,15 @@
         <v>65</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>84</v>
+        <v>443</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>85</v>
+        <v>442</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F67" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F67" s="1"/>
       <c r="G67" s="1"/>
     </row>
     <row r="68" spans="2:7" x14ac:dyDescent="0.35">
@@ -2953,10 +2963,10 @@
         <v>66</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>7</v>
@@ -2971,26 +2981,28 @@
         <v>67</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>88</v>
+        <v>444</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F69" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="G69" s="1"/>
     </row>
-    <row r="70" spans="2:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B70" s="6">
         <v>68</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E70" s="1" t="s">
         <v>5</v>
@@ -2998,15 +3010,15 @@
       <c r="F70" s="1"/>
       <c r="G70" s="1"/>
     </row>
-    <row r="71" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="71" spans="2:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B71" s="6">
         <v>69</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E71" s="1" t="s">
         <v>5</v>
@@ -3019,10 +3031,10 @@
         <v>70</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>332</v>
+        <v>91</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>333</v>
+        <v>92</v>
       </c>
       <c r="E72" s="1" t="s">
         <v>5</v>
@@ -3035,10 +3047,10 @@
         <v>71</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>424</v>
+        <v>331</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>423</v>
+        <v>332</v>
       </c>
       <c r="E73" s="1" t="s">
         <v>5</v>
@@ -3051,10 +3063,10 @@
         <v>72</v>
       </c>
       <c r="C74" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="D74" s="1" t="s">
         <v>422</v>
-      </c>
-      <c r="D74" s="1" t="s">
-        <v>421</v>
       </c>
       <c r="E74" s="1" t="s">
         <v>5</v>
@@ -3067,10 +3079,10 @@
         <v>73</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>94</v>
+        <v>421</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>95</v>
+        <v>420</v>
       </c>
       <c r="E75" s="1" t="s">
         <v>5</v>
@@ -3083,10 +3095,10 @@
         <v>74</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E76" s="1" t="s">
         <v>5</v>
@@ -3099,10 +3111,10 @@
         <v>75</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E77" s="1" t="s">
         <v>5</v>
@@ -3115,13 +3127,13 @@
         <v>76</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F78" s="1"/>
       <c r="G78" s="1"/>
@@ -3131,13 +3143,13 @@
         <v>77</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F79" s="1"/>
       <c r="G79" s="1"/>
@@ -3147,10 +3159,10 @@
         <v>78</v>
       </c>
       <c r="C80" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D80" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="D80" s="1" t="s">
-        <v>105</v>
       </c>
       <c r="E80" s="1" t="s">
         <v>5</v>
@@ -3163,13 +3175,13 @@
         <v>79</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>354</v>
+        <v>102</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>355</v>
+        <v>104</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F81" s="1"/>
       <c r="G81" s="1"/>
@@ -3179,17 +3191,15 @@
         <v>80</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>107</v>
+        <v>353</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>108</v>
+        <v>354</v>
       </c>
       <c r="E82" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F82" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="F82" s="1"/>
       <c r="G82" s="1"/>
     </row>
     <row r="83" spans="2:7" x14ac:dyDescent="0.35">
@@ -3197,10 +3207,10 @@
         <v>81</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>398</v>
+        <v>106</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>397</v>
+        <v>107</v>
       </c>
       <c r="E83" s="1" t="s">
         <v>7</v>
@@ -3215,10 +3225,10 @@
         <v>82</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>109</v>
+        <v>397</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>110</v>
+        <v>396</v>
       </c>
       <c r="E84" s="1" t="s">
         <v>7</v>
@@ -3233,15 +3243,17 @@
         <v>83</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>340</v>
+        <v>108</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>341</v>
+        <v>109</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F85" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="G85" s="1"/>
     </row>
     <row r="86" spans="2:7" x14ac:dyDescent="0.35">
@@ -3249,13 +3261,13 @@
         <v>84</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>111</v>
+        <v>339</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>112</v>
+        <v>340</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F86" s="1"/>
       <c r="G86" s="1"/>
@@ -3265,17 +3277,15 @@
         <v>85</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F87" s="1" t="s">
-        <v>27</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F87" s="1"/>
       <c r="G87" s="1"/>
     </row>
     <row r="88" spans="2:7" x14ac:dyDescent="0.35">
@@ -3283,15 +3293,17 @@
         <v>86</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F88" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F88" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G88" s="1"/>
     </row>
     <row r="89" spans="2:7" x14ac:dyDescent="0.35">
@@ -3299,10 +3311,10 @@
         <v>87</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>426</v>
+        <v>114</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>425</v>
+        <v>115</v>
       </c>
       <c r="E89" s="1" t="s">
         <v>5</v>
@@ -3315,10 +3327,10 @@
         <v>88</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>390</v>
+        <v>425</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>391</v>
+        <v>424</v>
       </c>
       <c r="E90" s="1" t="s">
         <v>5</v>
@@ -3331,10 +3343,10 @@
         <v>89</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>117</v>
+        <v>389</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>118</v>
+        <v>390</v>
       </c>
       <c r="E91" s="1" t="s">
         <v>5</v>
@@ -3347,10 +3359,10 @@
         <v>90</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E92" s="1" t="s">
         <v>5</v>
@@ -3363,10 +3375,10 @@
         <v>91</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E93" s="1" t="s">
         <v>5</v>
@@ -3379,10 +3391,10 @@
         <v>92</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E94" s="1" t="s">
         <v>5</v>
@@ -3395,10 +3407,10 @@
         <v>93</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="E95" s="1" t="s">
         <v>5</v>
@@ -3411,10 +3423,10 @@
         <v>94</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E96" s="1" t="s">
         <v>5</v>
@@ -3427,10 +3439,10 @@
         <v>95</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>372</v>
+        <v>126</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>373</v>
+        <v>127</v>
       </c>
       <c r="E97" s="1" t="s">
         <v>5</v>
@@ -3443,17 +3455,15 @@
         <v>96</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>349</v>
+        <v>371</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>348</v>
+        <v>372</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F98" s="1" t="s">
-        <v>27</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F98" s="1"/>
       <c r="G98" s="1"/>
     </row>
     <row r="99" spans="2:7" x14ac:dyDescent="0.35">
@@ -3461,15 +3471,17 @@
         <v>97</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>129</v>
+        <v>348</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>130</v>
+        <v>347</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F99" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F99" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G99" s="1"/>
     </row>
     <row r="100" spans="2:7" x14ac:dyDescent="0.35">
@@ -3477,10 +3489,10 @@
         <v>98</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>432</v>
+        <v>128</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>431</v>
+        <v>129</v>
       </c>
       <c r="E100" s="1" t="s">
         <v>5</v>
@@ -3493,17 +3505,15 @@
         <v>99</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>131</v>
+        <v>431</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>132</v>
+        <v>430</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F101" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F101" s="1"/>
       <c r="G101" s="1"/>
     </row>
     <row r="102" spans="2:7" x14ac:dyDescent="0.35">
@@ -3511,15 +3521,17 @@
         <v>100</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F102" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F102" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="G102" s="1"/>
     </row>
     <row r="103" spans="2:7" x14ac:dyDescent="0.35">
@@ -3527,17 +3539,15 @@
         <v>101</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F103" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F103" s="1"/>
       <c r="G103" s="1"/>
     </row>
     <row r="104" spans="2:7" x14ac:dyDescent="0.35">
@@ -3545,15 +3555,17 @@
         <v>102</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>356</v>
+        <v>134</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>357</v>
+        <v>135</v>
       </c>
       <c r="E104" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F104" s="1"/>
+      <c r="F104" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="G104" s="1"/>
     </row>
     <row r="105" spans="2:7" x14ac:dyDescent="0.35">
@@ -3561,13 +3573,13 @@
         <v>103</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>137</v>
+        <v>355</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>138</v>
+        <v>356</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F105" s="1"/>
       <c r="G105" s="1"/>
@@ -3577,17 +3589,15 @@
         <v>104</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>361</v>
+        <v>136</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>362</v>
+        <v>137</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F106" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F106" s="1"/>
       <c r="G106" s="1"/>
     </row>
     <row r="107" spans="2:7" x14ac:dyDescent="0.35">
@@ -3595,15 +3605,17 @@
         <v>105</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>314</v>
+        <v>360</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>315</v>
+        <v>361</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F107" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F107" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="G107" s="1"/>
     </row>
     <row r="108" spans="2:7" x14ac:dyDescent="0.35">
@@ -3611,10 +3623,10 @@
         <v>106</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>321</v>
+        <v>314</v>
       </c>
       <c r="E108" s="1" t="s">
         <v>5</v>
@@ -3627,17 +3639,15 @@
         <v>107</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>139</v>
+        <v>319</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>140</v>
+        <v>320</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F109" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F109" s="1"/>
       <c r="G109" s="1"/>
     </row>
     <row r="110" spans="2:7" x14ac:dyDescent="0.35">
@@ -3645,15 +3655,17 @@
         <v>108</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>322</v>
+        <v>138</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>323</v>
+        <v>139</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F110" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F110" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="G110" s="1"/>
     </row>
     <row r="111" spans="2:7" x14ac:dyDescent="0.35">
@@ -3661,10 +3673,10 @@
         <v>109</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>141</v>
+        <v>321</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>142</v>
+        <v>322</v>
       </c>
       <c r="E111" s="1" t="s">
         <v>5</v>
@@ -3677,10 +3689,10 @@
         <v>110</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>306</v>
+        <v>140</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>307</v>
+        <v>141</v>
       </c>
       <c r="E112" s="1" t="s">
         <v>5</v>
@@ -3693,10 +3705,10 @@
         <v>111</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>143</v>
+        <v>305</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>144</v>
+        <v>306</v>
       </c>
       <c r="E113" s="1" t="s">
         <v>5</v>
@@ -3709,10 +3721,10 @@
         <v>112</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E114" s="1" t="s">
         <v>5</v>
@@ -3725,17 +3737,15 @@
         <v>113</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>434</v>
+        <v>144</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>433</v>
+        <v>145</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F115" s="1" t="s">
-        <v>27</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F115" s="1"/>
       <c r="G115" s="1"/>
     </row>
     <row r="116" spans="2:7" x14ac:dyDescent="0.35">
@@ -3743,10 +3753,10 @@
         <v>114</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>147</v>
+        <v>433</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>148</v>
+        <v>432</v>
       </c>
       <c r="E116" s="1" t="s">
         <v>7</v>
@@ -3761,10 +3771,10 @@
         <v>115</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="E117" s="1" t="s">
         <v>7</v>
@@ -3779,16 +3789,16 @@
         <v>116</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="E118" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F118" s="1" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="G118" s="1"/>
     </row>
@@ -3797,15 +3807,17 @@
         <v>117</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F119" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F119" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="G119" s="1"/>
     </row>
     <row r="120" spans="2:7" x14ac:dyDescent="0.35">
@@ -3813,13 +3825,13 @@
         <v>118</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F120" s="1"/>
       <c r="G120" s="1"/>
@@ -3829,13 +3841,13 @@
         <v>119</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F121" s="1"/>
       <c r="G121" s="1"/>
@@ -3845,17 +3857,15 @@
         <v>120</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>405</v>
+        <v>156</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>406</v>
+        <v>157</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F122" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F122" s="1"/>
       <c r="G122" s="1"/>
     </row>
     <row r="123" spans="2:7" x14ac:dyDescent="0.35">
@@ -3863,15 +3873,17 @@
         <v>121</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>159</v>
+        <v>404</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>160</v>
+        <v>405</v>
       </c>
       <c r="E123" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F123" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F123" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="G123" s="1"/>
     </row>
     <row r="124" spans="2:7" x14ac:dyDescent="0.35">
@@ -3879,10 +3891,10 @@
         <v>122</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>328</v>
+        <v>158</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>329</v>
+        <v>159</v>
       </c>
       <c r="E124" s="1" t="s">
         <v>5</v>
@@ -3895,10 +3907,10 @@
         <v>123</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="E125" s="1" t="s">
         <v>5</v>
@@ -3911,17 +3923,15 @@
         <v>124</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>316</v>
+        <v>323</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>317</v>
+        <v>326</v>
       </c>
       <c r="E126" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F126" s="1" t="s">
-        <v>27</v>
-      </c>
+      <c r="F126" s="1"/>
       <c r="G126" s="1"/>
     </row>
     <row r="127" spans="2:7" x14ac:dyDescent="0.35">
@@ -3929,41 +3939,43 @@
         <v>125</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>379</v>
+        <v>315</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>378</v>
+        <v>316</v>
       </c>
       <c r="E127" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F127" s="1"/>
-      <c r="G127" s="1" t="s">
-        <v>380</v>
-      </c>
+      <c r="F127" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G127" s="1"/>
     </row>
     <row r="128" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B128" s="6">
         <v>126</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>311</v>
+        <v>378</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>310</v>
+        <v>377</v>
       </c>
       <c r="E128" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F128" s="1"/>
-      <c r="G128" s="1"/>
+      <c r="G128" s="1" t="s">
+        <v>379</v>
+      </c>
     </row>
     <row r="129" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B129" s="6">
         <v>127</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="D129" s="1" t="s">
         <v>309</v>
@@ -3979,10 +3991,10 @@
         <v>128</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>367</v>
+        <v>307</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>368</v>
+        <v>308</v>
       </c>
       <c r="E130" s="1" t="s">
         <v>5</v>
@@ -3995,10 +4007,10 @@
         <v>129</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>161</v>
+        <v>366</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>162</v>
+        <v>367</v>
       </c>
       <c r="E131" s="1" t="s">
         <v>5</v>
@@ -4011,10 +4023,10 @@
         <v>130</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="E132" s="1" t="s">
         <v>5</v>
@@ -4027,10 +4039,10 @@
         <v>131</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="E133" s="1" t="s">
         <v>5</v>
@@ -4043,10 +4055,10 @@
         <v>132</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="E134" s="1" t="s">
         <v>5</v>
@@ -4059,10 +4071,10 @@
         <v>133</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="E135" s="1" t="s">
         <v>5</v>
@@ -4075,10 +4087,10 @@
         <v>134</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>336</v>
+        <v>168</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E136" s="1" t="s">
         <v>5</v>
@@ -4091,10 +4103,10 @@
         <v>135</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>172</v>
+        <v>335</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E137" s="1" t="s">
         <v>5</v>
@@ -4107,10 +4119,10 @@
         <v>136</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>440</v>
+        <v>171</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>439</v>
+        <v>172</v>
       </c>
       <c r="E138" s="1" t="s">
         <v>5</v>
@@ -4123,17 +4135,15 @@
         <v>137</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>174</v>
+        <v>439</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>175</v>
+        <v>438</v>
       </c>
       <c r="E139" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F139" s="1" t="s">
-        <v>27</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F139" s="1"/>
       <c r="G139" s="1"/>
     </row>
     <row r="140" spans="2:7" x14ac:dyDescent="0.35">
@@ -4141,15 +4151,17 @@
         <v>138</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E140" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F140" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F140" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G140" s="1"/>
     </row>
     <row r="141" spans="2:7" x14ac:dyDescent="0.35">
@@ -4157,10 +4169,10 @@
         <v>139</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="E141" s="1" t="s">
         <v>5</v>
@@ -4173,10 +4185,10 @@
         <v>140</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E142" s="1" t="s">
         <v>5</v>
@@ -4189,10 +4201,10 @@
         <v>141</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="E143" s="1" t="s">
         <v>5</v>
@@ -4205,10 +4217,10 @@
         <v>142</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E144" s="1" t="s">
         <v>5</v>
@@ -4221,10 +4233,10 @@
         <v>143</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="E145" s="1" t="s">
         <v>5</v>
@@ -4237,10 +4249,10 @@
         <v>144</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="E146" s="1" t="s">
         <v>5</v>
@@ -4253,10 +4265,10 @@
         <v>145</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>377</v>
+        <v>187</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>337</v>
+        <v>188</v>
       </c>
       <c r="E147" s="1" t="s">
         <v>5</v>
@@ -4269,10 +4281,10 @@
         <v>146</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>371</v>
+        <v>376</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>191</v>
+        <v>336</v>
       </c>
       <c r="E148" s="1" t="s">
         <v>5</v>
@@ -4285,10 +4297,10 @@
         <v>147</v>
       </c>
       <c r="C149" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="D149" s="1" t="s">
         <v>190</v>
-      </c>
-      <c r="D149" s="1" t="s">
-        <v>191</v>
       </c>
       <c r="E149" s="1" t="s">
         <v>5</v>
@@ -4301,10 +4313,10 @@
         <v>148</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>334</v>
+        <v>189</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>335</v>
+        <v>190</v>
       </c>
       <c r="E150" s="1" t="s">
         <v>5</v>
@@ -4317,17 +4329,15 @@
         <v>149</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>374</v>
+        <v>333</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>375</v>
+        <v>334</v>
       </c>
       <c r="E151" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F151" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F151" s="1"/>
       <c r="G151" s="1"/>
     </row>
     <row r="152" spans="2:7" x14ac:dyDescent="0.35">
@@ -4335,10 +4345,10 @@
         <v>150</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>192</v>
+        <v>373</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>193</v>
+        <v>374</v>
       </c>
       <c r="E152" s="1" t="s">
         <v>7</v>
@@ -4353,15 +4363,17 @@
         <v>151</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="E153" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F153" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F153" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="G153" s="1"/>
     </row>
     <row r="154" spans="2:7" x14ac:dyDescent="0.35">
@@ -4369,10 +4381,10 @@
         <v>152</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="E154" s="1" t="s">
         <v>5</v>
@@ -4385,10 +4397,10 @@
         <v>153</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>347</v>
+        <v>195</v>
       </c>
       <c r="D155" s="1" t="s">
-        <v>346</v>
+        <v>196</v>
       </c>
       <c r="E155" s="1" t="s">
         <v>5</v>
@@ -4401,10 +4413,10 @@
         <v>154</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>198</v>
+        <v>346</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>199</v>
+        <v>345</v>
       </c>
       <c r="E156" s="1" t="s">
         <v>5</v>
@@ -4417,10 +4429,10 @@
         <v>155</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E157" s="1" t="s">
         <v>5</v>
@@ -4433,13 +4445,13 @@
         <v>156</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="D158" s="1" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="E158" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F158" s="1"/>
       <c r="G158" s="1"/>
@@ -4449,17 +4461,15 @@
         <v>157</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>358</v>
+        <v>201</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>359</v>
+        <v>202</v>
       </c>
       <c r="E159" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F159" s="1" t="s">
-        <v>27</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="F159" s="1"/>
       <c r="G159" s="1"/>
     </row>
     <row r="160" spans="2:7" x14ac:dyDescent="0.35">
@@ -4467,15 +4477,17 @@
         <v>158</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>204</v>
+        <v>357</v>
       </c>
       <c r="D160" s="1" t="s">
-        <v>205</v>
+        <v>358</v>
       </c>
       <c r="E160" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F160" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F160" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G160" s="1"/>
     </row>
     <row r="161" spans="2:7" x14ac:dyDescent="0.35">
@@ -4483,10 +4495,10 @@
         <v>159</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D161" s="1" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="E161" s="1" t="s">
         <v>5</v>
@@ -4499,10 +4511,10 @@
         <v>160</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D162" s="1" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="E162" s="1" t="s">
         <v>5</v>
@@ -4515,17 +4527,15 @@
         <v>161</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="D163" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="E163" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F163" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F163" s="1"/>
       <c r="G163" s="1"/>
     </row>
     <row r="164" spans="2:7" x14ac:dyDescent="0.35">
@@ -4533,15 +4543,17 @@
         <v>162</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="D164" s="1" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="E164" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F164" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F164" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="G164" s="1"/>
     </row>
     <row r="165" spans="2:7" x14ac:dyDescent="0.35">
@@ -4549,10 +4561,10 @@
         <v>163</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="D165" s="1" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="E165" s="1" t="s">
         <v>5</v>
@@ -4565,17 +4577,15 @@
         <v>164</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D166" s="1" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="E166" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F166" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F166" s="1"/>
       <c r="G166" s="1"/>
     </row>
     <row r="167" spans="2:7" x14ac:dyDescent="0.35">
@@ -4583,30 +4593,28 @@
         <v>165</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="D167" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E167" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F167" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G167" s="1" t="s">
-        <v>30</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="G167" s="1"/>
     </row>
     <row r="168" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B168" s="6">
         <v>166</v>
       </c>
       <c r="C168" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="D168" s="1" t="s">
         <v>219</v>
-      </c>
-      <c r="D168" s="1" t="s">
-        <v>221</v>
       </c>
       <c r="E168" s="1" t="s">
         <v>7</v>
@@ -4623,10 +4631,10 @@
         <v>167</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="D169" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E169" s="1" t="s">
         <v>7</v>
@@ -4635,7 +4643,7 @@
         <v>27</v>
       </c>
       <c r="G169" s="1" t="s">
-        <v>297</v>
+        <v>30</v>
       </c>
     </row>
     <row r="170" spans="2:7" x14ac:dyDescent="0.35">
@@ -4643,33 +4651,37 @@
         <v>168</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="D170" s="1" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="E170" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F170" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G170" s="1"/>
+        <v>15</v>
+      </c>
+      <c r="G170" s="1" t="s">
+        <v>296</v>
+      </c>
     </row>
     <row r="171" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B171" s="6">
         <v>169</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="D171" s="1" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="E171" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F171" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F171" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G171" s="1"/>
     </row>
     <row r="172" spans="2:7" x14ac:dyDescent="0.35">
@@ -4677,10 +4689,10 @@
         <v>170</v>
       </c>
       <c r="C172" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="D172" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="E172" s="1" t="s">
         <v>5</v>
@@ -4693,17 +4705,15 @@
         <v>171</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="D173" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="E173" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F173" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F173" s="1"/>
       <c r="G173" s="1"/>
     </row>
     <row r="174" spans="2:7" x14ac:dyDescent="0.35">
@@ -4711,17 +4721,15 @@
         <v>172</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>233</v>
+        <v>441</v>
       </c>
       <c r="D174" s="1" t="s">
-        <v>232</v>
+        <v>440</v>
       </c>
       <c r="E174" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F174" s="1" t="s">
-        <v>27</v>
-      </c>
+      <c r="F174" s="1"/>
       <c r="G174" s="1"/>
     </row>
     <row r="175" spans="2:7" x14ac:dyDescent="0.35">
@@ -4729,15 +4737,17 @@
         <v>173</v>
       </c>
       <c r="C175" s="1" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="D175" s="1" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="E175" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F175" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F175" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="G175" s="1"/>
     </row>
     <row r="176" spans="2:7" x14ac:dyDescent="0.35">
@@ -4745,15 +4755,17 @@
         <v>174</v>
       </c>
       <c r="C176" s="1" t="s">
-        <v>408</v>
+        <v>232</v>
       </c>
       <c r="D176" s="1" t="s">
-        <v>407</v>
+        <v>231</v>
       </c>
       <c r="E176" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F176" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F176" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G176" s="1"/>
     </row>
     <row r="177" spans="2:7" x14ac:dyDescent="0.35">
@@ -4761,10 +4773,10 @@
         <v>175</v>
       </c>
       <c r="C177" s="1" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="D177" s="1" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="E177" s="1" t="s">
         <v>5</v>
@@ -4777,10 +4789,10 @@
         <v>176</v>
       </c>
       <c r="C178" s="1" t="s">
-        <v>238</v>
+        <v>407</v>
       </c>
       <c r="D178" s="1" t="s">
-        <v>239</v>
+        <v>406</v>
       </c>
       <c r="E178" s="1" t="s">
         <v>5</v>
@@ -4793,10 +4805,10 @@
         <v>177</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="D179" s="1" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="E179" s="1" t="s">
         <v>5</v>
@@ -4809,17 +4821,15 @@
         <v>178</v>
       </c>
       <c r="C180" s="1" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="D180" s="1" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="E180" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F180" s="1" t="s">
-        <v>27</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F180" s="1"/>
       <c r="G180" s="1"/>
     </row>
     <row r="181" spans="2:7" x14ac:dyDescent="0.35">
@@ -4827,13 +4837,13 @@
         <v>179</v>
       </c>
       <c r="C181" s="1" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="D181" s="1" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="E181" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F181" s="1"/>
       <c r="G181" s="1"/>
@@ -4843,15 +4853,17 @@
         <v>180</v>
       </c>
       <c r="C182" s="1" t="s">
-        <v>381</v>
+        <v>241</v>
       </c>
       <c r="D182" s="1" t="s">
-        <v>382</v>
+        <v>242</v>
       </c>
       <c r="E182" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F182" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F182" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G182" s="1"/>
     </row>
     <row r="183" spans="2:7" x14ac:dyDescent="0.35">
@@ -4859,13 +4871,13 @@
         <v>181</v>
       </c>
       <c r="C183" s="1" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="D183" s="1" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="E183" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F183" s="1"/>
       <c r="G183" s="1"/>
@@ -4875,10 +4887,10 @@
         <v>182</v>
       </c>
       <c r="C184" s="1" t="s">
-        <v>248</v>
+        <v>380</v>
       </c>
       <c r="D184" s="1" t="s">
-        <v>249</v>
+        <v>381</v>
       </c>
       <c r="E184" s="1" t="s">
         <v>5</v>
@@ -4891,10 +4903,10 @@
         <v>183</v>
       </c>
       <c r="C185" s="1" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="D185" s="1" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="E185" s="1" t="s">
         <v>5</v>
@@ -4907,10 +4919,10 @@
         <v>184</v>
       </c>
       <c r="C186" s="1" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="D186" s="1" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="E186" s="1" t="s">
         <v>5</v>
@@ -4923,10 +4935,10 @@
         <v>185</v>
       </c>
       <c r="C187" s="1" t="s">
-        <v>353</v>
+        <v>249</v>
       </c>
       <c r="D187" s="1" t="s">
-        <v>352</v>
+        <v>250</v>
       </c>
       <c r="E187" s="1" t="s">
         <v>5</v>
@@ -4939,10 +4951,10 @@
         <v>186</v>
       </c>
       <c r="C188" s="1" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="D188" s="1" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="E188" s="1" t="s">
         <v>5</v>
@@ -4955,10 +4967,10 @@
         <v>187</v>
       </c>
       <c r="C189" s="1" t="s">
-        <v>383</v>
+        <v>352</v>
       </c>
       <c r="D189" s="1" t="s">
-        <v>384</v>
+        <v>351</v>
       </c>
       <c r="E189" s="1" t="s">
         <v>5</v>
@@ -4971,30 +4983,26 @@
         <v>188</v>
       </c>
       <c r="C190" s="1" t="s">
-        <v>385</v>
+        <v>253</v>
       </c>
       <c r="D190" s="1" t="s">
-        <v>386</v>
+        <v>254</v>
       </c>
       <c r="E190" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F190" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G190" s="1" t="s">
-        <v>387</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F190" s="1"/>
+      <c r="G190" s="1"/>
     </row>
     <row r="191" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B191" s="6">
         <v>189</v>
       </c>
       <c r="C191" s="1" t="s">
-        <v>256</v>
+        <v>382</v>
       </c>
       <c r="D191" s="1" t="s">
-        <v>257</v>
+        <v>383</v>
       </c>
       <c r="E191" s="1" t="s">
         <v>5</v>
@@ -5007,28 +5015,30 @@
         <v>190</v>
       </c>
       <c r="C192" s="1" t="s">
-        <v>258</v>
+        <v>384</v>
       </c>
       <c r="D192" s="1" t="s">
-        <v>259</v>
+        <v>385</v>
       </c>
       <c r="E192" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F192" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G192" s="1"/>
+        <v>15</v>
+      </c>
+      <c r="G192" s="1" t="s">
+        <v>386</v>
+      </c>
     </row>
     <row r="193" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B193" s="6">
         <v>191</v>
       </c>
       <c r="C193" s="1" t="s">
-        <v>369</v>
+        <v>255</v>
       </c>
       <c r="D193" s="1" t="s">
-        <v>370</v>
+        <v>256</v>
       </c>
       <c r="E193" s="1" t="s">
         <v>5</v>
@@ -5041,15 +5051,17 @@
         <v>192</v>
       </c>
       <c r="C194" s="1" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="D194" s="1" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="E194" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F194" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F194" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G194" s="1"/>
     </row>
     <row r="195" spans="2:7" x14ac:dyDescent="0.35">
@@ -5057,10 +5069,10 @@
         <v>193</v>
       </c>
       <c r="C195" s="1" t="s">
-        <v>262</v>
+        <v>368</v>
       </c>
       <c r="D195" s="1" t="s">
-        <v>263</v>
+        <v>369</v>
       </c>
       <c r="E195" s="1" t="s">
         <v>5</v>
@@ -5073,17 +5085,15 @@
         <v>194</v>
       </c>
       <c r="C196" s="1" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="D196" s="1" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="E196" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F196" s="1" t="s">
-        <v>27</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F196" s="1"/>
       <c r="G196" s="1"/>
     </row>
     <row r="197" spans="2:7" x14ac:dyDescent="0.35">
@@ -5091,17 +5101,15 @@
         <v>195</v>
       </c>
       <c r="C197" s="1" t="s">
-        <v>436</v>
+        <v>261</v>
       </c>
       <c r="D197" s="1" t="s">
-        <v>435</v>
+        <v>262</v>
       </c>
       <c r="E197" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F197" s="1" t="s">
-        <v>27</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F197" s="1"/>
       <c r="G197" s="1"/>
     </row>
     <row r="198" spans="2:7" x14ac:dyDescent="0.35">
@@ -5109,15 +5117,17 @@
         <v>196</v>
       </c>
       <c r="C198" s="1" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="D198" s="1" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="E198" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F198" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F198" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G198" s="1"/>
     </row>
     <row r="199" spans="2:7" x14ac:dyDescent="0.35">
@@ -5125,15 +5135,17 @@
         <v>197</v>
       </c>
       <c r="C199" s="1" t="s">
-        <v>268</v>
+        <v>435</v>
       </c>
       <c r="D199" s="1" t="s">
-        <v>269</v>
+        <v>434</v>
       </c>
       <c r="E199" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F199" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F199" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G199" s="1"/>
     </row>
     <row r="200" spans="2:7" x14ac:dyDescent="0.35">
@@ -5141,10 +5153,10 @@
         <v>198</v>
       </c>
       <c r="C200" s="1" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="D200" s="1" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="E200" s="1" t="s">
         <v>5</v>
@@ -5157,10 +5169,10 @@
         <v>199</v>
       </c>
       <c r="C201" s="1" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="D201" s="1" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="E201" s="1" t="s">
         <v>5</v>
@@ -5173,10 +5185,10 @@
         <v>200</v>
       </c>
       <c r="C202" s="1" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="D202" s="1" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="E202" s="1" t="s">
         <v>5</v>
@@ -5189,10 +5201,10 @@
         <v>201</v>
       </c>
       <c r="C203" s="1" t="s">
-        <v>10</v>
+        <v>271</v>
       </c>
       <c r="D203" s="1" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="E203" s="1" t="s">
         <v>5</v>
@@ -5205,13 +5217,13 @@
         <v>202</v>
       </c>
       <c r="C204" s="1" t="s">
-        <v>325</v>
+        <v>273</v>
       </c>
       <c r="D204" s="1" t="s">
-        <v>326</v>
+        <v>274</v>
       </c>
       <c r="E204" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F204" s="1"/>
       <c r="G204" s="1"/>
@@ -5221,10 +5233,10 @@
         <v>203</v>
       </c>
       <c r="C205" s="1" t="s">
-        <v>420</v>
+        <v>10</v>
       </c>
       <c r="D205" s="1" t="s">
-        <v>419</v>
+        <v>275</v>
       </c>
       <c r="E205" s="1" t="s">
         <v>5</v>
@@ -5237,17 +5249,15 @@
         <v>204</v>
       </c>
       <c r="C206" s="1" t="s">
-        <v>277</v>
+        <v>324</v>
       </c>
       <c r="D206" s="1" t="s">
-        <v>278</v>
+        <v>325</v>
       </c>
       <c r="E206" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F206" s="1" t="s">
-        <v>27</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="F206" s="1"/>
       <c r="G206" s="1"/>
     </row>
     <row r="207" spans="2:7" x14ac:dyDescent="0.35">
@@ -5255,10 +5265,10 @@
         <v>205</v>
       </c>
       <c r="C207" s="1" t="s">
-        <v>279</v>
+        <v>419</v>
       </c>
       <c r="D207" s="1" t="s">
-        <v>280</v>
+        <v>418</v>
       </c>
       <c r="E207" s="1" t="s">
         <v>5</v>
@@ -5271,15 +5281,17 @@
         <v>206</v>
       </c>
       <c r="C208" s="1" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="D208" s="1" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="E208" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F208" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F208" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G208" s="1"/>
     </row>
     <row r="209" spans="2:7" x14ac:dyDescent="0.35">
@@ -5287,17 +5299,15 @@
         <v>207</v>
       </c>
       <c r="C209" s="1" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="D209" s="1" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="E209" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F209" s="1" t="s">
-        <v>27</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F209" s="1"/>
       <c r="G209" s="1"/>
     </row>
     <row r="210" spans="2:7" x14ac:dyDescent="0.35">
@@ -5305,17 +5315,15 @@
         <v>208</v>
       </c>
       <c r="C210" s="1" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="D210" s="1" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="E210" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F210" s="1" t="s">
-        <v>27</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="F210" s="1"/>
       <c r="G210" s="1"/>
     </row>
     <row r="211" spans="2:7" x14ac:dyDescent="0.35">
@@ -5323,10 +5331,10 @@
         <v>209</v>
       </c>
       <c r="C211" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="D211" s="1" t="s">
         <v>285</v>
-      </c>
-      <c r="D211" s="1" t="s">
-        <v>288</v>
       </c>
       <c r="E211" s="1" t="s">
         <v>7</v>
@@ -5341,15 +5349,17 @@
         <v>210</v>
       </c>
       <c r="C212" s="1" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="D212" s="1" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="E212" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F212" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F212" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G212" s="1"/>
     </row>
     <row r="213" spans="2:7" x14ac:dyDescent="0.35">
@@ -5357,10 +5367,10 @@
         <v>211</v>
       </c>
       <c r="C213" s="1" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="D213" s="1" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="E213" s="1" t="s">
         <v>7</v>
@@ -5375,10 +5385,10 @@
         <v>212</v>
       </c>
       <c r="C214" s="1" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="D214" s="1" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="E214" s="1" t="s">
         <v>5</v>
@@ -5391,30 +5401,48 @@
         <v>213</v>
       </c>
       <c r="C215" s="1" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="D215" s="1" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="E215" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F215" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F215" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G215" s="1"/>
     </row>
     <row r="216" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B216" s="6"/>
-      <c r="C216" s="1"/>
-      <c r="D216" s="1"/>
-      <c r="E216" s="1"/>
+      <c r="B216" s="6">
+        <v>214</v>
+      </c>
+      <c r="C216" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="D216" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="E216" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F216" s="1"/>
       <c r="G216" s="1"/>
     </row>
     <row r="217" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B217" s="6"/>
-      <c r="C217" s="1"/>
-      <c r="D217" s="1"/>
-      <c r="E217" s="1"/>
+      <c r="B217" s="6">
+        <v>215</v>
+      </c>
+      <c r="C217" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="D217" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="E217" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F217" s="1"/>
       <c r="G217" s="1"/>
     </row>
@@ -5434,12 +5462,28 @@
       <c r="F219" s="1"/>
       <c r="G219" s="1"/>
     </row>
+    <row r="220" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B220" s="6"/>
+      <c r="C220" s="1"/>
+      <c r="D220" s="1"/>
+      <c r="E220" s="1"/>
+      <c r="F220" s="1"/>
+      <c r="G220" s="1"/>
+    </row>
+    <row r="221" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B221" s="6"/>
+      <c r="C221" s="1"/>
+      <c r="D221" s="1"/>
+      <c r="E221" s="1"/>
+      <c r="F221" s="1"/>
+      <c r="G221" s="1"/>
+    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E215" xr:uid="{7E8CE32C-29D1-4006-9E0F-69B72A0F4378}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E217" xr:uid="{7E8CE32C-29D1-4006-9E0F-69B72A0F4378}">
       <formula1>"[Application],[Directory],[Script]"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F219" xr:uid="{A5D947FB-5606-4B36-88C5-81CC2B61C636}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F221" xr:uid="{A5D947FB-5606-4B36-88C5-81CC2B61C636}">
       <formula1>"[bat],[vbs]"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>